<commit_message>
Adding costal items from starting area.
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA72E75E-9B74-4650-BF6D-39F67AF880B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008D769E-65D2-4C50-9291-CACFA13C061B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1890" windowWidth="21600" windowHeight="11295" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="128">
   <si>
     <t>Mission</t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t>Noise</t>
+  </si>
+  <si>
+    <t>Advance 1st Aid Kit</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,6 +487,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -684,7 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -828,6 +837,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -1143,10 +1158,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R82"/>
+  <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="M83" sqref="M83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L98" sqref="L98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,10 +1486,10 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="52">
         <v>2</v>
       </c>
       <c r="M17" s="1">
@@ -1511,7 +1527,7 @@
       <c r="R18" s="34"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="51" t="s">
         <v>25</v>
       </c>
       <c r="L19" s="9"/>
@@ -2501,6 +2517,220 @@
       </c>
       <c r="O82" s="2">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J83" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M83" s="1">
+        <v>4091</v>
+      </c>
+      <c r="N83" s="1">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J84" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M84" s="1">
+        <v>4100</v>
+      </c>
+      <c r="N84" s="1">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J85" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M85" s="1">
+        <v>4072</v>
+      </c>
+      <c r="N85" s="1">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F86" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G86" s="2">
+        <v>2</v>
+      </c>
+      <c r="M86" s="1">
+        <v>3798</v>
+      </c>
+      <c r="N86" s="1">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J87" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M87" s="1">
+        <v>3797</v>
+      </c>
+      <c r="N87" s="1">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J88" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K88" s="2">
+        <v>2</v>
+      </c>
+      <c r="L88" s="9"/>
+      <c r="M88" s="10">
+        <v>3797</v>
+      </c>
+      <c r="N88" s="14">
+        <v>1804</v>
+      </c>
+      <c r="O88" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J89" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L89" s="9"/>
+      <c r="M89" s="12"/>
+      <c r="N89" s="15"/>
+      <c r="O89" s="13"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I90" s="2">
+        <v>1</v>
+      </c>
+      <c r="M90" s="1">
+        <v>3792</v>
+      </c>
+      <c r="N90" s="1">
+        <v>1799</v>
+      </c>
+      <c r="O90" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L91" s="19">
+        <v>5</v>
+      </c>
+      <c r="M91" s="1">
+        <v>4223</v>
+      </c>
+      <c r="N91" s="1">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J92" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K92" s="2">
+        <v>3</v>
+      </c>
+      <c r="M92" s="1">
+        <v>4471</v>
+      </c>
+      <c r="N92" s="1">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J93" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M93" s="1">
+        <v>4476</v>
+      </c>
+      <c r="N93" s="1">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F94" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" s="2">
+        <v>1</v>
+      </c>
+      <c r="M94" s="1">
+        <v>4580</v>
+      </c>
+      <c r="N94" s="1">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J95" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K95" s="2">
+        <v>4</v>
+      </c>
+      <c r="M95" s="1">
+        <v>4130</v>
+      </c>
+      <c r="N95" s="1">
+        <v>2492</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J96" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K96" s="2">
+        <v>3</v>
+      </c>
+      <c r="L96" s="9"/>
+      <c r="M96" s="10">
+        <v>4325</v>
+      </c>
+      <c r="N96" s="14">
+        <v>2361</v>
+      </c>
+      <c r="O96" s="11"/>
+    </row>
+    <row r="97" spans="10:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J97" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K97" s="2">
+        <v>2</v>
+      </c>
+      <c r="L97" s="9"/>
+      <c r="M97" s="12"/>
+      <c r="N97" s="15"/>
+      <c r="O97" s="13"/>
+    </row>
+    <row r="98" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J98" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K98" s="2">
+        <v>3</v>
+      </c>
+      <c r="M98" s="1">
+        <v>4446</v>
+      </c>
+      <c r="N98" s="1">
+        <v>2371</v>
       </c>
     </row>
   </sheetData>
@@ -3663,8 +3893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49260601-DFFC-49C5-BC21-5E0477EEDF42}">
   <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding Equipment and Ammo Recycle data
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E812D84C-9B40-4318-A49A-41436B0BD3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC50A33-0964-4CBE-99B3-526FB3E5BBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="30135" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
-    <sheet name="Craft" sheetId="3" r:id="rId2"/>
+    <sheet name="Recycle" sheetId="3" r:id="rId2"/>
     <sheet name="Stats" sheetId="4" r:id="rId3"/>
     <sheet name="Names" sheetId="2" r:id="rId4"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="239">
   <si>
     <t>Mission</t>
   </si>
@@ -430,6 +430,9 @@
     <t>Ammo</t>
   </si>
   <si>
+    <t>0.32 FMJ</t>
+  </si>
+  <si>
     <t>HP</t>
   </si>
   <si>
@@ -442,12 +445,6 @@
     <t>Adhesive 3 | Rubber 6</t>
   </si>
   <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Number to Burn</t>
-  </si>
-  <si>
     <t>Adhesive 3 | Steel 6 | Titanium 2</t>
   </si>
   <si>
@@ -466,9 +463,6 @@
     <t>Medical</t>
   </si>
   <si>
-    <t>9mm</t>
-  </si>
-  <si>
     <t>HEAT</t>
   </si>
   <si>
@@ -491,13 +485,283 @@
   </si>
   <si>
     <t>Adhesive 2 | Steel 5</t>
+  </si>
+  <si>
+    <t>Adhesive 5 |Steel 10 | Copper 3</t>
+  </si>
+  <si>
+    <t>Adhesive 5 | Steel 10 | Titanium 3</t>
+  </si>
+  <si>
+    <t>Adhesive 4 | Plastic 8 |Aluminium 2</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>0.270</t>
+  </si>
+  <si>
+    <t>Explosive</t>
+  </si>
+  <si>
+    <t>9mm (H)</t>
+  </si>
+  <si>
+    <t>9mm (SMG)</t>
+  </si>
+  <si>
+    <t>Corrosive</t>
+  </si>
+  <si>
+    <t>12ga</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>Buck</t>
+  </si>
+  <si>
+    <t>Slug Corrosive</t>
+  </si>
+  <si>
+    <t>Slug Medical</t>
+  </si>
+  <si>
+    <t>7.62mm</t>
+  </si>
+  <si>
+    <t>Tar</t>
+  </si>
+  <si>
+    <t>5.56mm</t>
+  </si>
+  <si>
+    <t>9x39mm</t>
+  </si>
+  <si>
+    <t>arrows</t>
+  </si>
+  <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>napalm</t>
+  </si>
+  <si>
+    <t>LG-7V</t>
+  </si>
+  <si>
+    <t>High-Explosive</t>
+  </si>
+  <si>
+    <t>G79</t>
+  </si>
+  <si>
+    <t>EMP</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>Bundle Number</t>
+  </si>
+  <si>
+    <t>Adhesive 4 | Rubber 8 | Lead 2</t>
+  </si>
+  <si>
+    <t>Adhesive 2 | Explosive 2 | Textile 4 | Lead 1</t>
+  </si>
+  <si>
+    <t>Explosive 4 | Rubber 8 | Lead 2</t>
+  </si>
+  <si>
+    <t>Thread 4 | Accelerant 4 | Titanium 2 | Copper 2</t>
+  </si>
+  <si>
+    <t>Accelerant 1 | Steel 2</t>
+  </si>
+  <si>
+    <t>Explosive 2 | Steel 4 | Lead 1</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Thread 1 | Accelerant 1</t>
+  </si>
+  <si>
+    <t>Adrenaline Shot</t>
+  </si>
+  <si>
+    <t>Electrolyte 8 | Plastic 16 | Titanium 4 | Copper 4 | Tungsten 2</t>
+  </si>
+  <si>
+    <t>Thread 2 | Accelerant 2</t>
+  </si>
+  <si>
+    <t>Adhesive 1 | Steel 2</t>
+  </si>
+  <si>
+    <t>Electrolyte 1 | Rubber 2</t>
+  </si>
+  <si>
+    <t>Explosive 2 | Textile 4 | Lead 1</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>Thread 4 | Accelerant 4 | Titanium 2</t>
+  </si>
+  <si>
+    <t>Electrolyte 4 | Rubber 8 | Copper 2</t>
+  </si>
+  <si>
+    <t>Adhesive 4 | Plastic 8 | Lead 2</t>
+  </si>
+  <si>
+    <t>Explosive 2 | Textile 4 | Copper 1</t>
+  </si>
+  <si>
+    <t>Electrolyte 4 | Plastic 8 | Aluminium 2 | Lead 2</t>
+  </si>
+  <si>
+    <t>Adhesive 1 | Steel 2 | Plastic 2</t>
+  </si>
+  <si>
+    <t>Explosive 2 | Plastic 4 | Copper 1</t>
+  </si>
+  <si>
+    <t>Adhesive 4 | Steel 8 | Titanium 2</t>
+  </si>
+  <si>
+    <t>Accelerant 2 | Textile 4 | Lead 1</t>
+  </si>
+  <si>
+    <t>Electrolyte 4 | Steel 8 | Aluminium 2</t>
+  </si>
+  <si>
+    <t>Thread 2 | Explosive 2 | Textile 4 | Copper 1</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>0.243 SP</t>
+  </si>
+  <si>
+    <t>Explosive 2 | Lead 1</t>
+  </si>
+  <si>
+    <t>0.243 FMJ</t>
+  </si>
+  <si>
+    <t>9mm (H) FMJ</t>
+  </si>
+  <si>
+    <t>9mm (H) AP</t>
+  </si>
+  <si>
+    <t>9mm (SMG) FMJ</t>
+  </si>
+  <si>
+    <t>9mm (SMG) AP</t>
+  </si>
+  <si>
+    <t>0.270 SP</t>
+  </si>
+  <si>
+    <t>12ga Slug</t>
+  </si>
+  <si>
+    <t>12ga Bird</t>
+  </si>
+  <si>
+    <t>12ga Buck</t>
+  </si>
+  <si>
+    <t>7.62mm FMJ</t>
+  </si>
+  <si>
+    <t>7.62mm AP</t>
+  </si>
+  <si>
+    <t>5.56mm FMJ</t>
+  </si>
+  <si>
+    <t>5.56mm AP</t>
+  </si>
+  <si>
+    <t>9x39mm FMJ</t>
+  </si>
+  <si>
+    <t>9x39mm AP</t>
+  </si>
+  <si>
+    <t>Standard arrows</t>
+  </si>
+  <si>
+    <t>Explosive arrows</t>
+  </si>
+  <si>
+    <t>Flare arrows</t>
+  </si>
+  <si>
+    <t>G79 HE</t>
+  </si>
+  <si>
+    <t>G79 Smoke</t>
+  </si>
+  <si>
+    <t>G79 EMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dual-Purpose HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dual-Purpose Smoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dual-Purpose EMP</t>
+  </si>
+  <si>
+    <t>Explosive 2 | Copper 1</t>
+  </si>
+  <si>
+    <t>Steel 4 | Wood 4</t>
+  </si>
+  <si>
+    <t>Explosive 2 | Wood 4</t>
+  </si>
+  <si>
+    <t>Explosive 1 | Plastic 2 | Wood 2</t>
+  </si>
+  <si>
+    <t>Accelerant 2 | Plastic 4</t>
+  </si>
+  <si>
+    <t>Explosive 2 | Aluminium 1</t>
+  </si>
+  <si>
+    <t>Electrolyte 2 | Copper 1</t>
+  </si>
+  <si>
+    <t>0.270 FMJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,6 +804,20 @@
       <u/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -762,7 +1040,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -915,8 +1193,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1235,9 +1523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
   <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M99" sqref="M99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,447 +3119,1074 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:16" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="57" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" t="s">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="O10" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="P10" s="57" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" t="s">
-        <v>146</v>
-      </c>
-      <c r="J5" t="s">
-        <v>136</v>
-      </c>
-      <c r="P5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F13" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L16" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O16" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" t="s">
-        <v>69</v>
-      </c>
-      <c r="L10" t="s">
-        <v>70</v>
-      </c>
-      <c r="M10" t="s">
-        <v>71</v>
-      </c>
-      <c r="N10" t="s">
-        <v>72</v>
-      </c>
-      <c r="O10" t="s">
-        <v>73</v>
-      </c>
-      <c r="P10" t="s">
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="1">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="1">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="1">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="1">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="1">
+        <v>5</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="1">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="1">
+        <v>5</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="1">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" s="1">
+        <v>10</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="1">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="1">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="1">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="1">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="1">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="C61" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="D61" s="58" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="1">
+        <v>100</v>
+      </c>
+      <c r="C62" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="1">
+        <v>100</v>
+      </c>
+      <c r="C63" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B64" s="1">
+        <v>100</v>
+      </c>
+      <c r="C64" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B65" s="1">
+        <v>100</v>
+      </c>
+      <c r="C65" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B66" s="1">
+        <v>100</v>
+      </c>
+      <c r="C66" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B67" s="1">
+        <v>100</v>
+      </c>
+      <c r="C67" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B69" s="1">
+        <v>25</v>
+      </c>
+      <c r="C69" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" s="1">
+        <v>25</v>
+      </c>
+      <c r="C71" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B73" s="1">
+        <v>25</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B74" s="1">
+        <v>25</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B75" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="K13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="C75" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B77" s="1">
+        <v>125</v>
+      </c>
+      <c r="C77" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B79" s="1">
+        <v>75</v>
+      </c>
+      <c r="C79" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B80" s="1">
+        <v>75</v>
+      </c>
+      <c r="C80" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B81" s="1">
+        <v>20</v>
+      </c>
+      <c r="C81" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B82" s="1">
+        <v>10</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B83" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>110</v>
-      </c>
-      <c r="H16" t="s">
-        <v>110</v>
-      </c>
-      <c r="L16" t="s">
-        <v>110</v>
-      </c>
-      <c r="O16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>135</v>
-      </c>
-      <c r="C21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>108</v>
+      <c r="C83" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" s="1">
+        <v>500</v>
+      </c>
+      <c r="C84" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B85" s="1">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B91" s="1">
+        <v>4</v>
+      </c>
+      <c r="C91" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B92" s="1">
+        <v>4</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3279,15 +4194,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192052B0-48AC-449A-9DF0-ED0AB105E3CE}">
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96:D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
@@ -4102,14 +5031,41 @@
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>171</v>
+      </c>
+      <c r="C76" t="s">
+        <v>168</v>
+      </c>
       <c r="D76" s="53">
         <v>0.32</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="G76" t="s">
-        <v>142</v>
+        <v>155</v>
+      </c>
+      <c r="H76" t="s">
+        <v>158</v>
+      </c>
+      <c r="I76" t="s">
+        <v>158</v>
+      </c>
+      <c r="J76" t="s">
+        <v>156</v>
+      </c>
+      <c r="K76" t="s">
+        <v>156</v>
+      </c>
+      <c r="L76" t="s">
+        <v>156</v>
+      </c>
+      <c r="M76" t="s">
+        <v>172</v>
+      </c>
+      <c r="O76" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -4153,43 +5109,243 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B79" s="53">
+        <v>0.32</v>
+      </c>
+      <c r="C79" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="E79" t="s">
+        <v>164</v>
+      </c>
+      <c r="F79" t="s">
+        <v>164</v>
+      </c>
+      <c r="G79" t="s">
+        <v>164</v>
+      </c>
+      <c r="H79" t="s">
+        <v>164</v>
+      </c>
+      <c r="I79" t="s">
+        <v>166</v>
+      </c>
+      <c r="J79" t="s">
+        <v>166</v>
+      </c>
+      <c r="K79" t="s">
+        <v>167</v>
+      </c>
+      <c r="L79" t="s">
+        <v>164</v>
+      </c>
+      <c r="M79" t="s">
+        <v>166</v>
+      </c>
+      <c r="N79" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="55">
+        <v>0.32</v>
+      </c>
+      <c r="B82" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" t="s">
+        <v>131</v>
+      </c>
+      <c r="D82" t="s">
+        <v>132</v>
+      </c>
+      <c r="E82" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="54">
-        <v>0.32</v>
-      </c>
-      <c r="B82" t="s">
-        <v>138</v>
-      </c>
-      <c r="C82" t="s">
-        <v>130</v>
-      </c>
-      <c r="D82" t="s">
-        <v>131</v>
-      </c>
-      <c r="E82" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="54" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="B83" t="s">
         <v>137</v>
       </c>
       <c r="C83" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" t="s">
+        <v>141</v>
+      </c>
+      <c r="E83" t="s">
         <v>138</v>
       </c>
-      <c r="D83" t="s">
-        <v>143</v>
-      </c>
-      <c r="E83" t="s">
-        <v>139</v>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" t="s">
+        <v>136</v>
+      </c>
+      <c r="D84" t="s">
+        <v>157</v>
+      </c>
+      <c r="E84" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="B85" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" t="s">
+        <v>152</v>
+      </c>
+      <c r="D85" t="s">
+        <v>140</v>
+      </c>
+      <c r="E85" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="55">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="B86" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" t="s">
+        <v>152</v>
+      </c>
+      <c r="D86" t="s">
+        <v>141</v>
+      </c>
+      <c r="E86" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="B87" t="s">
+        <v>159</v>
+      </c>
+      <c r="C87" t="s">
+        <v>160</v>
+      </c>
+      <c r="D87" t="s">
+        <v>161</v>
+      </c>
+      <c r="E87" t="s">
+        <v>162</v>
+      </c>
+      <c r="F87" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" t="s">
+        <v>136</v>
+      </c>
+      <c r="D88" t="s">
+        <v>165</v>
+      </c>
+      <c r="E88" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" t="s">
+        <v>137</v>
+      </c>
+      <c r="C89" t="s">
+        <v>136</v>
+      </c>
+      <c r="D89" t="s">
+        <v>157</v>
+      </c>
+      <c r="E89" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="B90" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" t="s">
+        <v>170</v>
+      </c>
+      <c r="C91" t="s">
+        <v>154</v>
+      </c>
+      <c r="D91" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="55" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="B93" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="55">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="B96" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" t="s">
+        <v>176</v>
+      </c>
+      <c r="D96" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The First City Loot added
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEACB1A-8530-49CA-A429-71FF7E916983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F823D9-7226-4BF0-B361-05F45E43021A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="289">
   <si>
     <t>Mission</t>
   </si>
@@ -861,6 +861,51 @@
   </si>
   <si>
     <t>Adhesive 2 | Rubber 3</t>
+  </si>
+  <si>
+    <t>Mauser Hunting Rifle (Lock)</t>
+  </si>
+  <si>
+    <t>Fireworks</t>
+  </si>
+  <si>
+    <t>4_8x_Rifle_Scope</t>
+  </si>
+  <si>
+    <t>Simple 1st Aid Kit (Lock)</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>Seeker Prototype</t>
+  </si>
+  <si>
+    <t>Fireworks (Lock)</t>
+  </si>
+  <si>
+    <t>Emergency Flare (Lock)</t>
+  </si>
+  <si>
+    <t>Radioactive Barrows inside</t>
+  </si>
+  <si>
+    <t>Guitar party!!!</t>
+  </si>
+  <si>
+    <t>Double Locked Hunting Rifle</t>
+  </si>
+  <si>
+    <t>On top floor</t>
+  </si>
+  <si>
+    <t>The Home Team</t>
+  </si>
+  <si>
+    <t>Civil Defense =&gt; The Home Team</t>
   </si>
 </sst>
 </file>
@@ -949,7 +994,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1141,12 +1186,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1313,6 +1445,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1630,11 +1792,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R106"/>
+  <dimension ref="A1:R148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M149" sqref="M149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,7 +1806,7 @@
     <col min="3" max="3" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="2"/>
     <col min="8" max="8" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="2"/>
@@ -3076,7 +3238,7 @@
       <c r="N89" s="15"/>
       <c r="O89" s="13"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>30</v>
       </c>
@@ -3099,16 +3261,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L91" s="19">
+    <row r="91" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K91" s="47"/>
+      <c r="L91" s="63">
         <v>5</v>
       </c>
-      <c r="M91" s="1">
+      <c r="M91" s="64">
         <v>4223</v>
       </c>
-      <c r="N91" s="1">
+      <c r="N91" s="64">
         <v>1554</v>
       </c>
+      <c r="O91" s="65"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J92" s="52" t="s">
@@ -3179,7 +3343,7 @@
       </c>
       <c r="O96" s="11"/>
     </row>
-    <row r="97" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J97" s="51" t="s">
         <v>127</v>
       </c>
@@ -3191,7 +3355,7 @@
       <c r="N97" s="15"/>
       <c r="O97" s="13"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J98" s="51" t="s">
         <v>127</v>
       </c>
@@ -3205,7 +3369,7 @@
         <v>2371</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J99" s="9" t="s">
         <v>268</v>
       </c>
@@ -3219,7 +3383,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J100" s="9" t="s">
         <v>25</v>
       </c>
@@ -3233,7 +3397,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F101" s="1" t="s">
         <v>13</v>
       </c>
@@ -3247,7 +3411,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>270</v>
       </c>
@@ -3264,7 +3428,7 @@
         <v>2863</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J103" s="9" t="s">
         <v>17</v>
       </c>
@@ -3276,7 +3440,7 @@
       </c>
       <c r="O103" s="11"/>
     </row>
-    <row r="104" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J104" s="9" t="s">
         <v>11</v>
       </c>
@@ -3284,7 +3448,7 @@
       <c r="N104" s="15"/>
       <c r="O104" s="13"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J105" s="9" t="s">
         <v>17</v>
       </c>
@@ -3295,7 +3459,7 @@
         <v>2842</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J106" s="9" t="s">
         <v>25</v>
       </c>
@@ -3309,8 +3473,626 @@
         <v>2882</v>
       </c>
     </row>
+    <row r="107" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L107" s="63">
+        <v>2</v>
+      </c>
+      <c r="M107" s="64">
+        <v>1937</v>
+      </c>
+      <c r="N107" s="64">
+        <v>3083</v>
+      </c>
+      <c r="O107" s="65"/>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K108" s="47"/>
+      <c r="L108" s="60">
+        <v>3</v>
+      </c>
+      <c r="M108" s="14">
+        <v>1946</v>
+      </c>
+      <c r="N108" s="14">
+        <v>3078</v>
+      </c>
+      <c r="O108" s="11">
+        <v>2</v>
+      </c>
+      <c r="P108" s="66" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q108" s="67"/>
+      <c r="R108" s="68"/>
+    </row>
+    <row r="109" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F109" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G109" s="2">
+        <v>2</v>
+      </c>
+      <c r="K109" s="47"/>
+      <c r="L109" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="M109" s="15">
+        <v>1953</v>
+      </c>
+      <c r="N109" s="15">
+        <v>3081</v>
+      </c>
+      <c r="O109" s="13">
+        <v>2</v>
+      </c>
+      <c r="P109" s="69" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q109" s="70"/>
+      <c r="R109" s="71"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J110" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M110" s="1">
+        <v>2016</v>
+      </c>
+      <c r="N110" s="1">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J111" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K111" s="2">
+        <v>3</v>
+      </c>
+      <c r="M111" s="1">
+        <v>2022</v>
+      </c>
+      <c r="N111" s="1">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J112" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K112" s="2">
+        <v>3</v>
+      </c>
+      <c r="M112" s="1">
+        <v>1925</v>
+      </c>
+      <c r="N112" s="1">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J113" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="K113" s="2">
+        <v>4</v>
+      </c>
+      <c r="M113" s="1">
+        <v>1908</v>
+      </c>
+      <c r="N113" s="1">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J114" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K114" s="2">
+        <v>4</v>
+      </c>
+      <c r="M114" s="1">
+        <v>1910</v>
+      </c>
+      <c r="N114" s="1">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J115" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K115" s="2">
+        <v>2</v>
+      </c>
+      <c r="M115" s="10">
+        <v>1911</v>
+      </c>
+      <c r="N115" s="14">
+        <v>3030</v>
+      </c>
+      <c r="O115" s="11"/>
+    </row>
+    <row r="116" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J116" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M116" s="12"/>
+      <c r="N116" s="15"/>
+      <c r="O116" s="13"/>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J117" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K117" s="2">
+        <v>2</v>
+      </c>
+      <c r="M117" s="1">
+        <v>1857</v>
+      </c>
+      <c r="N117" s="1">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F118" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G118" s="2">
+        <v>1</v>
+      </c>
+      <c r="M118" s="1">
+        <v>1862</v>
+      </c>
+      <c r="N118" s="1">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M119" s="1">
+        <v>1854</v>
+      </c>
+      <c r="N119" s="1">
+        <v>3021</v>
+      </c>
+      <c r="O119" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J120" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M120" s="1">
+        <v>1858</v>
+      </c>
+      <c r="N120" s="1">
+        <v>3023</v>
+      </c>
+      <c r="O120" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L121" s="19">
+        <v>0</v>
+      </c>
+      <c r="M121" s="1">
+        <v>1855</v>
+      </c>
+      <c r="N121" s="1">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J122" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="M122" s="1">
+        <v>1898</v>
+      </c>
+      <c r="N122" s="1">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M123" s="1">
+        <v>1932</v>
+      </c>
+      <c r="N123" s="1">
+        <v>3102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J124" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M124" s="1">
+        <v>1932</v>
+      </c>
+      <c r="N124" s="1">
+        <v>3108</v>
+      </c>
+      <c r="O124" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L125" s="60">
+        <v>5</v>
+      </c>
+      <c r="M125" s="14">
+        <v>1823</v>
+      </c>
+      <c r="N125" s="14">
+        <v>3088</v>
+      </c>
+      <c r="O125" s="11"/>
+      <c r="P125" s="66" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q125" s="67"/>
+      <c r="R125" s="68"/>
+    </row>
+    <row r="126" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J126" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="K126" s="2">
+        <v>3</v>
+      </c>
+      <c r="L126" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="M126" s="15">
+        <v>1817</v>
+      </c>
+      <c r="N126" s="15">
+        <v>3085</v>
+      </c>
+      <c r="O126" s="13"/>
+      <c r="P126" s="69"/>
+      <c r="Q126" s="70"/>
+      <c r="R126" s="71"/>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="M127" s="10">
+        <v>1809</v>
+      </c>
+      <c r="N127" s="14">
+        <v>3136</v>
+      </c>
+      <c r="O127" s="11"/>
+    </row>
+    <row r="128" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J128" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M128" s="12"/>
+      <c r="N128" s="15"/>
+      <c r="O128" s="13"/>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="M129" s="1">
+        <v>1805</v>
+      </c>
+      <c r="N129" s="1">
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J130" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M130" s="1">
+        <v>1810</v>
+      </c>
+      <c r="N130" s="1">
+        <v>3138</v>
+      </c>
+      <c r="O130" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J131" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K131" s="2">
+        <v>2</v>
+      </c>
+      <c r="M131" s="1">
+        <v>1795</v>
+      </c>
+      <c r="N131" s="1">
+        <v>3055</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J132" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M132" s="10">
+        <v>1705</v>
+      </c>
+      <c r="N132" s="14">
+        <v>3063</v>
+      </c>
+      <c r="O132" s="11"/>
+    </row>
+    <row r="133" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J133" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="K133" s="2">
+        <v>3</v>
+      </c>
+      <c r="M133" s="12"/>
+      <c r="N133" s="15"/>
+      <c r="O133" s="13"/>
+    </row>
+    <row r="134" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="M134" s="1">
+        <v>1713</v>
+      </c>
+      <c r="N134" s="1">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J135" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K135" s="2">
+        <v>4</v>
+      </c>
+      <c r="M135" s="10">
+        <v>1670</v>
+      </c>
+      <c r="N135" s="14">
+        <v>2983</v>
+      </c>
+      <c r="O135" s="11"/>
+    </row>
+    <row r="136" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M136" s="12"/>
+      <c r="N136" s="15"/>
+      <c r="O136" s="13"/>
+    </row>
+    <row r="137" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J137" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K137" s="2">
+        <v>2</v>
+      </c>
+      <c r="M137" s="1">
+        <v>1668</v>
+      </c>
+      <c r="N137" s="1">
+        <v>2992</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J138" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="K138" s="2">
+        <v>3</v>
+      </c>
+      <c r="M138" s="10">
+        <v>1669</v>
+      </c>
+      <c r="N138" s="14">
+        <v>2983</v>
+      </c>
+      <c r="O138" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F139" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G139" s="2">
+        <v>1</v>
+      </c>
+      <c r="M139" s="12"/>
+      <c r="N139" s="15"/>
+      <c r="O139" s="13"/>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C140" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="M140" s="1">
+        <v>1302</v>
+      </c>
+      <c r="N140" s="1">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M141" s="1">
+        <v>1464</v>
+      </c>
+      <c r="N141" s="1">
+        <v>3485</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K142" s="47"/>
+      <c r="L142" s="60">
+        <v>4</v>
+      </c>
+      <c r="M142" s="14">
+        <v>1822</v>
+      </c>
+      <c r="N142" s="14">
+        <v>3015</v>
+      </c>
+      <c r="O142" s="11"/>
+      <c r="P142" s="66" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q142" s="67"/>
+      <c r="R142" s="68"/>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J143" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="K143" s="47">
+        <v>8</v>
+      </c>
+      <c r="L143" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="M143" s="47">
+        <v>1817</v>
+      </c>
+      <c r="N143" s="47">
+        <v>3014</v>
+      </c>
+      <c r="O143" s="25">
+        <v>2</v>
+      </c>
+      <c r="P143" s="72"/>
+      <c r="Q143" s="73"/>
+      <c r="R143" s="74"/>
+    </row>
+    <row r="144" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J144" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="K144" s="47">
+        <v>3</v>
+      </c>
+      <c r="L144" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="M144" s="47"/>
+      <c r="N144" s="47"/>
+      <c r="O144" s="25">
+        <v>2</v>
+      </c>
+      <c r="P144" s="72"/>
+      <c r="Q144" s="73"/>
+      <c r="R144" s="74"/>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J145" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="K145" s="47"/>
+      <c r="L145" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="M145" s="9">
+        <v>1826</v>
+      </c>
+      <c r="N145" s="47">
+        <v>3018</v>
+      </c>
+      <c r="O145" s="25">
+        <v>2</v>
+      </c>
+      <c r="P145" s="66"/>
+      <c r="Q145" s="67"/>
+      <c r="R145" s="67"/>
+    </row>
+    <row r="146" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J146" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K146" s="47"/>
+      <c r="L146" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="M146" s="75">
+        <v>1823</v>
+      </c>
+      <c r="N146" s="15">
+        <v>3025</v>
+      </c>
+      <c r="O146" s="13"/>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A147" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B147" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M147" s="10">
+        <v>2032</v>
+      </c>
+      <c r="N147" s="14">
+        <v>3125</v>
+      </c>
+      <c r="O147" s="11">
+        <v>-1</v>
+      </c>
+      <c r="P147" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q147" s="30"/>
+      <c r="R147" s="31"/>
+    </row>
+    <row r="148" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B148" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M148" s="12"/>
+      <c r="N148" s="15"/>
+      <c r="O148" s="13"/>
+      <c r="P148" s="35"/>
+      <c r="Q148" s="36"/>
+      <c r="R148" s="37"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="P147:R148"/>
     <mergeCell ref="P57:R58"/>
     <mergeCell ref="P74:R75"/>
     <mergeCell ref="P1:R1"/>
@@ -3332,11 +4114,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P116"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D112" sqref="D112"/>
+      <selection pane="topRight" activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4581,6 +5363,14 @@
       </c>
       <c r="B115" s="1" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -5772,8 +6562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49260601-DFFC-49C5-BC21-5E0477EEDF42}">
   <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
A chunk of farm and forested hills
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F823D9-7226-4BF0-B361-05F45E43021A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068580C4-33F4-4995-AD5B-9968EC21F368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="300">
   <si>
     <t>Mission</t>
   </si>
@@ -878,9 +878,6 @@
     <t>3c</t>
   </si>
   <si>
-    <t>3d</t>
-  </si>
-  <si>
     <t>Seeker Prototype</t>
   </si>
   <si>
@@ -906,6 +903,42 @@
   </si>
   <si>
     <t>Civil Defense =&gt; The Home Team</t>
+  </si>
+  <si>
+    <t>Jane + James' Dino-Mite Wedding Mix</t>
+  </si>
+  <si>
+    <t>Adhesive 3 | Plastic 6</t>
+  </si>
+  <si>
+    <t>3 opp</t>
+  </si>
+  <si>
+    <t>1 opp</t>
+  </si>
+  <si>
+    <t>Adhesive 4 | Plastic 8</t>
+  </si>
+  <si>
+    <t>Recycle Station Upgrades</t>
+  </si>
+  <si>
+    <t>Storage Station Upgrades</t>
+  </si>
+  <si>
+    <t>16 Steel | Electrolyte 8 | Aluminium 4</t>
+  </si>
+  <si>
+    <t>Adhesive 1 | Plastic 2</t>
+  </si>
+  <si>
+    <t>16 Wood | 8 Adhesive | Aluminium 4</t>
+  </si>
+  <si>
+    <t>Object_Penetration_Vision_Modulator</t>
+  </si>
+  <si>
+    <t>Strength in Numbers</t>
   </si>
 </sst>
 </file>
@@ -1792,25 +1825,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R148"/>
+  <dimension ref="A1:R183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M149" sqref="M149"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M184" sqref="M184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="2"/>
     <col min="8" max="8" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="2"/>
-    <col min="10" max="10" width="22.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.140625" style="1" bestFit="1" customWidth="1"/>
@@ -2419,9 +2452,6 @@
       <c r="D37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="2">
-        <v>1</v>
-      </c>
       <c r="M37" s="1">
         <v>3580</v>
       </c>
@@ -3500,7 +3530,7 @@
         <v>2</v>
       </c>
       <c r="P108" s="66" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q108" s="67"/>
       <c r="R108" s="68"/>
@@ -3526,7 +3556,7 @@
         <v>2</v>
       </c>
       <c r="P109" s="69" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q109" s="70"/>
       <c r="R109" s="71"/>
@@ -3742,7 +3772,7 @@
       </c>
       <c r="O125" s="11"/>
       <c r="P125" s="66" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Q125" s="67"/>
       <c r="R125" s="68"/>
@@ -3861,7 +3891,7 @@
         <v>120</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="M134" s="1">
         <v>1713</v>
@@ -3937,7 +3967,7 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C140" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M140" s="1">
         <v>1302</v>
@@ -3970,14 +4000,14 @@
       </c>
       <c r="O142" s="11"/>
       <c r="P142" s="66" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q142" s="67"/>
       <c r="R142" s="68"/>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J143" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K143" s="47">
         <v>8</v>
@@ -4000,7 +4030,7 @@
     </row>
     <row r="144" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J144" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K144" s="47">
         <v>3</v>
@@ -4071,14 +4101,14 @@
         <v>-1</v>
       </c>
       <c r="P147" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q147" s="30"/>
       <c r="R147" s="31"/>
     </row>
     <row r="148" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B148" s="13" t="s">
         <v>27</v>
@@ -4089,6 +4119,497 @@
       <c r="P148" s="35"/>
       <c r="Q148" s="36"/>
       <c r="R148" s="37"/>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C149" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="J149" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L149" s="9"/>
+      <c r="M149" s="10">
+        <v>1791</v>
+      </c>
+      <c r="N149" s="14">
+        <v>3347</v>
+      </c>
+      <c r="O149" s="11"/>
+    </row>
+    <row r="150" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J150" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L150" s="9"/>
+      <c r="M150" s="12"/>
+      <c r="N150" s="15"/>
+      <c r="O150" s="13"/>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J151" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="M151" s="1">
+        <v>1875</v>
+      </c>
+      <c r="N151" s="1">
+        <v>3341</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M152" s="1">
+        <v>1745</v>
+      </c>
+      <c r="N152" s="1">
+        <v>3386</v>
+      </c>
+      <c r="O152" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F153" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G153" s="2">
+        <v>1</v>
+      </c>
+      <c r="M153" s="1">
+        <v>1748</v>
+      </c>
+      <c r="N153" s="1">
+        <v>3379</v>
+      </c>
+      <c r="O153" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F154" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G154" s="2">
+        <v>1</v>
+      </c>
+      <c r="J154" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K154" s="2">
+        <v>2</v>
+      </c>
+      <c r="M154" s="10">
+        <v>1668</v>
+      </c>
+      <c r="N154" s="14">
+        <v>3265</v>
+      </c>
+      <c r="O154" s="11"/>
+    </row>
+    <row r="155" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J155" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="M155" s="12"/>
+      <c r="N155" s="15"/>
+      <c r="O155" s="13"/>
+    </row>
+    <row r="156" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B156" s="2">
+        <v>1</v>
+      </c>
+      <c r="J156" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M156" s="1">
+        <v>1613</v>
+      </c>
+      <c r="N156" s="1">
+        <v>3151</v>
+      </c>
+      <c r="O156" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A157" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B157" s="2">
+        <v>2</v>
+      </c>
+      <c r="J157" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="M157" s="10">
+        <v>1627</v>
+      </c>
+      <c r="N157" s="14">
+        <v>3146</v>
+      </c>
+      <c r="O157" s="11"/>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J158" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="M158" s="16"/>
+      <c r="O158" s="25"/>
+    </row>
+    <row r="159" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J159" s="51" t="s">
+        <v>268</v>
+      </c>
+      <c r="K159" s="2">
+        <v>2</v>
+      </c>
+      <c r="M159" s="12"/>
+      <c r="N159" s="15"/>
+      <c r="O159" s="13"/>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A160" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="J160" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K160" s="2">
+        <v>4</v>
+      </c>
+      <c r="M160" s="1">
+        <v>1624</v>
+      </c>
+      <c r="N160" s="1">
+        <v>3154</v>
+      </c>
+      <c r="O160" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J161" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K161" s="2">
+        <v>3</v>
+      </c>
+      <c r="M161" s="1">
+        <v>1211</v>
+      </c>
+      <c r="N161" s="1">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D162" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M162" s="1">
+        <v>1183</v>
+      </c>
+      <c r="N162" s="1">
+        <v>3363</v>
+      </c>
+      <c r="O162" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H163" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I163" s="2">
+        <v>1</v>
+      </c>
+      <c r="J163" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K163" s="2">
+        <v>3</v>
+      </c>
+      <c r="M163" s="10">
+        <v>1183</v>
+      </c>
+      <c r="N163" s="14">
+        <v>3367</v>
+      </c>
+      <c r="O163" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J164" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M164" s="12"/>
+      <c r="N164" s="15"/>
+      <c r="O164" s="13"/>
+    </row>
+    <row r="165" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F165" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G165" s="2">
+        <v>1</v>
+      </c>
+      <c r="J165" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K165" s="2">
+        <v>2</v>
+      </c>
+      <c r="M165" s="1">
+        <v>1186</v>
+      </c>
+      <c r="N165" s="1">
+        <v>3362</v>
+      </c>
+      <c r="O165" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F166" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G166" s="2">
+        <v>1</v>
+      </c>
+      <c r="J166" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M166" s="10">
+        <v>1200</v>
+      </c>
+      <c r="N166" s="14">
+        <v>3519</v>
+      </c>
+      <c r="O166" s="11"/>
+    </row>
+    <row r="167" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J167" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M167" s="16"/>
+      <c r="O167" s="25"/>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L168" s="9"/>
+      <c r="M168" s="48">
+        <v>800</v>
+      </c>
+      <c r="N168" s="14">
+        <v>3514</v>
+      </c>
+      <c r="O168" s="49"/>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J169" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M169" s="1">
+        <v>1095</v>
+      </c>
+      <c r="N169" s="1">
+        <v>3510</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J170" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K170" s="2">
+        <v>3</v>
+      </c>
+      <c r="M170" s="1">
+        <v>1316</v>
+      </c>
+      <c r="N170" s="1">
+        <v>3370</v>
+      </c>
+      <c r="O170" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J171" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="M171" s="1">
+        <v>950</v>
+      </c>
+      <c r="N171" s="1">
+        <v>3745</v>
+      </c>
+      <c r="O171" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J172" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M172" s="1">
+        <v>935</v>
+      </c>
+      <c r="N172" s="1">
+        <v>3586</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F173" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G173" s="2">
+        <v>1</v>
+      </c>
+      <c r="M173" s="1">
+        <v>915</v>
+      </c>
+      <c r="N173" s="1">
+        <v>3597</v>
+      </c>
+      <c r="O173" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J174" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M174" s="1">
+        <v>950</v>
+      </c>
+      <c r="N174" s="1">
+        <v>3486</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F175" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G175" s="2">
+        <v>1</v>
+      </c>
+      <c r="M175" s="1">
+        <v>995</v>
+      </c>
+      <c r="N175" s="1">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J176" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M176" s="1">
+        <v>942</v>
+      </c>
+      <c r="N176" s="1">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J177" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="M177" s="10">
+        <v>535</v>
+      </c>
+      <c r="N177" s="14">
+        <v>3398</v>
+      </c>
+      <c r="O177" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J178" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M178" s="12"/>
+      <c r="N178" s="15"/>
+      <c r="O178" s="13"/>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J179" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K179" s="2">
+        <v>3</v>
+      </c>
+      <c r="M179" s="1">
+        <v>462</v>
+      </c>
+      <c r="N179" s="1">
+        <v>3663</v>
+      </c>
+      <c r="O179" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M180" s="1">
+        <v>466</v>
+      </c>
+      <c r="N180" s="1">
+        <v>3641</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M181" s="1">
+        <v>466</v>
+      </c>
+      <c r="N181" s="1">
+        <v>3643</v>
+      </c>
+      <c r="O181" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J182" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K182" s="2">
+        <v>3</v>
+      </c>
+      <c r="M182" s="10">
+        <v>457</v>
+      </c>
+      <c r="N182" s="14">
+        <v>3641</v>
+      </c>
+      <c r="O182" s="11"/>
+    </row>
+    <row r="183" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J183" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M183" s="12"/>
+      <c r="N183" s="15"/>
+      <c r="O183" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -4114,21 +4635,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P116"/>
+  <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A87" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C116" sqref="C116"/>
+      <selection pane="topRight" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -4209,6 +4730,9 @@
       <c r="K3" s="1" t="s">
         <v>148</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -4336,6 +4860,9 @@
       <c r="G11" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -4344,6 +4871,9 @@
       <c r="B12" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -4614,6 +5144,15 @@
       <c r="A40" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="B40" s="1">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -4934,6 +5473,15 @@
       <c r="A70" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="B70" s="1">
+        <v>25</v>
+      </c>
+      <c r="C70" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
@@ -4953,6 +5501,15 @@
       <c r="A72" s="1" t="s">
         <v>213</v>
       </c>
+      <c r="B72" s="1">
+        <v>25</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
@@ -5000,6 +5557,15 @@
       <c r="A76" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="B76" s="1">
+        <v>75</v>
+      </c>
+      <c r="C76" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -5132,9 +5698,15 @@
       <c r="A88" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88"/>
+      <c r="B88" s="1">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
@@ -5262,6 +5834,9 @@
       <c r="A103" s="1" t="s">
         <v>253</v>
       </c>
+      <c r="B103" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="D103" s="1" t="s">
         <v>258</v>
       </c>
@@ -5345,6 +5920,9 @@
       <c r="A113" s="1" t="s">
         <v>260</v>
       </c>
+      <c r="B113" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="C113" s="1" t="s">
         <v>261</v>
       </c>
@@ -5371,6 +5949,14 @@
       </c>
       <c r="B116" s="1" t="s">
         <v>246</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -5386,12 +5972,131 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55303D08-B4AE-4EBE-A1E9-A3155C29D25A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6562,8 +7267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49260601-DFFC-49C5-BC21-5E0477EEDF42}">
   <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reached the Archipelago Region War Board
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068580C4-33F4-4995-AD5B-9968EC21F368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D06425A-8B64-42F1-B85B-70AF2D952C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="321">
   <si>
     <t>Mission</t>
   </si>
@@ -939,6 +939,69 @@
   </si>
   <si>
     <t>Strength in Numbers</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Bunker Door</t>
+  </si>
+  <si>
+    <t>.44 Magnus (Lock)</t>
+  </si>
+  <si>
+    <t>Boombox (Lock)</t>
+  </si>
+  <si>
+    <t>Adrenaline (Lock)</t>
+  </si>
+  <si>
+    <t>Advance 1st Aid Kit (Lock)</t>
+  </si>
+  <si>
+    <t>*-*</t>
+  </si>
+  <si>
+    <t>Collect 3 Key cards in area.</t>
+  </si>
+  <si>
+    <t>Unbearable Lightness</t>
+  </si>
+  <si>
+    <t>Blast-Resistant Pants</t>
+  </si>
+  <si>
+    <t>Adhesive 2 | Steel 4</t>
+  </si>
+  <si>
+    <t>2x_Red_Dot_Scope</t>
+  </si>
+  <si>
+    <t>IR_Vision_Processor</t>
+  </si>
+  <si>
+    <t>Electrolyte 1 | Plastic 2</t>
+  </si>
+  <si>
+    <t>2 TVs</t>
+  </si>
+  <si>
+    <t>Command Bunker Network</t>
+  </si>
+  <si>
+    <t>Where The Sun Sets</t>
+  </si>
+  <si>
+    <t>Calling For Help</t>
+  </si>
+  <si>
+    <t>First Contact</t>
+  </si>
+  <si>
+    <t>Another Castle</t>
+  </si>
+  <si>
+    <t>Archipelago Region War Board</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1090,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1306,12 +1369,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1510,6 +1586,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -1825,16 +1904,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R183"/>
+  <dimension ref="A1:R218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M184" sqref="M184"/>
+      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M219" sqref="M219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" bestFit="1" customWidth="1"/>
@@ -4070,7 +4149,7 @@
     </row>
     <row r="146" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J146" s="9" t="s">
-        <v>38</v>
+        <v>303</v>
       </c>
       <c r="K146" s="47"/>
       <c r="L146" s="12" t="s">
@@ -4610,6 +4689,523 @@
       <c r="M183" s="12"/>
       <c r="N183" s="15"/>
       <c r="O183" s="13"/>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J184" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K184" s="2">
+        <v>3</v>
+      </c>
+      <c r="M184" s="1">
+        <v>1213</v>
+      </c>
+      <c r="N184" s="1">
+        <v>3761</v>
+      </c>
+      <c r="O184" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J185" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K185" s="2">
+        <v>2</v>
+      </c>
+      <c r="M185" s="1">
+        <v>1679</v>
+      </c>
+      <c r="N185" s="1">
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J186" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M186" s="1">
+        <v>1687</v>
+      </c>
+      <c r="N186" s="1">
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F187" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G187" s="2">
+        <v>1</v>
+      </c>
+      <c r="M187" s="1">
+        <v>1681</v>
+      </c>
+      <c r="N187" s="1">
+        <v>3768</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F188" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G188" s="2">
+        <v>1</v>
+      </c>
+      <c r="M188" s="1">
+        <v>1689</v>
+      </c>
+      <c r="N188" s="1">
+        <v>3774</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K189" s="47"/>
+      <c r="L189" s="63">
+        <v>6</v>
+      </c>
+      <c r="M189" s="64">
+        <v>1537</v>
+      </c>
+      <c r="N189" s="64">
+        <v>3836</v>
+      </c>
+      <c r="O189" s="65"/>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A190" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B190" s="2">
+        <v>3</v>
+      </c>
+      <c r="M190" s="1">
+        <v>1409</v>
+      </c>
+      <c r="N190" s="1">
+        <v>3873</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A191" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M191" s="1">
+        <v>1516</v>
+      </c>
+      <c r="N191" s="1">
+        <v>3888</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="M192" s="1">
+        <v>1418</v>
+      </c>
+      <c r="N192" s="1">
+        <v>3925</v>
+      </c>
+    </row>
+    <row r="193" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L193" s="63">
+        <v>6</v>
+      </c>
+      <c r="M193" s="64">
+        <v>1382</v>
+      </c>
+      <c r="N193" s="64">
+        <v>3898</v>
+      </c>
+      <c r="O193" s="65"/>
+    </row>
+    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="L194" s="2"/>
+      <c r="M194" s="1">
+        <v>1516</v>
+      </c>
+      <c r="N194" s="1">
+        <v>3888</v>
+      </c>
+      <c r="O194" s="47"/>
+    </row>
+    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="M195" s="1">
+        <v>1577</v>
+      </c>
+      <c r="N195" s="1">
+        <v>3933</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="M196" s="1">
+        <v>1561</v>
+      </c>
+      <c r="N196" s="1">
+        <v>3753</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="M197" s="1">
+        <v>1409</v>
+      </c>
+      <c r="N197" s="1">
+        <v>3873</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J198" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K198" s="2">
+        <v>3</v>
+      </c>
+      <c r="M198" s="1">
+        <v>1711</v>
+      </c>
+      <c r="N198" s="1">
+        <v>4111</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J199" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K199" s="2">
+        <v>2</v>
+      </c>
+      <c r="M199" s="1">
+        <v>1719</v>
+      </c>
+      <c r="N199" s="1">
+        <v>4076</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J200" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K200" s="2">
+        <v>3</v>
+      </c>
+      <c r="M200" s="1">
+        <v>1708</v>
+      </c>
+      <c r="N200" s="1">
+        <v>4079</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F201" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G201" s="2">
+        <v>1</v>
+      </c>
+      <c r="M201" s="1">
+        <v>1570</v>
+      </c>
+      <c r="N201" s="1">
+        <v>4118</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F202" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="G202" s="2">
+        <v>1</v>
+      </c>
+      <c r="J202" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="K202" s="47">
+        <v>2</v>
+      </c>
+      <c r="L202" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="M202" s="14">
+        <v>1564</v>
+      </c>
+      <c r="N202" s="14">
+        <v>4115</v>
+      </c>
+      <c r="O202" s="11"/>
+    </row>
+    <row r="203" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J203" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="K203" s="47"/>
+      <c r="L203" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="M203" s="47"/>
+      <c r="N203" s="47"/>
+      <c r="O203" s="25"/>
+    </row>
+    <row r="204" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K204" s="47"/>
+      <c r="L204" s="48"/>
+      <c r="M204" s="48">
+        <v>1584</v>
+      </c>
+      <c r="N204" s="14">
+        <v>4274</v>
+      </c>
+      <c r="O204" s="49"/>
+    </row>
+    <row r="205" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B205" s="2">
+        <v>4</v>
+      </c>
+      <c r="M205" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="N205" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="O205" s="47"/>
+      <c r="P205" s="76" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q205" s="77"/>
+      <c r="R205" s="78"/>
+    </row>
+    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A206" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B206" s="2">
+        <v>5</v>
+      </c>
+      <c r="M206" s="1">
+        <v>1409</v>
+      </c>
+      <c r="N206" s="1">
+        <v>3873</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M207" s="1">
+        <v>1470</v>
+      </c>
+      <c r="N207" s="1">
+        <v>3864</v>
+      </c>
+      <c r="O207" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J208" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K208" s="2">
+        <v>3</v>
+      </c>
+      <c r="M208" s="1">
+        <v>1530</v>
+      </c>
+      <c r="N208" s="1">
+        <v>3834</v>
+      </c>
+      <c r="O208" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D209" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E209" s="2">
+        <v>1</v>
+      </c>
+      <c r="M209" s="1">
+        <v>1510</v>
+      </c>
+      <c r="N209" s="1">
+        <v>3793</v>
+      </c>
+      <c r="O209" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A210" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B210" s="2">
+        <v>6</v>
+      </c>
+      <c r="M210" s="1">
+        <v>1598</v>
+      </c>
+      <c r="N210" s="1">
+        <v>3880</v>
+      </c>
+      <c r="O210" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F211" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G211" s="2">
+        <v>1</v>
+      </c>
+      <c r="M211" s="1">
+        <v>1522</v>
+      </c>
+      <c r="N211" s="1">
+        <v>3775</v>
+      </c>
+      <c r="O211" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="M212" s="1">
+        <v>1520</v>
+      </c>
+      <c r="N212" s="1">
+        <v>3770</v>
+      </c>
+      <c r="O212" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A213" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L213" s="9"/>
+      <c r="M213" s="10">
+        <v>1523</v>
+      </c>
+      <c r="N213" s="14">
+        <v>3769</v>
+      </c>
+      <c r="O213" s="11">
+        <v>-1</v>
+      </c>
+      <c r="P213" s="66" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q213" s="67"/>
+      <c r="R213" s="68"/>
+    </row>
+    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L214" s="9"/>
+      <c r="M214" s="16"/>
+      <c r="N214" s="47"/>
+      <c r="O214" s="25"/>
+      <c r="P214" s="72"/>
+      <c r="Q214" s="73"/>
+      <c r="R214" s="74"/>
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L215" s="9"/>
+      <c r="M215" s="16"/>
+      <c r="N215" s="47"/>
+      <c r="O215" s="25"/>
+      <c r="P215" s="72"/>
+      <c r="Q215" s="73"/>
+      <c r="R215" s="74"/>
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L216" s="9"/>
+      <c r="M216" s="16"/>
+      <c r="N216" s="47"/>
+      <c r="O216" s="25"/>
+      <c r="P216" s="72"/>
+      <c r="Q216" s="73"/>
+      <c r="R216" s="74"/>
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L217" s="9"/>
+      <c r="M217" s="16"/>
+      <c r="N217" s="47"/>
+      <c r="O217" s="25"/>
+      <c r="P217" s="72"/>
+      <c r="Q217" s="73"/>
+      <c r="R217" s="74"/>
+    </row>
+    <row r="218" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L218" s="9"/>
+      <c r="M218" s="12"/>
+      <c r="N218" s="15"/>
+      <c r="O218" s="13"/>
+      <c r="P218" s="69"/>
+      <c r="Q218" s="70"/>
+      <c r="R218" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -4635,11 +5231,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P117"/>
+  <dimension ref="A1:P119"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A118" sqref="A118"/>
+      <selection pane="topRight" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4727,6 +5323,9 @@
       <c r="H3" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>148</v>
       </c>
@@ -5129,6 +5728,15 @@
       <c r="A37" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="B37" s="1">
+        <v>10</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -5138,6 +5746,15 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>92</v>
+      </c>
+      <c r="B39" s="1">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -5956,6 +6573,22 @@
         <v>298</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>272</v>
       </c>
     </row>
@@ -7267,8 +7900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49260601-DFFC-49C5-BC21-5E0477EEDF42}">
   <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mission Update for Recon Update
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC810E5-6E49-40FA-A36E-290017354BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3676C97-3A86-4EB9-9FF5-F09DE9B37320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="2310" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="328">
   <si>
     <t>Mission</t>
   </si>
@@ -395,9 +395,6 @@
     <t>Älgstudsare Hunting Rifle</t>
   </si>
   <si>
-    <t>S/E</t>
-  </si>
-  <si>
     <t>1-4x Rifle Scope</t>
   </si>
   <si>
@@ -1023,6 +1020,9 @@
   </si>
   <si>
     <t>Runner Prototype</t>
+  </si>
+  <si>
+    <t>The Home Team =&gt; Calling For Help</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1479,72 +1479,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1561,7 +1495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1569,9 +1503,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1602,7 +1533,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1610,6 +1540,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -1925,11 +1926,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R229"/>
+  <dimension ref="A1:R230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M230" sqref="M230"/>
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M231" sqref="M231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,42 +1953,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="26" t="s">
+      <c r="E1" s="63"/>
+      <c r="F1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="63"/>
+      <c r="H1" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="26" t="s">
+      <c r="I1" s="63"/>
+      <c r="J1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="27"/>
+      <c r="K1" s="63"/>
       <c r="L1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="26" t="s">
+      <c r="N1" s="62"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="27"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="63"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2051,11 +2052,11 @@
         <v>2197</v>
       </c>
       <c r="O3" s="1"/>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="40"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="69"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2068,9 +2069,9 @@
         <v>2199</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="43"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="72"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
@@ -2087,9 +2088,9 @@
         <v>2209</v>
       </c>
       <c r="O5" s="14"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="43"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="72"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J6" s="9" t="s">
@@ -2099,9 +2100,9 @@
       <c r="M6" s="12"/>
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="43"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="72"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J7" s="9" t="s">
@@ -2115,9 +2116,9 @@
         <v>2207</v>
       </c>
       <c r="O7" s="14"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="43"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="72"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J8" s="9" t="s">
@@ -2126,9 +2127,9 @@
       <c r="L8" s="9"/>
       <c r="M8" s="16"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="43"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="72"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J9" s="9" t="s">
@@ -2137,9 +2138,9 @@
       <c r="L9" s="9"/>
       <c r="M9" s="16"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="43"/>
+      <c r="P9" s="70"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="72"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="s">
@@ -2152,9 +2153,9 @@
       <c r="M10" s="12"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="43"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="72"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J11" s="9" t="s">
@@ -2169,9 +2170,9 @@
       <c r="O11" s="1">
         <v>2</v>
       </c>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="43"/>
+      <c r="P11" s="70"/>
+      <c r="Q11" s="71"/>
+      <c r="R11" s="72"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2190,9 +2191,9 @@
       <c r="O12" s="14">
         <v>2</v>
       </c>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="43"/>
+      <c r="P12" s="70"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="72"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="9" t="s">
@@ -2202,9 +2203,9 @@
       <c r="M13" s="12"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="43"/>
+      <c r="P13" s="70"/>
+      <c r="Q13" s="71"/>
+      <c r="R13" s="72"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J14" s="9" t="s">
@@ -2219,9 +2220,9 @@
       <c r="O14" s="1">
         <v>2</v>
       </c>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="43"/>
+      <c r="P14" s="70"/>
+      <c r="Q14" s="71"/>
+      <c r="R14" s="72"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
@@ -2234,9 +2235,9 @@
         <v>2210</v>
       </c>
       <c r="O15" s="1"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="46"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="75"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -2253,7 +2254,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J17" s="51" t="s">
+      <c r="J17" s="29" t="s">
         <v>11</v>
       </c>
       <c r="K17" s="2">
@@ -2266,11 +2267,11 @@
         <v>2243</v>
       </c>
       <c r="O17" s="1"/>
-      <c r="P17" s="29" t="s">
+      <c r="P17" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="31"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="57"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J18" s="9" t="s">
@@ -2289,28 +2290,28 @@
       <c r="O18" s="14">
         <v>2</v>
       </c>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="34"/>
+      <c r="P18" s="64"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="66"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J19" s="51" t="s">
+      <c r="J19" s="29" t="s">
         <v>25</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="16"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="34"/>
+      <c r="P19" s="64"/>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="66"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L20" s="9"/>
       <c r="M20" s="16"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="34"/>
+      <c r="P20" s="64"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="66"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
@@ -2322,9 +2323,9 @@
       <c r="L21" s="9"/>
       <c r="M21" s="16"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="34"/>
+      <c r="P21" s="64"/>
+      <c r="Q21" s="65"/>
+      <c r="R21" s="66"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H22" s="1" t="s">
@@ -2337,9 +2338,9 @@
       <c r="M22" s="12"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="37"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="60"/>
     </row>
     <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -2370,11 +2371,11 @@
         <v>2228</v>
       </c>
       <c r="O24" s="11"/>
-      <c r="P24" s="38" t="s">
+      <c r="P24" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="Q24" s="39"/>
-      <c r="R24" s="40"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="69"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
@@ -2387,9 +2388,9 @@
       <c r="M25" s="12"/>
       <c r="N25" s="15"/>
       <c r="O25" s="13"/>
-      <c r="P25" s="44"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="46"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="75"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -2406,7 +2407,7 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J27" s="51" t="s">
+      <c r="J27" s="29" t="s">
         <v>25</v>
       </c>
       <c r="M27" s="1">
@@ -2439,7 +2440,7 @@
       <c r="P28" s="22"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J29" s="51" t="s">
+      <c r="J29" s="29" t="s">
         <v>17</v>
       </c>
       <c r="M29" s="1">
@@ -2454,7 +2455,7 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J30" s="51" t="s">
+      <c r="J30" s="29" t="s">
         <v>17</v>
       </c>
       <c r="M30" s="1">
@@ -2471,7 +2472,7 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J31" s="51" t="s">
+      <c r="J31" s="29" t="s">
         <v>17</v>
       </c>
       <c r="M31" s="1">
@@ -2527,7 +2528,7 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J35" s="51" t="s">
+      <c r="J35" s="29" t="s">
         <v>11</v>
       </c>
       <c r="M35" s="1">
@@ -2624,11 +2625,11 @@
       <c r="O41" s="11">
         <v>2</v>
       </c>
-      <c r="P41" s="38" t="s">
+      <c r="P41" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="Q41" s="39"/>
-      <c r="R41" s="40"/>
+      <c r="Q41" s="68"/>
+      <c r="R41" s="69"/>
     </row>
     <row r="42" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
@@ -2641,9 +2642,9 @@
       <c r="M42" s="12"/>
       <c r="N42" s="15"/>
       <c r="O42" s="13"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="46"/>
+      <c r="P42" s="73"/>
+      <c r="Q42" s="74"/>
+      <c r="R42" s="75"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
@@ -2734,7 +2735,7 @@
       <c r="C48" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J48" s="52" t="s">
+      <c r="J48" s="30" t="s">
         <v>86</v>
       </c>
       <c r="L48" s="9"/>
@@ -2752,7 +2753,7 @@
       <c r="B49" s="2">
         <v>2</v>
       </c>
-      <c r="J49" s="52" t="s">
+      <c r="J49" s="30" t="s">
         <v>86</v>
       </c>
       <c r="K49" s="2">
@@ -2793,7 +2794,7 @@
       <c r="G51" s="2">
         <v>1</v>
       </c>
-      <c r="J51" s="51" t="s">
+      <c r="J51" s="29" t="s">
         <v>11</v>
       </c>
       <c r="K51" s="2">
@@ -2810,7 +2811,7 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J52" s="51" t="s">
+      <c r="J52" s="29" t="s">
         <v>11</v>
       </c>
       <c r="K52" s="2">
@@ -2825,7 +2826,7 @@
       <c r="O52" s="11"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J53" s="51" t="s">
+      <c r="J53" s="29" t="s">
         <v>85</v>
       </c>
       <c r="K53" s="2">
@@ -2862,7 +2863,7 @@
       </c>
     </row>
     <row r="56" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J56" s="51" t="s">
+      <c r="J56" s="29" t="s">
         <v>25</v>
       </c>
       <c r="K56" s="2">
@@ -2895,11 +2896,11 @@
       <c r="O57" s="11">
         <v>2</v>
       </c>
-      <c r="P57" s="29" t="s">
+      <c r="P57" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="Q57" s="30"/>
-      <c r="R57" s="31"/>
+      <c r="Q57" s="56"/>
+      <c r="R57" s="57"/>
     </row>
     <row r="58" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
@@ -2912,9 +2913,9 @@
       <c r="M58" s="12"/>
       <c r="N58" s="15"/>
       <c r="O58" s="13"/>
-      <c r="P58" s="35"/>
-      <c r="Q58" s="36"/>
-      <c r="R58" s="37"/>
+      <c r="P58" s="58"/>
+      <c r="Q58" s="59"/>
+      <c r="R58" s="60"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -2956,7 +2957,7 @@
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J62" s="51" t="s">
+      <c r="J62" s="29" t="s">
         <v>25</v>
       </c>
       <c r="K62" s="2">
@@ -2981,7 +2982,13 @@
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J64" s="51" t="s">
+      <c r="A64" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J64" s="29" t="s">
         <v>25</v>
       </c>
       <c r="K64" s="2">
@@ -3002,7 +3009,7 @@
         <v>115</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
       <c r="M65" s="1">
         <v>2324</v>
@@ -3055,19 +3062,19 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H69" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I69" s="2">
         <v>1</v>
       </c>
-      <c r="J69" s="51" t="s">
+      <c r="J69" s="29" t="s">
         <v>25</v>
       </c>
       <c r="L69" s="9"/>
       <c r="M69" s="9">
         <v>2088</v>
       </c>
-      <c r="N69" s="47">
+      <c r="N69" s="1">
         <v>3125</v>
       </c>
       <c r="O69" s="2">
@@ -3075,14 +3082,14 @@
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J70" s="51" t="s">
+      <c r="J70" s="29" t="s">
         <v>11</v>
       </c>
       <c r="L70" s="9"/>
       <c r="M70" s="9">
         <v>1983</v>
       </c>
-      <c r="N70" s="47">
+      <c r="N70" s="1">
         <v>3184</v>
       </c>
       <c r="O70" s="2">
@@ -3121,7 +3128,7 @@
       </c>
     </row>
     <row r="73" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J73" s="51" t="s">
+      <c r="J73" s="29" t="s">
         <v>11</v>
       </c>
       <c r="M73" s="1">
@@ -3150,15 +3157,15 @@
       <c r="O74" s="11">
         <v>-1</v>
       </c>
-      <c r="P74" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q74" s="30"/>
-      <c r="R74" s="31"/>
+      <c r="P74" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q74" s="56"/>
+      <c r="R74" s="57"/>
     </row>
     <row r="75" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>27</v>
@@ -3166,9 +3173,9 @@
       <c r="M75" s="12"/>
       <c r="N75" s="15"/>
       <c r="O75" s="13"/>
-      <c r="P75" s="35"/>
-      <c r="Q75" s="36"/>
-      <c r="R75" s="37"/>
+      <c r="P75" s="58"/>
+      <c r="Q75" s="59"/>
+      <c r="R75" s="60"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J76" s="9" t="s">
@@ -3200,7 +3207,7 @@
     </row>
     <row r="78" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E78" s="2">
         <v>1</v>
@@ -3245,30 +3252,29 @@
       </c>
       <c r="L80" s="9"/>
       <c r="M80" s="16"/>
-      <c r="N80" s="47"/>
       <c r="O80" s="25"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B81" s="2">
         <v>1</v>
       </c>
       <c r="L81" s="9"/>
-      <c r="M81" s="48">
+      <c r="M81" s="26">
         <v>2033</v>
       </c>
       <c r="N81" s="14">
         <v>3123</v>
       </c>
-      <c r="O81" s="49">
+      <c r="O81" s="27">
         <v>-1</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B82" s="2">
         <v>2</v>
@@ -3284,7 +3290,7 @@
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J83" s="51" t="s">
+      <c r="J83" s="29" t="s">
         <v>38</v>
       </c>
       <c r="M83" s="1">
@@ -3295,7 +3301,7 @@
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J84" s="51" t="s">
+      <c r="J84" s="29" t="s">
         <v>11</v>
       </c>
       <c r="M84" s="1">
@@ -3306,7 +3312,7 @@
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J85" s="51" t="s">
+      <c r="J85" s="29" t="s">
         <v>38</v>
       </c>
       <c r="M85" s="1">
@@ -3342,7 +3348,7 @@
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J88" s="51" t="s">
+      <c r="J88" s="29" t="s">
         <v>11</v>
       </c>
       <c r="K88" s="2">
@@ -3376,7 +3382,7 @@
         <v>28</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I90" s="2">
         <v>1</v>
@@ -3392,20 +3398,20 @@
       </c>
     </row>
     <row r="91" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K91" s="47"/>
-      <c r="L91" s="63">
+      <c r="K91" s="1"/>
+      <c r="L91" s="40">
         <v>5</v>
       </c>
-      <c r="M91" s="64">
+      <c r="M91" s="41">
         <v>4223</v>
       </c>
-      <c r="N91" s="64">
+      <c r="N91" s="41">
         <v>1554</v>
       </c>
-      <c r="O91" s="65"/>
+      <c r="O91" s="42"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J92" s="52" t="s">
+      <c r="J92" s="30" t="s">
         <v>86</v>
       </c>
       <c r="K92" s="2">
@@ -3419,7 +3425,7 @@
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J93" s="52" t="s">
+      <c r="J93" s="30" t="s">
         <v>86</v>
       </c>
       <c r="M93" s="1">
@@ -3444,7 +3450,7 @@
       </c>
     </row>
     <row r="95" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J95" s="51" t="s">
+      <c r="J95" s="29" t="s">
         <v>11</v>
       </c>
       <c r="K95" s="2">
@@ -3458,7 +3464,7 @@
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J96" s="51" t="s">
+      <c r="J96" s="29" t="s">
         <v>25</v>
       </c>
       <c r="K96" s="2">
@@ -3474,8 +3480,8 @@
       <c r="O96" s="11"/>
     </row>
     <row r="97" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J97" s="51" t="s">
-        <v>127</v>
+      <c r="J97" s="29" t="s">
+        <v>126</v>
       </c>
       <c r="K97" s="2">
         <v>2</v>
@@ -3486,8 +3492,8 @@
       <c r="O97" s="13"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J98" s="51" t="s">
-        <v>127</v>
+      <c r="J98" s="29" t="s">
+        <v>126</v>
       </c>
       <c r="K98" s="2">
         <v>3</v>
@@ -3501,7 +3507,7 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J99" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K99" s="2">
         <v>2</v>
@@ -3543,7 +3549,7 @@
     </row>
     <row r="102" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>27</v>
@@ -3604,20 +3610,20 @@
       </c>
     </row>
     <row r="107" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L107" s="63">
+      <c r="L107" s="40">
         <v>2</v>
       </c>
-      <c r="M107" s="64">
+      <c r="M107" s="41">
         <v>1937</v>
       </c>
-      <c r="N107" s="64">
+      <c r="N107" s="41">
         <v>3083</v>
       </c>
-      <c r="O107" s="65"/>
+      <c r="O107" s="42"/>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K108" s="47"/>
-      <c r="L108" s="60">
+      <c r="K108" s="1"/>
+      <c r="L108" s="37">
         <v>3</v>
       </c>
       <c r="M108" s="14">
@@ -3629,21 +3635,21 @@
       <c r="O108" s="11">
         <v>2</v>
       </c>
-      <c r="P108" s="66" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q108" s="67"/>
-      <c r="R108" s="68"/>
+      <c r="P108" s="43" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q108" s="44"/>
+      <c r="R108" s="45"/>
     </row>
     <row r="109" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F109" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G109" s="2">
         <v>2</v>
       </c>
-      <c r="K109" s="47"/>
-      <c r="L109" s="61" t="s">
+      <c r="K109" s="1"/>
+      <c r="L109" s="38" t="s">
         <v>110</v>
       </c>
       <c r="M109" s="15">
@@ -3655,11 +3661,11 @@
       <c r="O109" s="13">
         <v>2</v>
       </c>
-      <c r="P109" s="69" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q109" s="70"/>
-      <c r="R109" s="71"/>
+      <c r="P109" s="46" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q109" s="47"/>
+      <c r="R109" s="48"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J110" s="9" t="s">
@@ -3702,7 +3708,7 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J113" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K113" s="2">
         <v>4</v>
@@ -3781,7 +3787,7 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>40</v>
@@ -3834,7 +3840,7 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>41</v>
@@ -3861,7 +3867,7 @@
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="L125" s="60">
+      <c r="L125" s="37">
         <v>5</v>
       </c>
       <c r="M125" s="14">
@@ -3871,20 +3877,20 @@
         <v>3088</v>
       </c>
       <c r="O125" s="11"/>
-      <c r="P125" s="66" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q125" s="67"/>
-      <c r="R125" s="68"/>
+      <c r="P125" s="43" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q125" s="44"/>
+      <c r="R125" s="45"/>
     </row>
     <row r="126" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J126" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K126" s="2">
         <v>3</v>
       </c>
-      <c r="L126" s="61" t="s">
+      <c r="L126" s="38" t="s">
         <v>110</v>
       </c>
       <c r="M126" s="15">
@@ -3894,16 +3900,16 @@
         <v>3085</v>
       </c>
       <c r="O126" s="13"/>
-      <c r="P126" s="69"/>
-      <c r="Q126" s="70"/>
-      <c r="R126" s="71"/>
+      <c r="P126" s="46"/>
+      <c r="Q126" s="47"/>
+      <c r="R126" s="48"/>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M127" s="10">
         <v>1809</v>
@@ -3923,10 +3929,10 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M129" s="1">
         <v>1805</v>
@@ -3977,7 +3983,7 @@
     </row>
     <row r="133" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J133" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K133" s="2">
         <v>3</v>
@@ -3988,10 +3994,10 @@
     </row>
     <row r="134" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M134" s="1">
         <v>1713</v>
@@ -4039,7 +4045,7 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J138" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K138" s="2">
         <v>3</v>
@@ -4067,7 +4073,7 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C140" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M140" s="1">
         <v>1302</v>
@@ -4088,8 +4094,8 @@
       </c>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K142" s="47"/>
-      <c r="L142" s="60">
+      <c r="K142" s="1"/>
+      <c r="L142" s="37">
         <v>4</v>
       </c>
       <c r="M142" s="14">
@@ -4099,84 +4105,80 @@
         <v>3015</v>
       </c>
       <c r="O142" s="11"/>
-      <c r="P142" s="66" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q142" s="67"/>
-      <c r="R142" s="68"/>
+      <c r="P142" s="43" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q142" s="44"/>
+      <c r="R142" s="45"/>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J143" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="K143" s="47">
+        <v>279</v>
+      </c>
+      <c r="K143" s="1">
         <v>8</v>
       </c>
-      <c r="L143" s="62" t="s">
+      <c r="L143" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="M143" s="47">
+      <c r="M143" s="1">
         <v>1817</v>
       </c>
-      <c r="N143" s="47">
+      <c r="N143" s="1">
         <v>3014</v>
       </c>
       <c r="O143" s="25">
         <v>2</v>
       </c>
-      <c r="P143" s="72"/>
-      <c r="Q143" s="73"/>
-      <c r="R143" s="74"/>
+      <c r="P143" s="49"/>
+      <c r="R143" s="50"/>
     </row>
     <row r="144" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J144" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="K144" s="47">
+        <v>280</v>
+      </c>
+      <c r="K144" s="1">
         <v>3</v>
       </c>
-      <c r="L144" s="62" t="s">
+      <c r="L144" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="M144" s="47"/>
-      <c r="N144" s="47"/>
       <c r="O144" s="25">
         <v>2</v>
       </c>
-      <c r="P144" s="72"/>
-      <c r="Q144" s="73"/>
-      <c r="R144" s="74"/>
+      <c r="P144" s="49"/>
+      <c r="R144" s="50"/>
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J145" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="K145" s="47"/>
+        <v>276</v>
+      </c>
+      <c r="K145" s="1"/>
       <c r="L145" s="16" t="s">
         <v>110</v>
       </c>
       <c r="M145" s="9">
         <v>1826</v>
       </c>
-      <c r="N145" s="47">
+      <c r="N145" s="1">
         <v>3018</v>
       </c>
       <c r="O145" s="25">
         <v>2</v>
       </c>
-      <c r="P145" s="66"/>
-      <c r="Q145" s="67"/>
-      <c r="R145" s="67"/>
+      <c r="P145" s="43"/>
+      <c r="Q145" s="44"/>
+      <c r="R145" s="44"/>
     </row>
     <row r="146" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J146" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="K146" s="47"/>
+        <v>302</v>
+      </c>
+      <c r="K146" s="1"/>
       <c r="L146" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="M146" s="75">
+      <c r="M146" s="51">
         <v>1823</v>
       </c>
       <c r="N146" s="15">
@@ -4186,7 +4188,7 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B147" s="11" t="s">
         <v>28</v>
@@ -4200,15 +4202,15 @@
       <c r="O147" s="11">
         <v>-1</v>
       </c>
-      <c r="P147" s="29" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q147" s="30"/>
-      <c r="R147" s="31"/>
+      <c r="P147" s="55" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q147" s="56"/>
+      <c r="R147" s="57"/>
     </row>
     <row r="148" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B148" s="13" t="s">
         <v>27</v>
@@ -4216,13 +4218,13 @@
       <c r="M148" s="12"/>
       <c r="N148" s="15"/>
       <c r="O148" s="13"/>
-      <c r="P148" s="35"/>
-      <c r="Q148" s="36"/>
-      <c r="R148" s="37"/>
+      <c r="P148" s="58"/>
+      <c r="Q148" s="59"/>
+      <c r="R148" s="60"/>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C149" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J149" s="9" t="s">
         <v>91</v>
@@ -4310,20 +4312,20 @@
     </row>
     <row r="155" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J155" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M155" s="12"/>
       <c r="N155" s="15"/>
       <c r="O155" s="13"/>
     </row>
     <row r="156" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="47" t="s">
-        <v>286</v>
+      <c r="A156" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="B156" s="2">
         <v>1</v>
       </c>
-      <c r="J156" s="51" t="s">
+      <c r="J156" s="29" t="s">
         <v>11</v>
       </c>
       <c r="M156" s="1">
@@ -4337,13 +4339,13 @@
       </c>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A157" s="47" t="s">
-        <v>286</v>
+      <c r="A157" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="B157" s="2">
         <v>2</v>
       </c>
-      <c r="J157" s="51" t="s">
+      <c r="J157" s="29" t="s">
         <v>17</v>
       </c>
       <c r="M157" s="10">
@@ -4355,15 +4357,15 @@
       <c r="O157" s="11"/>
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J158" s="51" t="s">
+      <c r="J158" s="29" t="s">
         <v>87</v>
       </c>
       <c r="M158" s="16"/>
       <c r="O158" s="25"/>
     </row>
     <row r="159" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J159" s="51" t="s">
-        <v>268</v>
+      <c r="J159" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="K159" s="2">
         <v>2</v>
@@ -4373,13 +4375,13 @@
       <c r="O159" s="13"/>
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A160" s="47" t="s">
-        <v>286</v>
+      <c r="A160" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="J160" s="51" t="s">
+        <v>290</v>
+      </c>
+      <c r="J160" s="29" t="s">
         <v>25</v>
       </c>
       <c r="K160" s="2">
@@ -4425,7 +4427,7 @@
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H163" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I163" s="2">
         <v>1</v>
@@ -4507,13 +4509,13 @@
         <v>116</v>
       </c>
       <c r="L168" s="9"/>
-      <c r="M168" s="48">
+      <c r="M168" s="26">
         <v>800</v>
       </c>
       <c r="N168" s="14">
         <v>3514</v>
       </c>
-      <c r="O168" s="49"/>
+      <c r="O168" s="27"/>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J169" s="9" t="s">
@@ -4545,7 +4547,7 @@
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J171" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M171" s="1">
         <v>950</v>
@@ -4623,7 +4625,7 @@
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J177" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M177" s="10">
         <v>535</v>
@@ -4662,7 +4664,7 @@
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>27</v>
@@ -4782,21 +4784,21 @@
       </c>
     </row>
     <row r="189" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K189" s="47"/>
-      <c r="L189" s="63">
+      <c r="K189" s="1"/>
+      <c r="L189" s="40">
         <v>6</v>
       </c>
-      <c r="M189" s="64">
+      <c r="M189" s="41">
         <v>1537</v>
       </c>
-      <c r="N189" s="64">
+      <c r="N189" s="41">
         <v>3836</v>
       </c>
-      <c r="O189" s="65"/>
+      <c r="O189" s="42"/>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A190" s="47" t="s">
-        <v>286</v>
+      <c r="A190" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="B190" s="2">
         <v>3</v>
@@ -4809,11 +4811,11 @@
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A191" s="47" t="s">
-        <v>286</v>
+      <c r="A191" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M191" s="1">
         <v>1516</v>
@@ -4824,7 +4826,7 @@
     </row>
     <row r="192" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M192" s="1">
         <v>1418</v>
@@ -4834,20 +4836,20 @@
       </c>
     </row>
     <row r="193" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L193" s="63">
+      <c r="L193" s="40">
         <v>6</v>
       </c>
-      <c r="M193" s="64">
+      <c r="M193" s="41">
         <v>1382</v>
       </c>
-      <c r="N193" s="64">
+      <c r="N193" s="41">
         <v>3898</v>
       </c>
-      <c r="O193" s="65"/>
+      <c r="O193" s="42"/>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L194" s="2"/>
       <c r="M194" s="1">
@@ -4856,11 +4858,11 @@
       <c r="N194" s="1">
         <v>3888</v>
       </c>
-      <c r="O194" s="47"/>
+      <c r="O194" s="1"/>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M195" s="1">
         <v>1577</v>
@@ -4871,7 +4873,7 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M196" s="1">
         <v>1561</v>
@@ -4882,7 +4884,7 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M197" s="1">
         <v>1409</v>
@@ -4949,18 +4951,18 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F202" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G202" s="2">
         <v>1</v>
       </c>
       <c r="J202" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="K202" s="47">
+        <v>304</v>
+      </c>
+      <c r="K202" s="1">
         <v>2</v>
       </c>
-      <c r="L202" s="60" t="s">
+      <c r="L202" s="37" t="s">
         <v>110</v>
       </c>
       <c r="M202" s="14">
@@ -4973,53 +4975,51 @@
     </row>
     <row r="203" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J203" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="K203" s="47"/>
-      <c r="L203" s="62" t="s">
+        <v>303</v>
+      </c>
+      <c r="K203" s="1"/>
+      <c r="L203" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="M203" s="47"/>
-      <c r="N203" s="47"/>
       <c r="O203" s="25"/>
     </row>
     <row r="204" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K204" s="47"/>
-      <c r="L204" s="48"/>
-      <c r="M204" s="48">
+      <c r="K204" s="1"/>
+      <c r="L204" s="26"/>
+      <c r="M204" s="26">
         <v>1584</v>
       </c>
       <c r="N204" s="14">
         <v>4274</v>
       </c>
-      <c r="O204" s="49"/>
+      <c r="O204" s="27"/>
     </row>
     <row r="205" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="47" t="s">
-        <v>286</v>
+      <c r="A205" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="B205" s="2">
         <v>4</v>
       </c>
       <c r="M205" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="N205" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="O205" s="1"/>
+      <c r="P205" s="52" t="s">
         <v>306</v>
       </c>
-      <c r="N205" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="O205" s="47"/>
-      <c r="P205" s="76" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q205" s="77"/>
-      <c r="R205" s="78"/>
+      <c r="Q205" s="53"/>
+      <c r="R205" s="54"/>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A206" s="47" t="s">
-        <v>286</v>
+      <c r="A206" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="B206" s="2">
         <v>5</v>
@@ -5033,7 +5033,7 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>27</v>
@@ -5067,7 +5067,7 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D209" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E209" s="2">
         <v>1</v>
@@ -5083,8 +5083,8 @@
       </c>
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A210" s="47" t="s">
-        <v>286</v>
+      <c r="A210" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="B210" s="2">
         <v>6</v>
@@ -5118,7 +5118,7 @@
     </row>
     <row r="212" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M212" s="1">
         <v>1520</v>
@@ -5129,10 +5129,11 @@
       <c r="O212" s="2">
         <v>-1</v>
       </c>
+      <c r="P212" s="79"/>
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B213" s="11" t="s">
         <v>28</v>
@@ -5147,75 +5148,74 @@
       <c r="O213" s="11">
         <v>-1</v>
       </c>
-      <c r="P213" s="66" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q213" s="67"/>
-      <c r="R213" s="68"/>
-    </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A214" s="16" t="s">
-        <v>315</v>
+      <c r="P213" s="55" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q213" s="56"/>
+      <c r="R213" s="57"/>
+    </row>
+    <row r="214" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="B214" s="25" t="s">
         <v>27</v>
       </c>
       <c r="L214" s="9"/>
       <c r="M214" s="16"/>
-      <c r="N214" s="47"/>
+      <c r="N214" s="77"/>
       <c r="O214" s="25"/>
-      <c r="P214" s="72"/>
-      <c r="Q214" s="73"/>
-      <c r="R214" s="74"/>
+      <c r="P214" s="58"/>
+      <c r="Q214" s="59"/>
+      <c r="R214" s="60"/>
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="16" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B215" s="25" t="s">
         <v>27</v>
       </c>
       <c r="L215" s="9"/>
       <c r="M215" s="16"/>
-      <c r="N215" s="47"/>
       <c r="O215" s="25"/>
-      <c r="P215" s="72"/>
-      <c r="Q215" s="73"/>
-      <c r="R215" s="74"/>
+      <c r="P215" s="43" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q215" s="44"/>
+      <c r="R215" s="45"/>
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B216" s="25" t="s">
         <v>27</v>
       </c>
       <c r="L216" s="9"/>
       <c r="M216" s="16"/>
-      <c r="N216" s="47"/>
       <c r="O216" s="25"/>
-      <c r="P216" s="72"/>
-      <c r="Q216" s="73"/>
-      <c r="R216" s="74"/>
+      <c r="P216" s="49"/>
+      <c r="Q216" s="78"/>
+      <c r="R216" s="50"/>
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B217" s="25" t="s">
         <v>27</v>
       </c>
       <c r="L217" s="9"/>
       <c r="M217" s="16"/>
-      <c r="N217" s="47"/>
       <c r="O217" s="25"/>
-      <c r="P217" s="72"/>
-      <c r="Q217" s="73"/>
-      <c r="R217" s="74"/>
+      <c r="P217" s="49"/>
+      <c r="Q217" s="78"/>
+      <c r="R217" s="50"/>
     </row>
     <row r="218" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B218" s="13" t="s">
         <v>27</v>
@@ -5224,9 +5224,9 @@
       <c r="M218" s="12"/>
       <c r="N218" s="15"/>
       <c r="O218" s="13"/>
-      <c r="P218" s="69"/>
-      <c r="Q218" s="70"/>
-      <c r="R218" s="71"/>
+      <c r="P218" s="46"/>
+      <c r="Q218" s="47"/>
+      <c r="R218" s="48"/>
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
@@ -5258,7 +5258,7 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B221" s="11" t="s">
         <v>28</v>
@@ -5270,15 +5270,15 @@
         <v>2853</v>
       </c>
       <c r="O221" s="11"/>
-      <c r="P221" s="29" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q221" s="30"/>
-      <c r="R221" s="31"/>
+      <c r="P221" s="55" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q221" s="56"/>
+      <c r="R221" s="57"/>
     </row>
     <row r="222" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B222" s="13" t="s">
         <v>27</v>
@@ -5286,13 +5286,13 @@
       <c r="M222" s="12"/>
       <c r="N222" s="15"/>
       <c r="O222" s="13"/>
-      <c r="P222" s="35"/>
-      <c r="Q222" s="36"/>
-      <c r="R222" s="37"/>
+      <c r="P222" s="58"/>
+      <c r="Q222" s="59"/>
+      <c r="R222" s="60"/>
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B223" s="2">
         <v>1</v>
@@ -5306,7 +5306,7 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>28</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="225" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M225" s="1">
         <v>3294</v>
@@ -5331,7 +5331,7 @@
     </row>
     <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J226" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K226" s="2">
         <v>10</v>
@@ -5356,7 +5356,7 @@
     </row>
     <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M228" s="1">
         <v>3324</v>
@@ -5367,7 +5367,7 @@
     </row>
     <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C229" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M229" s="1">
         <v>3181</v>
@@ -5376,8 +5376,31 @@
         <v>3040</v>
       </c>
     </row>
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B230" s="2">
+        <v>1</v>
+      </c>
+      <c r="M230" s="1">
+        <v>1506</v>
+      </c>
+      <c r="N230" s="1">
+        <v>3842</v>
+      </c>
+      <c r="O230" s="2">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="P147:R148"/>
     <mergeCell ref="P221:R222"/>
     <mergeCell ref="P57:R58"/>
@@ -5387,12 +5410,7 @@
     <mergeCell ref="P3:R15"/>
     <mergeCell ref="P24:R25"/>
     <mergeCell ref="P41:R42"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="P213:R214"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5433,50 +5451,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+    <row r="2" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="57" t="s">
+      <c r="M2" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="57" t="s">
+      <c r="N2" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="57" t="s">
+      <c r="O2" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="57" t="s">
+      <c r="P2" s="35" t="s">
         <v>74</v>
       </c>
     </row>
@@ -5485,25 +5503,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -5511,13 +5529,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -5525,22 +5543,22 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -5575,50 +5593,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57" t="s">
+    <row r="10" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="57" t="s">
+      <c r="H10" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="57" t="s">
+      <c r="I10" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="57" t="s">
+      <c r="J10" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="57" t="s">
+      <c r="K10" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="57" t="s">
+      <c r="L10" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="57" t="s">
+      <c r="M10" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="57" t="s">
+      <c r="N10" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="O10" s="57" t="s">
+      <c r="O10" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="P10" s="57" t="s">
+      <c r="P10" s="35" t="s">
         <v>75</v>
       </c>
     </row>
@@ -5627,16 +5645,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -5644,10 +5662,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -5655,25 +5673,25 @@
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -5704,17 +5722,17 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
-        <v>204</v>
-      </c>
-      <c r="B21" s="58" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="58" t="s">
-        <v>184</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>192</v>
+      <c r="A21" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5728,7 +5746,7 @@
         <v>0.05</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5742,7 +5760,7 @@
         <v>0.1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5756,7 +5774,7 @@
         <v>0.2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5770,7 +5788,7 @@
         <v>0.2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5784,7 +5802,7 @@
         <v>0.05</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5803,7 +5821,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5817,7 +5835,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5831,7 +5849,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5845,7 +5863,7 @@
         <v>0.2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5859,7 +5877,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5873,7 +5891,7 @@
         <v>0.2</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5887,7 +5905,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5911,7 +5929,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5930,7 +5948,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -5944,7 +5962,7 @@
         <v>0.5</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -5973,7 +5991,7 @@
         <v>0.2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -5987,7 +6005,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6001,7 +6019,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -6020,7 +6038,7 @@
         <v>0.2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6034,7 +6052,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6048,7 +6066,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6062,7 +6080,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6076,7 +6094,7 @@
         <v>0.2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6090,7 +6108,7 @@
         <v>0.2</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6104,7 +6122,7 @@
         <v>1</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6118,7 +6136,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -6133,7 +6151,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B58" s="1">
         <v>5</v>
@@ -6142,26 +6160,26 @@
         <v>0.05</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="B61" s="58" t="s">
-        <v>177</v>
-      </c>
-      <c r="C61" s="58" t="s">
-        <v>184</v>
-      </c>
-      <c r="D61" s="58" t="s">
-        <v>192</v>
+      <c r="A61" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="D61" s="36" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B62" s="1">
         <v>100</v>
@@ -6170,7 +6188,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6184,12 +6202,12 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B64" s="1">
         <v>100</v>
@@ -6198,12 +6216,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B65" s="1">
         <v>100</v>
@@ -6212,12 +6230,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B66" s="1">
         <v>100</v>
@@ -6226,12 +6244,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B67" s="1">
         <v>100</v>
@@ -6240,17 +6258,17 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B69" s="1">
         <v>25</v>
@@ -6259,12 +6277,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B70" s="1">
         <v>25</v>
@@ -6273,12 +6291,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B71" s="1">
         <v>25</v>
@@ -6287,12 +6305,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B72" s="1">
         <v>25</v>
@@ -6301,12 +6319,12 @@
         <v>1.6E-2</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B73" s="1">
         <v>25</v>
@@ -6315,12 +6333,12 @@
         <v>1.6E-2</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B74" s="1">
         <v>25</v>
@@ -6329,12 +6347,12 @@
         <v>1.6E-2</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B75" s="1">
         <v>75</v>
@@ -6343,12 +6361,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B76" s="1">
         <v>75</v>
@@ -6357,12 +6375,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B77" s="1">
         <v>125</v>
@@ -6371,17 +6389,17 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B79" s="1">
         <v>75</v>
@@ -6390,12 +6408,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B80" s="1">
         <v>75</v>
@@ -6404,12 +6422,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B81" s="1">
         <v>20</v>
@@ -6418,12 +6436,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B82" s="1">
         <v>10</v>
@@ -6432,12 +6450,12 @@
         <v>0.1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B83" s="1">
         <v>4</v>
@@ -6446,12 +6464,12 @@
         <v>0.22</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B84" s="1">
         <v>500</v>
@@ -6460,12 +6478,12 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B85" s="1">
         <v>4</v>
@@ -6474,7 +6492,7 @@
         <v>0.25</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -6489,7 +6507,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B88" s="1">
         <v>4</v>
@@ -6498,22 +6516,22 @@
         <v>0.25</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B91" s="1">
         <v>4</v>
@@ -6522,12 +6540,12 @@
         <v>0.25</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B92" s="1">
         <v>4</v>
@@ -6536,12 +6554,12 @@
         <v>0.25</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B93" s="1">
         <v>4</v>
@@ -6550,247 +6568,247 @@
         <v>0.25</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="59" t="s">
+      <c r="A96" s="76" t="s">
+        <v>238</v>
+      </c>
+      <c r="B96" s="76" t="s">
+        <v>191</v>
+      </c>
+      <c r="C96" s="76"/>
+      <c r="D96" s="76"/>
+      <c r="E96" s="76"/>
+      <c r="F96" s="76"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="76"/>
+      <c r="B97" s="76"/>
+      <c r="C97" s="76"/>
+      <c r="D97" s="76"/>
+      <c r="E97" s="76"/>
+      <c r="F97" s="76"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="76"/>
+      <c r="B98" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B96" s="59" t="s">
-        <v>192</v>
-      </c>
-      <c r="C96" s="59"/>
-      <c r="D96" s="59"/>
-      <c r="E96" s="59"/>
-      <c r="F96" s="59"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="59"/>
-      <c r="B97" s="59"/>
-      <c r="C97" s="59"/>
-      <c r="D97" s="59"/>
-      <c r="E97" s="59"/>
-      <c r="F97" s="59"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="59"/>
-      <c r="B98" s="1" t="s">
+      <c r="C98" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="F98" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -6816,7 +6834,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6824,7 +6842,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6874,7 +6892,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -6882,7 +6900,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -6963,10 +6981,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="50">
+      <c r="B1" s="28">
         <v>1</v>
       </c>
     </row>
@@ -7019,22 +7037,22 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -7086,29 +7104,29 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="50">
+      <c r="B14" s="28">
         <v>2</v>
       </c>
     </row>
@@ -7161,22 +7179,22 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -7228,29 +7246,29 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="50" t="s">
+      <c r="A27" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="50">
+      <c r="B27" s="28">
         <v>3</v>
       </c>
     </row>
@@ -7303,22 +7321,22 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -7370,29 +7388,29 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="50">
+      <c r="B40" s="28">
         <v>4</v>
       </c>
     </row>
@@ -7445,22 +7463,22 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -7512,29 +7530,29 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A53" s="50" t="s">
+      <c r="A53" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="50">
+      <c r="B53" s="28">
         <v>5</v>
       </c>
     </row>
@@ -7587,22 +7605,22 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -7654,29 +7672,29 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A66" s="50" t="s">
+      <c r="A66" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B66" s="50">
+      <c r="B66" s="28">
         <v>6</v>
       </c>
     </row>
@@ -7705,29 +7723,29 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A74" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="B74" s="50"/>
+      <c r="A74" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" s="28"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
@@ -7775,40 +7793,40 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
+        <v>170</v>
+      </c>
+      <c r="C76" t="s">
+        <v>167</v>
+      </c>
+      <c r="D76" s="31">
+        <v>0.32</v>
+      </c>
+      <c r="E76" t="s">
+        <v>154</v>
+      </c>
+      <c r="G76" t="s">
+        <v>154</v>
+      </c>
+      <c r="H76" t="s">
+        <v>157</v>
+      </c>
+      <c r="I76" t="s">
+        <v>157</v>
+      </c>
+      <c r="J76" t="s">
+        <v>155</v>
+      </c>
+      <c r="K76" t="s">
+        <v>155</v>
+      </c>
+      <c r="L76" t="s">
+        <v>155</v>
+      </c>
+      <c r="M76" t="s">
         <v>171</v>
       </c>
-      <c r="C76" t="s">
-        <v>168</v>
-      </c>
-      <c r="D76" s="53">
-        <v>0.32</v>
-      </c>
-      <c r="E76" t="s">
-        <v>155</v>
-      </c>
-      <c r="G76" t="s">
-        <v>155</v>
-      </c>
-      <c r="H76" t="s">
-        <v>158</v>
-      </c>
-      <c r="I76" t="s">
-        <v>158</v>
-      </c>
-      <c r="J76" t="s">
-        <v>156</v>
-      </c>
-      <c r="K76" t="s">
-        <v>156</v>
-      </c>
-      <c r="L76" t="s">
-        <v>156</v>
-      </c>
-      <c r="M76" t="s">
-        <v>172</v>
-      </c>
       <c r="O76" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -7853,242 +7871,242 @@
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="53">
+      <c r="B79" s="31">
         <v>0.32</v>
       </c>
-      <c r="C79" s="56" t="s">
-        <v>153</v>
+      <c r="C79" s="34" t="s">
+        <v>152</v>
       </c>
       <c r="E79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I79" t="s">
+        <v>165</v>
+      </c>
+      <c r="J79" t="s">
+        <v>165</v>
+      </c>
+      <c r="K79" t="s">
         <v>166</v>
       </c>
-      <c r="J79" t="s">
-        <v>166</v>
-      </c>
-      <c r="K79" t="s">
-        <v>167</v>
-      </c>
       <c r="L79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M79" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="33">
+        <v>0.32</v>
+      </c>
+      <c r="B82" t="s">
+        <v>136</v>
+      </c>
+      <c r="C82" t="s">
+        <v>130</v>
+      </c>
+      <c r="D82" t="s">
+        <v>131</v>
+      </c>
+      <c r="E82" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="55">
-        <v>0.32</v>
-      </c>
-      <c r="B82" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B83" t="s">
+        <v>136</v>
+      </c>
+      <c r="C83" t="s">
+        <v>135</v>
+      </c>
+      <c r="D83" t="s">
+        <v>140</v>
+      </c>
+      <c r="E83" t="s">
         <v>137</v>
       </c>
-      <c r="C82" t="s">
-        <v>131</v>
-      </c>
-      <c r="D82" t="s">
-        <v>132</v>
-      </c>
-      <c r="E82" t="s">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="B84" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" t="s">
+        <v>135</v>
+      </c>
+      <c r="D84" t="s">
+        <v>156</v>
+      </c>
+      <c r="E84" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B85" t="s">
+        <v>136</v>
+      </c>
+      <c r="C85" t="s">
+        <v>151</v>
+      </c>
+      <c r="D85" t="s">
+        <v>139</v>
+      </c>
+      <c r="E85" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="33">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="B86" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" t="s">
+        <v>151</v>
+      </c>
+      <c r="D86" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="B83" t="s">
+      <c r="E86" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B87" t="s">
+        <v>158</v>
+      </c>
+      <c r="C87" t="s">
+        <v>159</v>
+      </c>
+      <c r="D87" t="s">
+        <v>160</v>
+      </c>
+      <c r="E87" t="s">
+        <v>161</v>
+      </c>
+      <c r="F87" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B88" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" t="s">
+        <v>135</v>
+      </c>
+      <c r="D88" t="s">
+        <v>164</v>
+      </c>
+      <c r="E88" t="s">
         <v>137</v>
       </c>
-      <c r="C83" t="s">
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="B89" t="s">
         <v>136</v>
       </c>
-      <c r="D83" t="s">
-        <v>141</v>
-      </c>
-      <c r="E83" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="54" t="s">
+      <c r="C89" t="s">
+        <v>135</v>
+      </c>
+      <c r="D89" t="s">
         <v>156</v>
       </c>
-      <c r="B84" t="s">
-        <v>137</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="E89" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B90" t="s">
         <v>136</v>
       </c>
-      <c r="D84" t="s">
-        <v>157</v>
-      </c>
-      <c r="E84" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="55" t="s">
+      <c r="C90" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B91" t="s">
+        <v>169</v>
+      </c>
+      <c r="C91" t="s">
         <v>153</v>
       </c>
-      <c r="B85" t="s">
-        <v>137</v>
-      </c>
-      <c r="C85" t="s">
-        <v>152</v>
-      </c>
-      <c r="D85" t="s">
-        <v>140</v>
-      </c>
-      <c r="E85" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="55">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="B86" t="s">
-        <v>137</v>
-      </c>
-      <c r="C86" t="s">
-        <v>152</v>
-      </c>
-      <c r="D86" t="s">
-        <v>141</v>
-      </c>
-      <c r="E86" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="55" t="s">
-        <v>158</v>
-      </c>
-      <c r="B87" t="s">
-        <v>159</v>
-      </c>
-      <c r="C87" t="s">
-        <v>160</v>
-      </c>
-      <c r="D87" t="s">
-        <v>161</v>
-      </c>
-      <c r="E87" t="s">
-        <v>162</v>
-      </c>
-      <c r="F87" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="55" t="s">
-        <v>164</v>
-      </c>
-      <c r="B88" t="s">
-        <v>137</v>
-      </c>
-      <c r="C88" t="s">
-        <v>136</v>
-      </c>
-      <c r="D88" t="s">
-        <v>165</v>
-      </c>
-      <c r="E88" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="55" t="s">
-        <v>166</v>
-      </c>
-      <c r="B89" t="s">
-        <v>137</v>
-      </c>
-      <c r="C89" t="s">
-        <v>136</v>
-      </c>
-      <c r="D89" t="s">
-        <v>157</v>
-      </c>
-      <c r="E89" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="55" t="s">
-        <v>167</v>
-      </c>
-      <c r="B90" t="s">
-        <v>137</v>
-      </c>
-      <c r="C90" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="55" t="s">
+      <c r="D91" t="s">
         <v>168</v>
       </c>
-      <c r="B91" t="s">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="C91" t="s">
-        <v>154</v>
-      </c>
-      <c r="D91" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="55" t="s">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="33" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="55" t="s">
+      <c r="B93" t="s">
         <v>172</v>
       </c>
-      <c r="B93" t="s">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="33">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="33" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="55">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="55" t="s">
+      <c r="B96" t="s">
+        <v>172</v>
+      </c>
+      <c r="C96" t="s">
+        <v>175</v>
+      </c>
+      <c r="D96" t="s">
         <v>174</v>
-      </c>
-      <c r="B96" t="s">
-        <v>173</v>
-      </c>
-      <c r="C96" t="s">
-        <v>176</v>
-      </c>
-      <c r="D96" t="s">
-        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -8317,7 +8335,7 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
South Light house and West Cost
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3676C97-3A86-4EB9-9FF5-F09DE9B37320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7613314A-584B-4FAD-9600-05F51779A737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="339">
   <si>
     <t>Mission</t>
   </si>
@@ -389,9 +389,6 @@
     <t>Shooting Practice</t>
   </si>
   <si>
-    <t>Becon</t>
-  </si>
-  <si>
     <t>Älgstudsare Hunting Rifle</t>
   </si>
   <si>
@@ -863,9 +860,6 @@
     <t>Mauser Hunting Rifle (Lock)</t>
   </si>
   <si>
-    <t>Fireworks</t>
-  </si>
-  <si>
     <t>4_8x_Rifle_Scope</t>
   </si>
   <si>
@@ -878,9 +872,6 @@
     <t>Seeker Prototype</t>
   </si>
   <si>
-    <t>Fireworks (Lock)</t>
-  </si>
-  <si>
     <t>Emergency Flare (Lock)</t>
   </si>
   <si>
@@ -1023,6 +1014,48 @@
   </si>
   <si>
     <t>The Home Team =&gt; Calling For Help</t>
+  </si>
+  <si>
+    <t>Standard 1st Aid Kit (Lock)</t>
+  </si>
+  <si>
+    <t>Firework (Lock)</t>
+  </si>
+  <si>
+    <t>Radio (Lock)</t>
+  </si>
+  <si>
+    <t>Scope (Bugged)</t>
+  </si>
+  <si>
+    <t>0.44 FMJ</t>
+  </si>
+  <si>
+    <t>32 Wood | 16 Adhesive | 8 Lead</t>
+  </si>
+  <si>
+    <t>Beacon</t>
+  </si>
+  <si>
+    <t>Klaucke 17 (Lock)</t>
+  </si>
+  <si>
+    <t>1-4x Rifle Scope (Lock)</t>
+  </si>
+  <si>
+    <t>HP5 (Lock)</t>
+  </si>
+  <si>
+    <t>Vantage 8x42 Binoculars (Lock)</t>
+  </si>
+  <si>
+    <t>Stealthy Shirt</t>
+  </si>
+  <si>
+    <t>2x Red Dot Scope</t>
+  </si>
+  <si>
+    <t>Electrolyte 4 | Rubber 8 | Lead 2</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1107,6 +1140,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1408,7 +1447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1611,6 +1650,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -1926,11 +1968,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R230"/>
+  <dimension ref="A1:R268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M231" sqref="M231"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J267" sqref="J267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,9 +1984,9 @@
     <col min="5" max="5" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="2"/>
-    <col min="10" max="10" width="24.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.140625" style="1" bestFit="1" customWidth="1"/>
@@ -3037,7 +3079,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>116</v>
+        <v>331</v>
       </c>
       <c r="M67" s="1">
         <v>2113</v>
@@ -3048,7 +3090,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F68" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G68" s="2">
         <v>1</v>
@@ -3062,7 +3104,7 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H69" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I69" s="2">
         <v>1</v>
@@ -3158,14 +3200,14 @@
         <v>-1</v>
       </c>
       <c r="P74" s="55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q74" s="56"/>
       <c r="R74" s="57"/>
     </row>
     <row r="75" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>27</v>
@@ -3207,7 +3249,7 @@
     </row>
     <row r="78" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E78" s="2">
         <v>1</v>
@@ -3256,7 +3298,7 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B81" s="2">
         <v>1</v>
@@ -3274,7 +3316,7 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B82" s="2">
         <v>2</v>
@@ -3382,7 +3424,7 @@
         <v>28</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I90" s="2">
         <v>1</v>
@@ -3481,7 +3523,7 @@
     </row>
     <row r="97" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J97" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K97" s="2">
         <v>2</v>
@@ -3493,7 +3535,7 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J98" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K98" s="2">
         <v>3</v>
@@ -3507,7 +3549,7 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J99" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K99" s="2">
         <v>2</v>
@@ -3549,7 +3591,7 @@
     </row>
     <row r="102" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>27</v>
@@ -3636,14 +3678,14 @@
         <v>2</v>
       </c>
       <c r="P108" s="43" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="Q108" s="44"/>
       <c r="R108" s="45"/>
     </row>
     <row r="109" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F109" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G109" s="2">
         <v>2</v>
@@ -3662,7 +3704,7 @@
         <v>2</v>
       </c>
       <c r="P109" s="46" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="Q109" s="47"/>
       <c r="R109" s="48"/>
@@ -3708,7 +3750,7 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J113" s="9" t="s">
-        <v>274</v>
+        <v>79</v>
       </c>
       <c r="K113" s="2">
         <v>4</v>
@@ -3787,7 +3829,7 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>40</v>
@@ -3840,7 +3882,7 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>41</v>
@@ -3878,14 +3920,14 @@
       </c>
       <c r="O125" s="11"/>
       <c r="P125" s="43" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="Q125" s="44"/>
       <c r="R125" s="45"/>
     </row>
     <row r="126" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J126" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K126" s="2">
         <v>3</v>
@@ -3906,10 +3948,10 @@
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M127" s="10">
         <v>1809</v>
@@ -3929,10 +3971,10 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M129" s="1">
         <v>1805</v>
@@ -3983,7 +4025,7 @@
     </row>
     <row r="133" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J133" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K133" s="2">
         <v>3</v>
@@ -3994,10 +4036,10 @@
     </row>
     <row r="134" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="M134" s="1">
         <v>1713</v>
@@ -4045,7 +4087,7 @@
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J138" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K138" s="2">
         <v>3</v>
@@ -4073,7 +4115,7 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C140" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M140" s="1">
         <v>1302</v>
@@ -4084,7 +4126,7 @@
     </row>
     <row r="141" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>116</v>
+        <v>331</v>
       </c>
       <c r="M141" s="1">
         <v>1464</v>
@@ -4106,14 +4148,14 @@
       </c>
       <c r="O142" s="11"/>
       <c r="P142" s="43" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="Q142" s="44"/>
       <c r="R142" s="45"/>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J143" s="9" t="s">
-        <v>279</v>
+        <v>326</v>
       </c>
       <c r="K143" s="1">
         <v>8</v>
@@ -4135,7 +4177,7 @@
     </row>
     <row r="144" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J144" s="9" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="K144" s="1">
         <v>3</v>
@@ -4151,7 +4193,7 @@
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J145" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K145" s="1"/>
       <c r="L145" s="16" t="s">
@@ -4172,7 +4214,7 @@
     </row>
     <row r="146" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J146" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="K146" s="1"/>
       <c r="L146" s="12" t="s">
@@ -4188,7 +4230,7 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B147" s="11" t="s">
         <v>28</v>
@@ -4203,14 +4245,14 @@
         <v>-1</v>
       </c>
       <c r="P147" s="55" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="Q147" s="56"/>
       <c r="R147" s="57"/>
     </row>
     <row r="148" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B148" s="13" t="s">
         <v>27</v>
@@ -4224,7 +4266,7 @@
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C149" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J149" s="9" t="s">
         <v>91</v>
@@ -4312,7 +4354,7 @@
     </row>
     <row r="155" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J155" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M155" s="12"/>
       <c r="N155" s="15"/>
@@ -4320,7 +4362,7 @@
     </row>
     <row r="156" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B156" s="2">
         <v>1</v>
@@ -4340,7 +4382,7 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B157" s="2">
         <v>2</v>
@@ -4365,7 +4407,7 @@
     </row>
     <row r="159" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J159" s="29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K159" s="2">
         <v>2</v>
@@ -4376,10 +4418,10 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J160" s="29" t="s">
         <v>25</v>
@@ -4427,7 +4469,7 @@
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H163" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I163" s="2">
         <v>1</v>
@@ -4506,7 +4548,7 @@
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>116</v>
+        <v>331</v>
       </c>
       <c r="L168" s="9"/>
       <c r="M168" s="26">
@@ -4547,7 +4589,7 @@
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J171" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M171" s="1">
         <v>950</v>
@@ -4625,7 +4667,7 @@
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J177" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M177" s="10">
         <v>535</v>
@@ -4664,7 +4706,7 @@
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>27</v>
@@ -4771,7 +4813,7 @@
     </row>
     <row r="188" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F188" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G188" s="2">
         <v>1</v>
@@ -4798,7 +4840,7 @@
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B190" s="2">
         <v>3</v>
@@ -4812,10 +4854,10 @@
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="M191" s="1">
         <v>1516</v>
@@ -4826,7 +4868,7 @@
     </row>
     <row r="192" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="M192" s="1">
         <v>1418</v>
@@ -4849,7 +4891,7 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="L194" s="2"/>
       <c r="M194" s="1">
@@ -4862,7 +4904,7 @@
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M195" s="1">
         <v>1577</v>
@@ -4873,7 +4915,7 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M196" s="1">
         <v>1561</v>
@@ -4884,7 +4926,7 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M197" s="1">
         <v>1409</v>
@@ -4951,13 +4993,13 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F202" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G202" s="2">
         <v>1</v>
       </c>
-      <c r="J202" s="9" t="s">
-        <v>304</v>
+      <c r="J202" s="80" t="s">
+        <v>301</v>
       </c>
       <c r="K202" s="1">
         <v>2</v>
@@ -4975,7 +5017,7 @@
     </row>
     <row r="203" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J203" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="K203" s="1"/>
       <c r="L203" s="39" t="s">
@@ -4985,7 +5027,7 @@
     </row>
     <row r="204" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>116</v>
+        <v>331</v>
       </c>
       <c r="K204" s="1"/>
       <c r="L204" s="26"/>
@@ -4999,27 +5041,27 @@
     </row>
     <row r="205" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B205" s="2">
         <v>4</v>
       </c>
       <c r="M205" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="N205" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="O205" s="1"/>
       <c r="P205" s="52" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="Q205" s="53"/>
       <c r="R205" s="54"/>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B206" s="2">
         <v>5</v>
@@ -5033,7 +5075,7 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>27</v>
@@ -5067,7 +5109,7 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D209" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E209" s="2">
         <v>1</v>
@@ -5084,7 +5126,7 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B210" s="2">
         <v>6</v>
@@ -5118,7 +5160,7 @@
     </row>
     <row r="212" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="M212" s="1">
         <v>1520</v>
@@ -5133,7 +5175,7 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B213" s="11" t="s">
         <v>28</v>
@@ -5149,14 +5191,14 @@
         <v>-1</v>
       </c>
       <c r="P213" s="55" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Q213" s="56"/>
       <c r="R213" s="57"/>
     </row>
     <row r="214" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B214" s="25" t="s">
         <v>27</v>
@@ -5171,7 +5213,7 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="16" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B215" s="25" t="s">
         <v>27</v>
@@ -5180,14 +5222,14 @@
       <c r="M215" s="16"/>
       <c r="O215" s="25"/>
       <c r="P215" s="43" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="Q215" s="44"/>
       <c r="R215" s="45"/>
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="16" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B216" s="25" t="s">
         <v>27</v>
@@ -5201,7 +5243,7 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="16" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B217" s="25" t="s">
         <v>27</v>
@@ -5215,7 +5257,7 @@
     </row>
     <row r="218" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B218" s="13" t="s">
         <v>27</v>
@@ -5258,7 +5300,7 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="10" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B221" s="11" t="s">
         <v>28</v>
@@ -5271,14 +5313,14 @@
       </c>
       <c r="O221" s="11"/>
       <c r="P221" s="55" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Q221" s="56"/>
       <c r="R221" s="57"/>
     </row>
     <row r="222" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B222" s="13" t="s">
         <v>27</v>
@@ -5292,7 +5334,7 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B223" s="2">
         <v>1</v>
@@ -5306,7 +5348,7 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>28</v>
@@ -5320,7 +5362,7 @@
     </row>
     <row r="225" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="M225" s="1">
         <v>3294</v>
@@ -5331,7 +5373,7 @@
     </row>
     <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J226" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K226" s="2">
         <v>10</v>
@@ -5356,7 +5398,7 @@
     </row>
     <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="M228" s="1">
         <v>3324</v>
@@ -5367,7 +5409,7 @@
     </row>
     <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C229" s="19" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="M229" s="1">
         <v>3181</v>
@@ -5378,7 +5420,7 @@
     </row>
     <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B230" s="2">
         <v>1</v>
@@ -5391,6 +5433,579 @@
       </c>
       <c r="O230" s="2">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F231" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G231" s="2">
+        <v>1</v>
+      </c>
+      <c r="J231" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M231" s="1">
+        <v>1514</v>
+      </c>
+      <c r="N231" s="1">
+        <v>4344</v>
+      </c>
+      <c r="O231" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J232" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M232" s="1">
+        <v>1508</v>
+      </c>
+      <c r="N232" s="1">
+        <v>4345</v>
+      </c>
+      <c r="O232" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K233" s="77"/>
+      <c r="L233" s="37">
+        <v>5</v>
+      </c>
+      <c r="M233" s="14">
+        <v>1510</v>
+      </c>
+      <c r="N233" s="14">
+        <v>4351</v>
+      </c>
+      <c r="O233" s="11"/>
+    </row>
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J234" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="K234" s="77"/>
+      <c r="L234" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="M234" s="77">
+        <v>1510</v>
+      </c>
+      <c r="N234" s="77">
+        <v>4345</v>
+      </c>
+      <c r="O234" s="25"/>
+    </row>
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J235" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="K235" s="77"/>
+      <c r="L235" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="M235" s="77">
+        <v>1506</v>
+      </c>
+      <c r="N235" s="77">
+        <v>4346</v>
+      </c>
+      <c r="O235" s="25"/>
+    </row>
+    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J236" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="K236" s="77"/>
+      <c r="L236" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="M236" s="77">
+        <v>1513</v>
+      </c>
+      <c r="N236" s="77">
+        <v>4339</v>
+      </c>
+      <c r="O236" s="25"/>
+    </row>
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F237" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G237" s="2">
+        <v>2</v>
+      </c>
+      <c r="J237" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="K237" s="77"/>
+      <c r="L237" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="M237" s="77">
+        <v>1503</v>
+      </c>
+      <c r="N237" s="77">
+        <v>4343</v>
+      </c>
+      <c r="O237" s="25"/>
+    </row>
+    <row r="238" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J238" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="K238" s="77"/>
+      <c r="L238" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="M238" s="15">
+        <v>1500</v>
+      </c>
+      <c r="N238" s="15">
+        <v>4341</v>
+      </c>
+      <c r="O238" s="13"/>
+    </row>
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J239" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M239" s="1">
+        <v>1560</v>
+      </c>
+      <c r="N239" s="1">
+        <v>4374</v>
+      </c>
+    </row>
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J240" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="K240" s="2">
+        <v>2</v>
+      </c>
+      <c r="M240" s="1">
+        <v>1564</v>
+      </c>
+      <c r="N240" s="1">
+        <v>4374</v>
+      </c>
+    </row>
+    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H241" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="M241" s="1">
+        <v>1582</v>
+      </c>
+      <c r="N241" s="1">
+        <v>4395</v>
+      </c>
+    </row>
+    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="M242" s="1">
+        <v>1785</v>
+      </c>
+      <c r="N242" s="1">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="243" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F243" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G243" s="2">
+        <v>1</v>
+      </c>
+      <c r="M243" s="1">
+        <v>1720</v>
+      </c>
+      <c r="N243" s="1">
+        <v>4535</v>
+      </c>
+    </row>
+    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F244" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G244" s="2">
+        <v>1</v>
+      </c>
+      <c r="L244" s="9"/>
+      <c r="M244" s="10">
+        <v>1725</v>
+      </c>
+      <c r="N244" s="14">
+        <v>4539</v>
+      </c>
+      <c r="O244" s="11"/>
+    </row>
+    <row r="245" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F245" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G245" s="2">
+        <v>1</v>
+      </c>
+      <c r="L245" s="9"/>
+      <c r="M245" s="12"/>
+      <c r="N245" s="15"/>
+      <c r="O245" s="13"/>
+    </row>
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F246" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G246" s="2">
+        <v>1</v>
+      </c>
+      <c r="M246" s="10">
+        <v>1722</v>
+      </c>
+      <c r="N246" s="14">
+        <v>4534</v>
+      </c>
+      <c r="O246" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F247" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G247" s="2">
+        <v>1</v>
+      </c>
+      <c r="M247" s="16"/>
+      <c r="N247" s="77"/>
+      <c r="O247" s="25"/>
+    </row>
+    <row r="248" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J248" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="K248" s="1">
+        <v>3</v>
+      </c>
+      <c r="L248" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="M248" s="41">
+        <v>1722</v>
+      </c>
+      <c r="N248" s="41">
+        <v>4532</v>
+      </c>
+      <c r="O248" s="42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F249" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G249" s="2">
+        <v>2</v>
+      </c>
+      <c r="H249" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="I249" s="2">
+        <v>2</v>
+      </c>
+      <c r="K249" s="77"/>
+      <c r="L249" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="M249" s="14">
+        <v>1721</v>
+      </c>
+      <c r="N249" s="14">
+        <v>4532</v>
+      </c>
+      <c r="O249" s="42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J250" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="K250" s="77"/>
+      <c r="L250" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="M250" s="41">
+        <v>1721</v>
+      </c>
+      <c r="N250" s="41">
+        <v>4530</v>
+      </c>
+      <c r="O250" s="42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F251" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G251" s="2">
+        <v>1</v>
+      </c>
+      <c r="K251" s="77"/>
+      <c r="L251" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="M251" s="41">
+        <v>1722</v>
+      </c>
+      <c r="N251" s="41">
+        <v>4542</v>
+      </c>
+      <c r="O251" s="42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A252" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M252" s="1">
+        <v>1826</v>
+      </c>
+      <c r="N252" s="1">
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F253" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G253" s="2">
+        <v>2</v>
+      </c>
+      <c r="J253" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="K253" s="77"/>
+      <c r="L253" s="37">
+        <v>4</v>
+      </c>
+      <c r="M253" s="14">
+        <v>1823</v>
+      </c>
+      <c r="N253" s="14">
+        <v>4637</v>
+      </c>
+      <c r="O253" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J254" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="K254" s="77">
+        <v>3</v>
+      </c>
+      <c r="L254" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="M254" s="77"/>
+      <c r="N254" s="77"/>
+      <c r="O254" s="25"/>
+    </row>
+    <row r="255" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J255" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="K255" s="77"/>
+      <c r="L255" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="M255" s="15"/>
+      <c r="N255" s="15"/>
+      <c r="O255" s="13"/>
+    </row>
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D256" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E256" s="2">
+        <v>1</v>
+      </c>
+      <c r="M256" s="1">
+        <v>1915</v>
+      </c>
+      <c r="N256" s="1">
+        <v>4661</v>
+      </c>
+      <c r="O256" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F257" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G257" s="2">
+        <v>2</v>
+      </c>
+      <c r="M257" s="1">
+        <v>1912</v>
+      </c>
+      <c r="N257" s="1">
+        <v>4658</v>
+      </c>
+      <c r="O257" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J258" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M258" s="1">
+        <v>1334</v>
+      </c>
+      <c r="N258" s="1">
+        <v>4202</v>
+      </c>
+    </row>
+    <row r="259" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J259" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M259" s="1">
+        <v>1245</v>
+      </c>
+      <c r="N259" s="1">
+        <v>4092</v>
+      </c>
+    </row>
+    <row r="260" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="H260" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I260" s="2">
+        <v>1</v>
+      </c>
+      <c r="M260" s="1">
+        <v>1244</v>
+      </c>
+      <c r="N260" s="1">
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="261" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J261" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M261" s="1">
+        <v>1239</v>
+      </c>
+      <c r="N261" s="1">
+        <v>4045</v>
+      </c>
+    </row>
+    <row r="262" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J262" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="M262" s="1">
+        <v>1237</v>
+      </c>
+      <c r="N262" s="1">
+        <v>4051</v>
+      </c>
+      <c r="O262" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J263" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M263" s="1">
+        <v>1243</v>
+      </c>
+      <c r="N263" s="1">
+        <v>4045</v>
+      </c>
+      <c r="O263" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J264" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="M264" s="1">
+        <v>1240</v>
+      </c>
+      <c r="N264" s="1">
+        <v>4041</v>
+      </c>
+      <c r="O264" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J265" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K265" s="2">
+        <v>2</v>
+      </c>
+      <c r="M265" s="1">
+        <v>1240</v>
+      </c>
+      <c r="N265" s="1">
+        <v>4044</v>
+      </c>
+      <c r="O265" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J266" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="M266" s="1">
+        <v>1229</v>
+      </c>
+      <c r="N266" s="1">
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="267" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="J267" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="M267" s="1">
+        <v>1205</v>
+      </c>
+      <c r="N267" s="1">
+        <v>4036</v>
+      </c>
+    </row>
+    <row r="268" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F268" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G268" s="2">
+        <v>1</v>
+      </c>
+      <c r="M268" s="1">
+        <v>1197</v>
+      </c>
+      <c r="N268" s="1">
+        <v>4339</v>
       </c>
     </row>
   </sheetData>
@@ -5421,9 +6036,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
   <dimension ref="A1:P121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5503,25 +6118,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -5529,13 +6147,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -5543,22 +6170,22 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -5645,16 +6272,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -5662,10 +6289,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -5673,25 +6300,25 @@
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -5723,16 +6350,16 @@
     </row>
     <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5746,7 +6373,7 @@
         <v>0.05</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -5760,7 +6387,7 @@
         <v>0.1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -5774,7 +6401,7 @@
         <v>0.2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -5788,7 +6415,7 @@
         <v>0.2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -5802,7 +6429,7 @@
         <v>0.05</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5821,7 +6448,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5835,7 +6462,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5849,7 +6476,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5863,7 +6490,7 @@
         <v>0.2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -5877,7 +6504,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -5891,7 +6518,7 @@
         <v>0.2</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -5905,7 +6532,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5929,7 +6556,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5948,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -5962,7 +6589,7 @@
         <v>0.5</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -5991,7 +6618,7 @@
         <v>0.2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -6005,7 +6632,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6019,7 +6646,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -6038,7 +6665,7 @@
         <v>0.2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -6052,7 +6679,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -6066,7 +6693,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -6080,7 +6707,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -6094,7 +6721,7 @@
         <v>0.2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6108,7 +6735,7 @@
         <v>0.2</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -6122,7 +6749,7 @@
         <v>1</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -6136,7 +6763,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -6148,10 +6775,19 @@
       <c r="A57" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="B57" s="1">
+        <v>5</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B58" s="1">
         <v>5</v>
@@ -6160,26 +6796,26 @@
         <v>0.05</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A61" s="36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C61" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D61" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B62" s="1">
         <v>100</v>
@@ -6188,7 +6824,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6202,12 +6838,12 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B64" s="1">
         <v>100</v>
@@ -6216,12 +6852,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B65" s="1">
         <v>100</v>
@@ -6230,12 +6866,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B66" s="1">
         <v>100</v>
@@ -6244,12 +6880,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B67" s="1">
         <v>100</v>
@@ -6258,17 +6894,17 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B69" s="1">
         <v>25</v>
@@ -6277,12 +6913,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B70" s="1">
         <v>25</v>
@@ -6291,12 +6927,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B71" s="1">
         <v>25</v>
@@ -6305,12 +6941,12 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B72" s="1">
         <v>25</v>
@@ -6319,12 +6955,12 @@
         <v>1.6E-2</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B73" s="1">
         <v>25</v>
@@ -6333,12 +6969,12 @@
         <v>1.6E-2</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B74" s="1">
         <v>25</v>
@@ -6347,12 +6983,12 @@
         <v>1.6E-2</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B75" s="1">
         <v>75</v>
@@ -6361,12 +6997,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B76" s="1">
         <v>75</v>
@@ -6375,12 +7011,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B77" s="1">
         <v>125</v>
@@ -6389,17 +7025,17 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B79" s="1">
         <v>75</v>
@@ -6408,12 +7044,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B80" s="1">
         <v>75</v>
@@ -6422,12 +7058,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B81" s="1">
         <v>20</v>
@@ -6436,12 +7072,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B82" s="1">
         <v>10</v>
@@ -6450,12 +7086,12 @@
         <v>0.1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B83" s="1">
         <v>4</v>
@@ -6464,12 +7100,12 @@
         <v>0.22</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B84" s="1">
         <v>500</v>
@@ -6478,12 +7114,12 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B85" s="1">
         <v>4</v>
@@ -6492,12 +7128,21 @@
         <v>0.25</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>0.44</v>
+      <c r="A86" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B86" s="1">
+        <v>50</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -6507,7 +7152,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B88" s="1">
         <v>4</v>
@@ -6516,22 +7161,22 @@
         <v>0.25</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B91" s="1">
         <v>4</v>
@@ -6540,12 +7185,12 @@
         <v>0.25</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B92" s="1">
         <v>4</v>
@@ -6554,12 +7199,12 @@
         <v>0.25</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B93" s="1">
         <v>4</v>
@@ -6568,15 +7213,15 @@
         <v>0.25</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="76" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B96" s="76" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C96" s="76"/>
       <c r="D96" s="76"/>
@@ -6594,221 +7239,227 @@
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="76"/>
       <c r="B98" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="F98" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -6824,127 +7475,145 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55303D08-B4AE-4EBE-A1E9-A3155C29D25A}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B2" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="C15" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>2</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>10</v>
       </c>
     </row>
@@ -7037,22 +7706,22 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -7104,22 +7773,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="21" x14ac:dyDescent="0.35">
@@ -7179,22 +7848,22 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -7246,22 +7915,22 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="21" x14ac:dyDescent="0.35">
@@ -7321,22 +7990,22 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -7388,22 +8057,22 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="21" x14ac:dyDescent="0.35">
@@ -7463,22 +8132,22 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -7530,22 +8199,22 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="21" x14ac:dyDescent="0.35">
@@ -7605,22 +8274,22 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -7672,22 +8341,22 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.35">
@@ -7723,27 +8392,27 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A74" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B74" s="28"/>
     </row>
@@ -7793,40 +8462,40 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C76" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D76" s="31">
         <v>0.32</v>
       </c>
       <c r="E76" t="s">
+        <v>153</v>
+      </c>
+      <c r="G76" t="s">
+        <v>153</v>
+      </c>
+      <c r="H76" t="s">
+        <v>156</v>
+      </c>
+      <c r="I76" t="s">
+        <v>156</v>
+      </c>
+      <c r="J76" t="s">
         <v>154</v>
       </c>
-      <c r="G76" t="s">
+      <c r="K76" t="s">
         <v>154</v>
       </c>
-      <c r="H76" t="s">
-        <v>157</v>
-      </c>
-      <c r="I76" t="s">
-        <v>157</v>
-      </c>
-      <c r="J76" t="s">
-        <v>155</v>
-      </c>
-      <c r="K76" t="s">
-        <v>155</v>
-      </c>
       <c r="L76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O76" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -7875,42 +8544,42 @@
         <v>0.32</v>
       </c>
       <c r="C79" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I79" t="s">
+        <v>164</v>
+      </c>
+      <c r="J79" t="s">
+        <v>164</v>
+      </c>
+      <c r="K79" t="s">
         <v>165</v>
       </c>
-      <c r="J79" t="s">
-        <v>165</v>
-      </c>
-      <c r="K79" t="s">
-        <v>166</v>
-      </c>
       <c r="L79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M79" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -7918,67 +8587,67 @@
         <v>0.32</v>
       </c>
       <c r="B82" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C82" t="s">
+        <v>129</v>
+      </c>
+      <c r="D82" t="s">
         <v>130</v>
       </c>
-      <c r="D82" t="s">
-        <v>131</v>
-      </c>
       <c r="E82" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B83" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" t="s">
+        <v>134</v>
+      </c>
+      <c r="D83" t="s">
+        <v>139</v>
+      </c>
+      <c r="E83" t="s">
         <v>136</v>
-      </c>
-      <c r="C83" t="s">
-        <v>135</v>
-      </c>
-      <c r="D83" t="s">
-        <v>140</v>
-      </c>
-      <c r="E83" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" t="s">
+        <v>135</v>
+      </c>
+      <c r="C84" t="s">
+        <v>134</v>
+      </c>
+      <c r="D84" t="s">
         <v>155</v>
       </c>
-      <c r="B84" t="s">
-        <v>136</v>
-      </c>
-      <c r="C84" t="s">
-        <v>135</v>
-      </c>
-      <c r="D84" t="s">
-        <v>156</v>
-      </c>
       <c r="E84" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B85" t="s">
+        <v>135</v>
+      </c>
+      <c r="C85" t="s">
+        <v>150</v>
+      </c>
+      <c r="D85" t="s">
+        <v>138</v>
+      </c>
+      <c r="E85" t="s">
         <v>136</v>
-      </c>
-      <c r="C85" t="s">
-        <v>151</v>
-      </c>
-      <c r="D85" t="s">
-        <v>139</v>
-      </c>
-      <c r="E85" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -7986,108 +8655,108 @@
         <v>0.24299999999999999</v>
       </c>
       <c r="B86" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C86" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D86" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E86" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B87" t="s">
         <v>157</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>158</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>159</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>160</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>161</v>
-      </c>
-      <c r="F87" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B88" t="s">
+        <v>135</v>
+      </c>
+      <c r="C88" t="s">
+        <v>134</v>
+      </c>
+      <c r="D88" t="s">
         <v>163</v>
       </c>
-      <c r="B88" t="s">
+      <c r="E88" t="s">
         <v>136</v>
-      </c>
-      <c r="C88" t="s">
-        <v>135</v>
-      </c>
-      <c r="D88" t="s">
-        <v>164</v>
-      </c>
-      <c r="E88" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B89" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C89" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D89" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E89" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B90" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" t="s">
+        <v>168</v>
+      </c>
+      <c r="C91" t="s">
+        <v>152</v>
+      </c>
+      <c r="D91" t="s">
         <v>167</v>
-      </c>
-      <c r="B91" t="s">
-        <v>169</v>
-      </c>
-      <c r="C91" t="s">
-        <v>153</v>
-      </c>
-      <c r="D91" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" t="s">
         <v>171</v>
-      </c>
-      <c r="B93" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -8097,16 +8766,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B96" t="s">
+        <v>171</v>
+      </c>
+      <c r="C96" t="s">
+        <v>174</v>
+      </c>
+      <c r="D96" t="s">
         <v>173</v>
-      </c>
-      <c r="B96" t="s">
-        <v>172</v>
-      </c>
-      <c r="C96" t="s">
-        <v>175</v>
-      </c>
-      <c r="D96" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -8119,8 +8788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49260601-DFFC-49C5-BC21-5E0477EEDF42}">
   <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8335,7 +9004,7 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made it to the next church
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266F0C67-25FB-4949-AAE6-94FBC87E66DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ED2208-4B23-4CA0-A34B-F049DB788FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="353">
   <si>
     <t>Mission</t>
   </si>
@@ -1089,6 +1089,15 @@
   </si>
   <si>
     <t>Ed</t>
+  </si>
+  <si>
+    <t>12ga Birdshot Ammo</t>
+  </si>
+  <si>
+    <t>Beakon</t>
+  </si>
+  <si>
+    <t>Black Dala Horse</t>
   </si>
 </sst>
 </file>
@@ -2016,11 +2025,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R297"/>
+  <dimension ref="A1:R312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M298" sqref="M298"/>
+      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M313" sqref="M313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4714,7 +4723,7 @@
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J177" s="9" t="s">
+      <c r="J177" s="56" t="s">
         <v>266</v>
       </c>
       <c r="M177" s="10">
@@ -4728,7 +4737,7 @@
       </c>
     </row>
     <row r="178" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J178" s="9" t="s">
+      <c r="J178" s="56" t="s">
         <v>11</v>
       </c>
       <c r="M178" s="12"/>
@@ -4781,7 +4790,7 @@
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J182" s="9" t="s">
+      <c r="J182" s="56" t="s">
         <v>25</v>
       </c>
       <c r="K182" s="2">
@@ -4796,7 +4805,7 @@
       <c r="O182" s="11"/>
     </row>
     <row r="183" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J183" s="9" t="s">
+      <c r="J183" s="56" t="s">
         <v>98</v>
       </c>
       <c r="M183" s="12"/>
@@ -6469,6 +6478,214 @@
       </c>
       <c r="O297" s="2">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D298" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="M298" s="1">
+        <v>-133</v>
+      </c>
+      <c r="N298" s="1">
+        <v>3571</v>
+      </c>
+    </row>
+    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F299" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G299" s="2">
+        <v>2</v>
+      </c>
+      <c r="M299" s="1">
+        <v>-120</v>
+      </c>
+      <c r="N299" s="1">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="300" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F300" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G300" s="2">
+        <v>2</v>
+      </c>
+      <c r="M300" s="1">
+        <v>-106</v>
+      </c>
+      <c r="N300" s="1">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A301" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J301" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L301" s="9"/>
+      <c r="M301" s="10">
+        <v>-102</v>
+      </c>
+      <c r="N301" s="14">
+        <v>3300</v>
+      </c>
+      <c r="O301" s="11"/>
+    </row>
+    <row r="302" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J302" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="L302" s="9"/>
+      <c r="M302" s="16"/>
+      <c r="N302" s="79"/>
+      <c r="O302" s="25"/>
+    </row>
+    <row r="303" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J303" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K303" s="2">
+        <v>2</v>
+      </c>
+      <c r="L303" s="9"/>
+      <c r="M303" s="12"/>
+      <c r="N303" s="15"/>
+      <c r="O303" s="13"/>
+    </row>
+    <row r="304" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F304" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G304" s="2">
+        <v>1</v>
+      </c>
+      <c r="J304" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M304" s="1">
+        <v>327</v>
+      </c>
+      <c r="N304" s="1">
+        <v>2892</v>
+      </c>
+      <c r="O304" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J305" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K305" s="2">
+        <v>2</v>
+      </c>
+      <c r="M305" s="1">
+        <v>342</v>
+      </c>
+      <c r="N305" s="1">
+        <v>2885</v>
+      </c>
+    </row>
+    <row r="306" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J306" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="M306" s="1">
+        <v>351</v>
+      </c>
+      <c r="N306" s="1">
+        <v>2872</v>
+      </c>
+    </row>
+    <row r="307" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J307" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K307" s="2">
+        <v>3</v>
+      </c>
+      <c r="M307" s="1">
+        <v>346</v>
+      </c>
+      <c r="N307" s="1">
+        <v>2871</v>
+      </c>
+    </row>
+    <row r="308" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J308" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K308" s="2">
+        <v>2</v>
+      </c>
+      <c r="M308" s="1">
+        <v>343</v>
+      </c>
+      <c r="N308" s="1">
+        <v>2881</v>
+      </c>
+    </row>
+    <row r="309" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A309" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="M309" s="1">
+        <v>168</v>
+      </c>
+      <c r="N309" s="1">
+        <v>2585</v>
+      </c>
+    </row>
+    <row r="310" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C310" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="M310" s="1">
+        <v>140</v>
+      </c>
+      <c r="N310" s="1">
+        <v>2773</v>
+      </c>
+      <c r="O310" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J311" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="M311" s="1">
+        <v>127</v>
+      </c>
+      <c r="N311" s="1">
+        <v>2772</v>
+      </c>
+      <c r="O311" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="312" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F312" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G312" s="2">
+        <v>1</v>
+      </c>
+      <c r="M312" s="1">
+        <v>130</v>
+      </c>
+      <c r="N312" s="1">
+        <v>2779</v>
+      </c>
+      <c r="O312" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6500,9 +6717,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
   <dimension ref="A1:P121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O12" sqref="O12"/>
+      <selection pane="topRight" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
The whole Finx pinn. Looted.
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADA0992-0BCD-4DFB-8167-BA048AD2033C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8572EAA6-1F61-4603-8802-42115946A3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="373">
   <si>
     <t>Mission</t>
   </si>
@@ -914,15 +914,9 @@
     <t>Storage Station Upgrades</t>
   </si>
   <si>
-    <t>16 Steel | Electrolyte 8 | Aluminium 4</t>
-  </si>
-  <si>
     <t>Adhesive 1 | Plastic 2</t>
   </si>
   <si>
-    <t>16 Wood | 8 Adhesive | Aluminium 4</t>
-  </si>
-  <si>
     <t>Object_Penetration_Vision_Modulator</t>
   </si>
   <si>
@@ -1031,9 +1025,6 @@
     <t>0.44 FMJ</t>
   </si>
   <si>
-    <t>32 Wood | 16 Adhesive | 8 Lead</t>
-  </si>
-  <si>
     <t>Beacon</t>
   </si>
   <si>
@@ -1125,6 +1116,48 @@
   </si>
   <si>
     <t>Adhesive 6 | Plastic 11</t>
+  </si>
+  <si>
+    <t>Shotgun Silencer</t>
+  </si>
+  <si>
+    <t>Shotgun Silencer (Lock)</t>
+  </si>
+  <si>
+    <t>Adrenaline  (Lock)</t>
+  </si>
+  <si>
+    <t>Standard 1st Aid Kit  (Lock)</t>
+  </si>
+  <si>
+    <t>M/46 “Kpist” SMG (Lock)</t>
+  </si>
+  <si>
+    <t>Dual Mode Low Light / IR Module</t>
+  </si>
+  <si>
+    <t>Adhesive 2 | Rubber 4 | Plastic 4 | Titanium 1 | Aluminium 1</t>
+  </si>
+  <si>
+    <t>Steel 16 | Electrolyte 8 | Aluminium 4</t>
+  </si>
+  <si>
+    <t>Wood 32 | Adhesive 16 | Lead 8</t>
+  </si>
+  <si>
+    <t>Steel 13 | Electrolyte 16 | Lead 8</t>
+  </si>
+  <si>
+    <t>Wood 16 | Adhesive 8 | Aluminium 4</t>
+  </si>
+  <si>
+    <t>Wood 48 | Adhesive 24 | Copper 12</t>
+  </si>
+  <si>
+    <t>Wood 88 | Adhesive 44 |  Titanium 22</t>
+  </si>
+  <si>
+    <t>Steel 48 | Electrolyte 24 | Copper 12</t>
   </si>
 </sst>
 </file>
@@ -2052,11 +2085,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R357"/>
+  <dimension ref="A1:R392"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A337" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M358" sqref="M358"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A375" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M393" sqref="M393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3163,7 +3196,7 @@
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="M67" s="1">
         <v>2113</v>
@@ -4210,7 +4243,7 @@
     </row>
     <row r="141" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="M141" s="1">
         <v>1464</v>
@@ -4239,7 +4272,7 @@
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J143" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K143" s="1">
         <v>8</v>
@@ -4298,7 +4331,7 @@
     </row>
     <row r="146" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J146" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K146" s="1"/>
       <c r="L146" s="12" t="s">
@@ -4632,7 +4665,7 @@
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L168" s="9"/>
       <c r="M168" s="26">
@@ -4790,7 +4823,7 @@
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>27</v>
@@ -4952,7 +4985,7 @@
     </row>
     <row r="192" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M192" s="1">
         <v>1418</v>
@@ -4975,7 +5008,7 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L194" s="2"/>
       <c r="M194" s="1">
@@ -4988,7 +5021,7 @@
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M195" s="1">
         <v>1577</v>
@@ -4999,7 +5032,7 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M196" s="1">
         <v>1561</v>
@@ -5010,7 +5043,7 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M197" s="1">
         <v>1409</v>
@@ -5077,13 +5110,13 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F202" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G202" s="2">
         <v>1</v>
       </c>
       <c r="J202" s="56" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K202" s="1">
         <v>2</v>
@@ -5101,7 +5134,7 @@
     </row>
     <row r="203" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J203" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K203" s="1"/>
       <c r="L203" s="39" t="s">
@@ -5111,7 +5144,7 @@
     </row>
     <row r="204" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="K204" s="1"/>
       <c r="L204" s="26"/>
@@ -5131,14 +5164,14 @@
         <v>4</v>
       </c>
       <c r="M205" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="N205" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O205" s="1"/>
       <c r="P205" s="52" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="Q205" s="53"/>
       <c r="R205" s="54"/>
@@ -5159,7 +5192,7 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>27</v>
@@ -5193,7 +5226,7 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D209" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E209" s="2">
         <v>1</v>
@@ -5244,7 +5277,7 @@
     </row>
     <row r="212" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="M212" s="1">
         <v>1520</v>
@@ -5275,14 +5308,14 @@
         <v>-1</v>
       </c>
       <c r="P213" s="58" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="Q213" s="59"/>
       <c r="R213" s="60"/>
     </row>
     <row r="214" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B214" s="25" t="s">
         <v>27</v>
@@ -5296,7 +5329,7 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B215" s="25" t="s">
         <v>27</v>
@@ -5305,14 +5338,14 @@
       <c r="M215" s="16"/>
       <c r="O215" s="25"/>
       <c r="P215" s="43" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="Q215" s="44"/>
       <c r="R215" s="45"/>
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B216" s="25" t="s">
         <v>27</v>
@@ -5325,7 +5358,7 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B217" s="25" t="s">
         <v>27</v>
@@ -5338,7 +5371,7 @@
     </row>
     <row r="218" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B218" s="13" t="s">
         <v>27</v>
@@ -5381,7 +5414,7 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B221" s="11" t="s">
         <v>28</v>
@@ -5394,14 +5427,14 @@
       </c>
       <c r="O221" s="11"/>
       <c r="P221" s="58" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="Q221" s="59"/>
       <c r="R221" s="60"/>
     </row>
     <row r="222" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B222" s="13" t="s">
         <v>27</v>
@@ -5415,7 +5448,7 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B223" s="2">
         <v>1</v>
@@ -5429,7 +5462,7 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>28</v>
@@ -5443,7 +5476,7 @@
     </row>
     <row r="225" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M225" s="1">
         <v>3294</v>
@@ -5479,7 +5512,7 @@
     </row>
     <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M228" s="1">
         <v>3324</v>
@@ -5490,7 +5523,7 @@
     </row>
     <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C229" s="19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="M229" s="1">
         <v>3181</v>
@@ -5501,7 +5534,7 @@
     </row>
     <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B230" s="2">
         <v>1</v>
@@ -5565,7 +5598,7 @@
     </row>
     <row r="234" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J234" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K234" s="1"/>
       <c r="L234" s="39" t="s">
@@ -5581,7 +5614,7 @@
     </row>
     <row r="235" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J235" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K235" s="1"/>
       <c r="L235" s="39" t="s">
@@ -5597,7 +5630,7 @@
     </row>
     <row r="236" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J236" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K236" s="1"/>
       <c r="L236" s="39" t="s">
@@ -5619,7 +5652,7 @@
         <v>2</v>
       </c>
       <c r="J237" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K237" s="1"/>
       <c r="L237" s="39" t="s">
@@ -5635,7 +5668,7 @@
     </row>
     <row r="238" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J238" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K238" s="1"/>
       <c r="L238" s="38" t="s">
@@ -5676,7 +5709,7 @@
     </row>
     <row r="241" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H241" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M241" s="1">
         <v>1582</v>
@@ -5687,7 +5720,7 @@
     </row>
     <row r="242" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="M242" s="1">
         <v>1785</v>
@@ -5767,7 +5800,7 @@
     </row>
     <row r="248" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J248" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K248" s="1">
         <v>3</v>
@@ -5787,13 +5820,13 @@
     </row>
     <row r="249" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F249" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G249" s="2">
         <v>2</v>
       </c>
       <c r="H249" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="I249" s="2">
         <v>2</v>
@@ -5814,7 +5847,7 @@
     </row>
     <row r="250" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J250" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K250" s="1"/>
       <c r="L250" s="40" t="s">
@@ -5832,7 +5865,7 @@
     </row>
     <row r="251" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F251" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G251" s="2">
         <v>1</v>
@@ -5864,7 +5897,7 @@
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F253" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G253" s="2">
         <v>2</v>
@@ -5900,7 +5933,7 @@
     </row>
     <row r="255" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J255" s="9" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K255" s="1"/>
       <c r="L255" s="38" t="s">
@@ -5912,7 +5945,7 @@
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D256" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E256" s="2">
         <v>1</v>
@@ -5968,7 +6001,7 @@
     </row>
     <row r="260" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H260" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I260" s="2">
         <v>1</v>
@@ -6088,7 +6121,7 @@
     </row>
     <row r="269" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B269" s="2">
         <v>1</v>
@@ -6115,7 +6148,7 @@
     </row>
     <row r="271" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F271" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G271" s="2">
         <v>2</v>
@@ -6137,7 +6170,7 @@
     </row>
     <row r="272" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J272" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K272" s="1"/>
       <c r="L272" s="39" t="s">
@@ -6147,7 +6180,7 @@
     </row>
     <row r="273" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J273" s="9" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="K273" s="1">
         <v>4</v>
@@ -6159,7 +6192,7 @@
     </row>
     <row r="274" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J274" s="9" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="K274" s="1">
         <v>3</v>
@@ -6173,7 +6206,7 @@
     </row>
     <row r="275" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K275" s="1"/>
       <c r="L275" s="57"/>
@@ -6187,7 +6220,7 @@
     </row>
     <row r="276" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M276" s="1">
         <v>786</v>
@@ -6198,7 +6231,7 @@
     </row>
     <row r="277" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>27</v>
@@ -6265,7 +6298,7 @@
     </row>
     <row r="282" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B282" s="2">
         <v>2</v>
@@ -6279,7 +6312,7 @@
     </row>
     <row r="283" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B283" s="2">
         <v>3</v>
@@ -6293,7 +6326,7 @@
     </row>
     <row r="284" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A284" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B284" s="11" t="s">
         <v>28</v>
@@ -6306,14 +6339,14 @@
       </c>
       <c r="O284" s="11"/>
       <c r="P284" s="58" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="Q284" s="59"/>
       <c r="R284" s="60"/>
     </row>
     <row r="285" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="12" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B285" s="13" t="s">
         <v>27</v>
@@ -6327,7 +6360,7 @@
     </row>
     <row r="286" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B286" s="2">
         <v>1</v>
@@ -6369,7 +6402,7 @@
     </row>
     <row r="289" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B289" s="2">
         <v>2</v>
@@ -6384,7 +6417,7 @@
     </row>
     <row r="290" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M290" s="12"/>
       <c r="N290" s="15"/>
@@ -6392,7 +6425,7 @@
     </row>
     <row r="291" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M291" s="1">
         <v>684</v>
@@ -6403,7 +6436,7 @@
     </row>
     <row r="292" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B292" s="2">
         <v>3</v>
@@ -6420,10 +6453,10 @@
     </row>
     <row r="293" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="M293" s="1">
         <v>752</v>
@@ -6437,10 +6470,10 @@
     </row>
     <row r="294" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="M294" s="1">
         <v>790</v>
@@ -6471,10 +6504,10 @@
     </row>
     <row r="296" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="M296" s="1">
         <v>826</v>
@@ -6488,10 +6521,10 @@
     </row>
     <row r="297" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M297" s="1">
         <v>815</v>
@@ -6505,7 +6538,7 @@
     </row>
     <row r="298" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D298" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="M298" s="1">
         <v>-133</v>
@@ -6544,7 +6577,7 @@
     </row>
     <row r="301" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>28</v>
@@ -6656,7 +6689,7 @@
     </row>
     <row r="309" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="M309" s="1">
         <v>168</v>
@@ -6667,7 +6700,7 @@
     </row>
     <row r="310" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C310" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="M310" s="1">
         <v>140</v>
@@ -6752,7 +6785,7 @@
     </row>
     <row r="316" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>27</v>
@@ -6772,7 +6805,7 @@
     </row>
     <row r="317" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B317" s="2">
         <v>1</v>
@@ -6815,7 +6848,7 @@
     </row>
     <row r="320" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J320" s="9" t="s">
-        <v>84</v>
+        <v>266</v>
       </c>
       <c r="K320" s="2">
         <v>5</v>
@@ -6857,7 +6890,7 @@
     </row>
     <row r="323" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M323" s="1">
         <v>-34</v>
@@ -6868,7 +6901,7 @@
     </row>
     <row r="324" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M324" s="1">
         <v>-13</v>
@@ -6896,7 +6929,7 @@
     </row>
     <row r="326" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D326" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E326" s="2">
         <v>1</v>
@@ -6947,7 +6980,7 @@
     </row>
     <row r="329" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="M329" s="1">
         <v>-337</v>
@@ -6997,7 +7030,7 @@
     </row>
     <row r="333" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="M333" s="1">
         <v>-1197</v>
@@ -7008,10 +7041,10 @@
     </row>
     <row r="334" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A334" s="10" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B334" s="11" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="M334" s="10">
         <v>-1559</v>
@@ -7021,14 +7054,14 @@
       </c>
       <c r="O334" s="11"/>
       <c r="P334" s="58" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Q334" s="59"/>
       <c r="R334" s="60"/>
     </row>
     <row r="335" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="12" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B335" s="13" t="s">
         <v>27</v>
@@ -7101,7 +7134,7 @@
         <v>2</v>
       </c>
       <c r="J340" s="9" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="K340" s="2">
         <v>2</v>
@@ -7297,7 +7330,7 @@
     </row>
     <row r="353" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C353" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="M353" s="1">
         <v>-1612</v>
@@ -7322,7 +7355,7 @@
     </row>
     <row r="355" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B355" s="2">
         <v>1</v>
@@ -7339,7 +7372,7 @@
     </row>
     <row r="356" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M356" s="1">
         <v>-1675</v>
@@ -7362,6 +7395,490 @@
         <v>3832</v>
       </c>
       <c r="O357" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J358" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M358" s="1">
+        <v>-936</v>
+      </c>
+      <c r="N358" s="1">
+        <v>3527</v>
+      </c>
+    </row>
+    <row r="359" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J359" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="M359" s="1">
+        <v>-942</v>
+      </c>
+      <c r="N359" s="1">
+        <v>3369</v>
+      </c>
+    </row>
+    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J360" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M360" s="1">
+        <v>-938</v>
+      </c>
+      <c r="N360" s="1">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="361" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J361" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="M361" s="1">
+        <v>-940</v>
+      </c>
+      <c r="N361" s="1">
+        <v>3366</v>
+      </c>
+    </row>
+    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F362" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G362" s="2">
+        <v>2</v>
+      </c>
+      <c r="J362" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="L362" s="9"/>
+      <c r="M362" s="10">
+        <v>-944</v>
+      </c>
+      <c r="N362" s="14">
+        <v>3366</v>
+      </c>
+      <c r="O362" s="11"/>
+    </row>
+    <row r="363" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J363" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="L363" s="9"/>
+      <c r="M363" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="N363" s="15"/>
+      <c r="O363" s="13"/>
+    </row>
+    <row r="364" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J364" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="K364" s="2">
+        <v>2</v>
+      </c>
+      <c r="M364" s="1">
+        <v>-981</v>
+      </c>
+      <c r="N364" s="1">
+        <v>3382</v>
+      </c>
+    </row>
+    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J365" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K365" s="2">
+        <v>2</v>
+      </c>
+      <c r="M365" s="10">
+        <v>-1011</v>
+      </c>
+      <c r="N365" s="14">
+        <v>361</v>
+      </c>
+      <c r="O365" s="11"/>
+    </row>
+    <row r="366" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J366" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M366" s="12"/>
+      <c r="N366" s="15"/>
+      <c r="O366" s="13"/>
+    </row>
+    <row r="367" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J367" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M367" s="1">
+        <v>-946</v>
+      </c>
+      <c r="N367" s="1">
+        <v>3334</v>
+      </c>
+    </row>
+    <row r="368" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F368" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G368" s="2">
+        <v>1</v>
+      </c>
+      <c r="M368" s="1">
+        <v>-959</v>
+      </c>
+      <c r="N368" s="1">
+        <v>3332</v>
+      </c>
+      <c r="O368" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="369" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B369" s="2">
+        <v>2</v>
+      </c>
+      <c r="M369" s="1">
+        <v>-821</v>
+      </c>
+      <c r="N369" s="1">
+        <v>3303</v>
+      </c>
+      <c r="O369" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="370" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A370" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B370" s="2">
+        <v>3</v>
+      </c>
+      <c r="M370" s="1">
+        <v>-808</v>
+      </c>
+      <c r="N370" s="1">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="371" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K371" s="80"/>
+      <c r="L371" s="40">
+        <v>4</v>
+      </c>
+      <c r="M371" s="41">
+        <v>-834</v>
+      </c>
+      <c r="N371" s="41">
+        <v>3295</v>
+      </c>
+      <c r="O371" s="42"/>
+    </row>
+    <row r="372" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J372" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M372" s="1">
+        <v>-648</v>
+      </c>
+      <c r="N372" s="1">
+        <v>3401</v>
+      </c>
+    </row>
+    <row r="373" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F373" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G373" s="2">
+        <v>1</v>
+      </c>
+      <c r="M373" s="1">
+        <v>-652</v>
+      </c>
+      <c r="N373" s="1">
+        <v>3392</v>
+      </c>
+    </row>
+    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F374" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="G374" s="2">
+        <v>3</v>
+      </c>
+      <c r="J374" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="K374" s="80"/>
+      <c r="L374" s="37">
+        <v>6</v>
+      </c>
+      <c r="M374" s="14">
+        <v>-432</v>
+      </c>
+      <c r="N374" s="14">
+        <v>3124</v>
+      </c>
+      <c r="O374" s="11"/>
+    </row>
+    <row r="375" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J375" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="K375" s="80">
+        <v>2</v>
+      </c>
+      <c r="L375" s="39"/>
+      <c r="M375" s="80"/>
+      <c r="N375" s="80"/>
+      <c r="O375" s="25"/>
+    </row>
+    <row r="376" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J376" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="K376" s="80"/>
+      <c r="L376" s="38"/>
+      <c r="M376" s="15"/>
+      <c r="N376" s="15"/>
+      <c r="O376" s="13"/>
+    </row>
+    <row r="377" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J377" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="M377" s="1">
+        <v>-584</v>
+      </c>
+      <c r="N377" s="1">
+        <v>3196</v>
+      </c>
+      <c r="O377" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="378" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A378" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F378" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G378" s="2">
+        <v>2</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I378" s="2">
+        <v>1</v>
+      </c>
+      <c r="L378" s="9"/>
+      <c r="M378" s="10">
+        <v>-580</v>
+      </c>
+      <c r="N378" s="14">
+        <v>3196</v>
+      </c>
+      <c r="O378" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="379" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H379" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="I379" s="2">
+        <v>1</v>
+      </c>
+      <c r="L379" s="9"/>
+      <c r="M379" s="12"/>
+      <c r="N379" s="15"/>
+      <c r="O379" s="13"/>
+    </row>
+    <row r="380" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F380" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G380" s="2">
+        <v>1</v>
+      </c>
+      <c r="M380" s="1">
+        <v>135</v>
+      </c>
+      <c r="N380" s="1">
+        <v>2817</v>
+      </c>
+    </row>
+    <row r="381" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J381" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="M381" s="1">
+        <v>-519</v>
+      </c>
+      <c r="N381" s="1">
+        <v>3180</v>
+      </c>
+      <c r="O381" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="382" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J382" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M382" s="1">
+        <v>-512</v>
+      </c>
+      <c r="N382" s="1">
+        <v>3182</v>
+      </c>
+      <c r="O382" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="383" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J383" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="M383" s="1">
+        <v>-509</v>
+      </c>
+      <c r="N383" s="1">
+        <v>3181</v>
+      </c>
+      <c r="O383" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="384" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F384" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G384" s="2">
+        <v>1</v>
+      </c>
+      <c r="M384" s="1">
+        <v>-511</v>
+      </c>
+      <c r="N384" s="1">
+        <v>3186</v>
+      </c>
+    </row>
+    <row r="385" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J385" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M385" s="1">
+        <v>-513</v>
+      </c>
+      <c r="N385" s="1">
+        <v>3183</v>
+      </c>
+    </row>
+    <row r="386" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J386" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M386" s="1">
+        <v>-521</v>
+      </c>
+      <c r="N386" s="1">
+        <v>3182</v>
+      </c>
+    </row>
+    <row r="387" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F387" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G387" s="2">
+        <v>1</v>
+      </c>
+      <c r="M387" s="1">
+        <v>-296</v>
+      </c>
+      <c r="N387" s="1">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="388" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F388" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G388" s="2">
+        <v>1</v>
+      </c>
+      <c r="M388" s="1">
+        <v>-274</v>
+      </c>
+      <c r="N388" s="1">
+        <v>3057</v>
+      </c>
+    </row>
+    <row r="389" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J389" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M389" s="1">
+        <v>-275</v>
+      </c>
+      <c r="N389" s="1">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="390" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F390" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G390" s="2">
+        <v>1</v>
+      </c>
+      <c r="M390" s="1">
+        <v>-274</v>
+      </c>
+      <c r="N390" s="1">
+        <v>3051</v>
+      </c>
+      <c r="O390" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="391" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A391" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="M391" s="1">
+        <v>409</v>
+      </c>
+      <c r="N391" s="1">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="392" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F392" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G392" s="2">
+        <v>1</v>
+      </c>
+      <c r="M392" s="1">
+        <v>418</v>
+      </c>
+      <c r="N392" s="1">
+        <v>3463</v>
+      </c>
+      <c r="O392" s="2">
         <v>-1</v>
       </c>
     </row>
@@ -7393,17 +7910,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P122"/>
+  <dimension ref="A1:P124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" style="1" bestFit="1" customWidth="1"/>
@@ -7489,7 +8006,7 @@
         <v>126</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>146</v>
@@ -7552,6 +8069,9 @@
       <c r="J5" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="O5" s="1" t="s">
         <v>149</v>
       </c>
@@ -7675,7 +8195,7 @@
         <v>288</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -7948,7 +8468,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -8082,7 +8602,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="1">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>181</v>
@@ -8174,7 +8694,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -8424,6 +8944,15 @@
       <c r="A78" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="B78" s="1">
+        <v>125</v>
+      </c>
+      <c r="C78" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
@@ -8525,7 +9054,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B86" s="1">
         <v>50</v>
@@ -8539,7 +9068,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B87" s="1">
         <v>50</v>
@@ -8759,6 +9288,9 @@
       <c r="B110" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="C110" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
@@ -8784,7 +9316,7 @@
         <v>258</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>259</v>
@@ -8797,6 +9329,9 @@
       <c r="B114" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="C114" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
@@ -8819,7 +9354,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>270</v>
@@ -8827,7 +9362,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>244</v>
@@ -8835,7 +9370,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>270</v>
@@ -8843,32 +9378,48 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>187</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -8887,7 +9438,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8911,18 +9462,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>291</v>
+        <v>366</v>
+      </c>
+      <c r="C2" s="1">
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C3" s="1">
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C4" s="1">
+        <v>400</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -8972,7 +9538,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>293</v>
+        <v>369</v>
       </c>
       <c r="C15" s="1">
         <v>240</v>
@@ -8983,45 +9549,60 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+      <c r="C16" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C17" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C18" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>10</v>
       </c>
@@ -10197,8 +10778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49260601-DFFC-49C5-BC21-5E0477EEDF42}">
   <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Loot around the crowed field of machines.
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8572EAA6-1F61-4603-8802-42115946A3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F17C69-FC24-40E9-9483-5AB06044C8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="374">
   <si>
     <t>Mission</t>
   </si>
@@ -1158,6 +1158,9 @@
   </si>
   <si>
     <t>Steel 48 | Electrolyte 24 | Copper 12</t>
+  </si>
+  <si>
+    <t>Car Battery</t>
   </si>
 </sst>
 </file>
@@ -2085,11 +2088,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R392"/>
+  <dimension ref="A1:R416"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A375" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M393" sqref="M393"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A384" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M417" sqref="M417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7880,6 +7883,311 @@
       </c>
       <c r="O392" s="2">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J393" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="M393" s="1">
+        <v>350</v>
+      </c>
+      <c r="N393" s="1">
+        <v>2688</v>
+      </c>
+    </row>
+    <row r="394" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J394" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M394" s="1">
+        <v>340</v>
+      </c>
+      <c r="N394" s="1">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="395" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J395" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M395" s="1">
+        <v>136</v>
+      </c>
+      <c r="N395" s="1">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="396" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J396" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M396" s="1">
+        <v>202</v>
+      </c>
+      <c r="N396" s="1">
+        <v>2763</v>
+      </c>
+    </row>
+    <row r="397" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J397" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L397" s="9"/>
+      <c r="M397" s="10">
+        <v>638</v>
+      </c>
+      <c r="N397" s="14">
+        <v>2663</v>
+      </c>
+      <c r="O397" s="11"/>
+    </row>
+    <row r="398" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J398" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L398" s="9"/>
+      <c r="M398" s="12"/>
+      <c r="N398" s="15"/>
+      <c r="O398" s="13"/>
+    </row>
+    <row r="399" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J399" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M399" s="10">
+        <v>646</v>
+      </c>
+      <c r="N399" s="14">
+        <v>2661</v>
+      </c>
+      <c r="O399" s="11"/>
+    </row>
+    <row r="400" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J400" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="M400" s="16"/>
+      <c r="N400" s="80"/>
+      <c r="O400" s="25"/>
+    </row>
+    <row r="401" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J401" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="K401" s="80"/>
+      <c r="L401" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="M401" s="14">
+        <v>525</v>
+      </c>
+      <c r="N401" s="14">
+        <v>2552</v>
+      </c>
+      <c r="O401" s="11"/>
+    </row>
+    <row r="402" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J402" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K402" s="80"/>
+      <c r="L402" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="M402" s="15"/>
+      <c r="N402" s="15"/>
+      <c r="O402" s="13"/>
+    </row>
+    <row r="403" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J403" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M403" s="1">
+        <v>495</v>
+      </c>
+      <c r="N403" s="1">
+        <v>2602</v>
+      </c>
+    </row>
+    <row r="404" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A404" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B404" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M404" s="1">
+        <v>569</v>
+      </c>
+      <c r="N404" s="1">
+        <v>2226</v>
+      </c>
+    </row>
+    <row r="405" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H405" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I405" s="2">
+        <v>1</v>
+      </c>
+      <c r="J405" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="K405" s="2">
+        <v>8</v>
+      </c>
+      <c r="L405" s="9"/>
+      <c r="M405" s="10">
+        <v>533</v>
+      </c>
+      <c r="N405" s="14">
+        <v>2234</v>
+      </c>
+      <c r="O405" s="11"/>
+    </row>
+    <row r="406" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H406" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I406" s="2">
+        <v>1</v>
+      </c>
+      <c r="L406" s="9"/>
+      <c r="M406" s="12"/>
+      <c r="N406" s="15"/>
+      <c r="O406" s="13"/>
+    </row>
+    <row r="407" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J407" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M407" s="1">
+        <v>511</v>
+      </c>
+      <c r="N407" s="1">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="408" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J408" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M408" s="1">
+        <v>519</v>
+      </c>
+      <c r="N408" s="1">
+        <v>2226</v>
+      </c>
+      <c r="O408" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="409" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J409" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M409" s="1">
+        <v>443</v>
+      </c>
+      <c r="N409" s="1">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="410" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J410" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="K410" s="2">
+        <v>2</v>
+      </c>
+      <c r="M410" s="1">
+        <v>718</v>
+      </c>
+      <c r="N410" s="1">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="411" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F411" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G411" s="2">
+        <v>1</v>
+      </c>
+      <c r="J411" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="K411" s="2">
+        <v>1</v>
+      </c>
+      <c r="M411" s="1">
+        <v>711</v>
+      </c>
+      <c r="N411" s="1">
+        <v>2266</v>
+      </c>
+      <c r="O411" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="412" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J412" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M412" s="10">
+        <v>703</v>
+      </c>
+      <c r="N412" s="14">
+        <v>2212</v>
+      </c>
+      <c r="O412" s="11"/>
+    </row>
+    <row r="413" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J413" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M413" s="12"/>
+      <c r="N413" s="15"/>
+      <c r="O413" s="13"/>
+    </row>
+    <row r="414" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H414" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I414" s="2">
+        <v>1</v>
+      </c>
+      <c r="M414" s="1">
+        <v>698</v>
+      </c>
+      <c r="N414" s="1">
+        <v>2247</v>
+      </c>
+      <c r="O414" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="415" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J415" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M415" s="1">
+        <v>688</v>
+      </c>
+      <c r="N415" s="1">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="416" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J416" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M416" s="1">
+        <v>687</v>
+      </c>
+      <c r="N416" s="1">
+        <v>2248</v>
       </c>
     </row>
   </sheetData>
@@ -7912,9 +8220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
   <dimension ref="A1:P124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B35" sqref="B35"/>
+      <selection pane="topRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8167,6 +8475,9 @@
       </c>
       <c r="C11" s="1" t="s">
         <v>145</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>145</v>
@@ -10779,7 +11090,7 @@
   <dimension ref="A1:A84"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Looting Farmland staging base.
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F60540-4C85-40C3-9CDB-056DD7D94D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1937A05A-E307-4512-80AE-0D23E1A26214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="375">
   <si>
     <t>Mission</t>
   </si>
@@ -2088,11 +2088,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R428"/>
+  <dimension ref="A1:R432"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A406" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M429" sqref="M429"/>
+      <pane ySplit="1" topLeftCell="A417" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M433" sqref="M433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8342,6 +8342,62 @@
       </c>
       <c r="N428" s="1">
         <v>2040</v>
+      </c>
+    </row>
+    <row r="429" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F429" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G429" s="2">
+        <v>1</v>
+      </c>
+      <c r="M429" s="1">
+        <v>-203</v>
+      </c>
+      <c r="N429" s="1">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="430" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F430" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G430" s="2">
+        <v>1</v>
+      </c>
+      <c r="M430" s="1">
+        <v>-188</v>
+      </c>
+      <c r="N430" s="1">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="431" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F431" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G431" s="2">
+        <v>1</v>
+      </c>
+      <c r="M431" s="1">
+        <v>-167</v>
+      </c>
+      <c r="N431" s="1">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="432" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F432" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G432" s="2">
+        <v>1</v>
+      </c>
+      <c r="M432" s="1">
+        <v>-244</v>
+      </c>
+      <c r="N432" s="1">
+        <v>2050</v>
       </c>
     </row>
   </sheetData>
@@ -8374,9 +8430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
   <dimension ref="A1:P124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D13" sqref="D13"/>
+      <selection pane="topRight" activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9874,6 +9930,9 @@
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>359</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>271</v>

</xml_diff>

<commit_message>
Loot up to 5.5mm FMJ
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD67BE4-48E9-4F1A-94DC-6D72F8B9128D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FB4E2C-9AF9-4AAB-B6F2-53619E22033B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="417">
   <si>
     <t>Mission</t>
   </si>
@@ -1236,6 +1236,60 @@
   </si>
   <si>
     <t>Classic Dala Horse (???)</t>
+  </si>
+  <si>
+    <t>Explosive 4 | Steel 8 | Lead 2 | Copper 2</t>
+  </si>
+  <si>
+    <t>AG_4_Magazine</t>
+  </si>
+  <si>
+    <t>Advesive 3 | Steel 6 | Aluminium 1 | Tungsten 1</t>
+  </si>
+  <si>
+    <t>AI_76_Magazine</t>
+  </si>
+  <si>
+    <t>Wood 160 | Adhesive 80 | Tungsten 20</t>
+  </si>
+  <si>
+    <t>12ga Buckshot Ammo</t>
+  </si>
+  <si>
+    <t>Athletic Pants</t>
+  </si>
+  <si>
+    <t>12ga Slug Ammo</t>
+  </si>
+  <si>
+    <t>9mm FMJ Ammo (SMG)</t>
+  </si>
+  <si>
+    <t>Bullet-Resistant Shirt (Lock)</t>
+  </si>
+  <si>
+    <t>Emil Sandberg's radio hits</t>
+  </si>
+  <si>
+    <t>9mm AP Ammo (SMG)</t>
+  </si>
+  <si>
+    <t>7.62mm FMG Ammo</t>
+  </si>
+  <si>
+    <t>Ingrid Granqvist's mixtape</t>
+  </si>
+  <si>
+    <t>The Ruin of Many a Poor Man</t>
+  </si>
+  <si>
+    <t>Camouflage Pants</t>
+  </si>
+  <si>
+    <t>4-8x Rifle Scope</t>
+  </si>
+  <si>
+    <t>5.56mm FMG Ammo</t>
   </si>
 </sst>
 </file>
@@ -2163,16 +2217,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R480"/>
+  <dimension ref="A1:R500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A453" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M481" sqref="M481"/>
+      <pane ySplit="1" topLeftCell="A466" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M501" sqref="M501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -9137,6 +9191,279 @@
       </c>
       <c r="N480" s="1">
         <v>-3475</v>
+      </c>
+    </row>
+    <row r="481" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A481" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="M481" s="1">
+        <v>-1674</v>
+      </c>
+      <c r="N481" s="1">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="482" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A482" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="M482" s="1">
+        <v>-2367</v>
+      </c>
+      <c r="N482" s="1">
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="483" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D483" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="M483" s="1">
+        <v>-2456</v>
+      </c>
+      <c r="N483" s="1">
+        <v>3255</v>
+      </c>
+    </row>
+    <row r="484" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D484" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E484" s="2">
+        <v>1</v>
+      </c>
+      <c r="M484" s="1">
+        <v>952</v>
+      </c>
+      <c r="N484" s="1">
+        <v>-2577</v>
+      </c>
+    </row>
+    <row r="485" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D485" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="M485" s="1">
+        <v>1734</v>
+      </c>
+      <c r="N485" s="1">
+        <v>-2629</v>
+      </c>
+    </row>
+    <row r="486" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D486" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="M486" s="1">
+        <v>-413</v>
+      </c>
+      <c r="N486" s="1">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="487" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D487" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E487" s="2">
+        <v>1</v>
+      </c>
+      <c r="K487" s="80"/>
+      <c r="L487" s="40">
+        <v>4</v>
+      </c>
+      <c r="M487" s="41">
+        <v>-365</v>
+      </c>
+      <c r="N487" s="41">
+        <v>924</v>
+      </c>
+      <c r="O487" s="42"/>
+    </row>
+    <row r="488" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C488" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J488" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="M488" s="1">
+        <v>597</v>
+      </c>
+      <c r="N488" s="1">
+        <v>-3712</v>
+      </c>
+    </row>
+    <row r="489" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F489" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G489" s="2">
+        <v>3</v>
+      </c>
+      <c r="M489" s="1">
+        <v>572</v>
+      </c>
+      <c r="N489" s="1">
+        <v>-3702</v>
+      </c>
+      <c r="O489" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="490" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A490" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="M490" s="1">
+        <v>442</v>
+      </c>
+      <c r="N490" s="1">
+        <v>-3790</v>
+      </c>
+    </row>
+    <row r="491" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J491" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M491" s="1">
+        <v>563</v>
+      </c>
+      <c r="N491" s="1">
+        <v>3699</v>
+      </c>
+      <c r="O491" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="492" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D492" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="M492" s="1">
+        <v>443</v>
+      </c>
+      <c r="N492" s="1">
+        <v>-4042</v>
+      </c>
+      <c r="O492" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="493" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D493" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="M493" s="1">
+        <v>-1123</v>
+      </c>
+      <c r="N493" s="1">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="494" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C494" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="M494" s="1">
+        <v>1549</v>
+      </c>
+      <c r="N494" s="1">
+        <v>-3112</v>
+      </c>
+      <c r="O494" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="495" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A495" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B495" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M495" s="1">
+        <v>1548</v>
+      </c>
+      <c r="N495" s="1">
+        <v>-3109</v>
+      </c>
+      <c r="O495" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="496" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A496" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B496" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D496" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E496" s="2">
+        <v>1</v>
+      </c>
+      <c r="F496" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G496" s="2">
+        <v>4</v>
+      </c>
+      <c r="H496" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="M496" s="1">
+        <v>1572</v>
+      </c>
+      <c r="N496" s="1">
+        <v>-3330</v>
+      </c>
+    </row>
+    <row r="497" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M497" s="1">
+        <v>1372</v>
+      </c>
+      <c r="N497" s="1">
+        <v>-3744</v>
+      </c>
+    </row>
+    <row r="498" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A498" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="M498" s="1">
+        <v>1123</v>
+      </c>
+      <c r="N498" s="1">
+        <v>-3593</v>
+      </c>
+    </row>
+    <row r="499" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D499" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="M499" s="1">
+        <v>-3780</v>
+      </c>
+      <c r="N499" s="1">
+        <v>4125</v>
+      </c>
+    </row>
+    <row r="500" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F500" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G500" s="2">
+        <v>3</v>
+      </c>
+      <c r="M500" s="1">
+        <v>-3968</v>
+      </c>
+      <c r="N500" s="1">
+        <v>4194</v>
       </c>
     </row>
   </sheetData>
@@ -9167,18 +9494,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P126"/>
+  <dimension ref="A1:P128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G12" sqref="G12"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.85546875" style="1" customWidth="1"/>
@@ -9320,6 +9647,9 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>144</v>
       </c>
@@ -9626,6 +9956,15 @@
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="B27" s="1">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -9870,6 +10209,12 @@
       <c r="A47" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -10425,6 +10770,15 @@
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>228</v>
+      </c>
+      <c r="B90" s="1">
+        <v>4</v>
+      </c>
+      <c r="C90" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -10623,6 +10977,9 @@
       <c r="C110" s="1" t="s">
         <v>271</v>
       </c>
+      <c r="D110" s="1" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
@@ -10643,7 +11000,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>258</v>
       </c>
@@ -10654,7 +11011,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>265</v>
       </c>
@@ -10668,7 +11025,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>269</v>
       </c>
@@ -10676,7 +11033,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>273</v>
       </c>
@@ -10687,7 +11044,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>292</v>
       </c>
@@ -10695,7 +11052,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>305</v>
       </c>
@@ -10703,7 +11060,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>306</v>
       </c>
@@ -10711,7 +11068,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>315</v>
       </c>
@@ -10722,7 +11079,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>317</v>
       </c>
@@ -10732,8 +11089,11 @@
       <c r="C121" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F121" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>356</v>
       </c>
@@ -10744,7 +11104,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>359</v>
       </c>
@@ -10755,7 +11115,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>364</v>
       </c>
@@ -10763,7 +11123,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>378</v>
       </c>
@@ -10774,12 +11134,28 @@
         <v>379</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>380</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>291</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -10798,7 +11174,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10940,6 +11316,12 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C19" s="1">
+        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
.243 FMJ Ammo Looted
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FB4E2C-9AF9-4AAB-B6F2-53619E22033B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E3C4D5-B558-47BF-BD26-0F11936D474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="426">
   <si>
     <t>Mission</t>
   </si>
@@ -1290,6 +1290,33 @@
   </si>
   <si>
     <t>5.56mm FMG Ammo</t>
+  </si>
+  <si>
+    <t>Top of the World</t>
+  </si>
+  <si>
+    <t>Tank (Army)</t>
+  </si>
+  <si>
+    <t>5.56mm AP Ammo</t>
+  </si>
+  <si>
+    <t>Supply Run</t>
+  </si>
+  <si>
+    <t>.243 SP Ammo</t>
+  </si>
+  <si>
+    <t>Not Alone</t>
+  </si>
+  <si>
+    <t>Good News</t>
+  </si>
+  <si>
+    <t>.243 FMJ Ammo</t>
+  </si>
+  <si>
+    <t>Call of the Wild</t>
   </si>
 </sst>
 </file>
@@ -1694,7 +1721,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1833,6 +1860,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1842,6 +1878,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1849,24 +1894,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1897,9 +1924,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2217,11 +2241,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:R500"/>
+  <dimension ref="A1:R523"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A466" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M501" sqref="M501"/>
+      <pane ySplit="1" topLeftCell="A514" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M524" sqref="M524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,42 +2268,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="64" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="64" t="s">
+      <c r="G1" s="59"/>
+      <c r="H1" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="66"/>
-      <c r="J1" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="66"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="59"/>
       <c r="L1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="64" t="s">
+      <c r="N1" s="60"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="66"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="59"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2558,11 +2582,11 @@
         <v>2243</v>
       </c>
       <c r="O17" s="1"/>
-      <c r="P17" s="58" t="s">
+      <c r="P17" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="60"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="63"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J18" s="9" t="s">
@@ -2581,9 +2605,9 @@
       <c r="O18" s="14">
         <v>2</v>
       </c>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="68"/>
-      <c r="R18" s="69"/>
+      <c r="P18" s="64"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="66"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J19" s="29" t="s">
@@ -2592,17 +2616,17 @@
       <c r="L19" s="9"/>
       <c r="M19" s="16"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="67"/>
-      <c r="Q19" s="68"/>
-      <c r="R19" s="69"/>
+      <c r="P19" s="64"/>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="66"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L20" s="9"/>
       <c r="M20" s="16"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="68"/>
-      <c r="R20" s="69"/>
+      <c r="P20" s="64"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="66"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
@@ -2614,9 +2638,9 @@
       <c r="L21" s="9"/>
       <c r="M21" s="16"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="67"/>
-      <c r="Q21" s="68"/>
-      <c r="R21" s="69"/>
+      <c r="P21" s="64"/>
+      <c r="Q21" s="65"/>
+      <c r="R21" s="66"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H22" s="1" t="s">
@@ -2629,9 +2653,9 @@
       <c r="M22" s="12"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="62"/>
-      <c r="R22" s="63"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="68"/>
+      <c r="R22" s="69"/>
     </row>
     <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -3187,11 +3211,11 @@
       <c r="O57" s="11">
         <v>2</v>
       </c>
-      <c r="P57" s="58" t="s">
+      <c r="P57" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="Q57" s="59"/>
-      <c r="R57" s="60"/>
+      <c r="Q57" s="62"/>
+      <c r="R57" s="63"/>
     </row>
     <row r="58" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
@@ -3204,9 +3228,9 @@
       <c r="M58" s="12"/>
       <c r="N58" s="15"/>
       <c r="O58" s="13"/>
-      <c r="P58" s="61"/>
-      <c r="Q58" s="62"/>
-      <c r="R58" s="63"/>
+      <c r="P58" s="67"/>
+      <c r="Q58" s="68"/>
+      <c r="R58" s="69"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -3448,11 +3472,11 @@
       <c r="O74" s="11">
         <v>-1</v>
       </c>
-      <c r="P74" s="58" t="s">
+      <c r="P74" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="Q74" s="59"/>
-      <c r="R74" s="60"/>
+      <c r="Q74" s="62"/>
+      <c r="R74" s="63"/>
     </row>
     <row r="75" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
@@ -3464,9 +3488,9 @@
       <c r="M75" s="12"/>
       <c r="N75" s="15"/>
       <c r="O75" s="13"/>
-      <c r="P75" s="61"/>
-      <c r="Q75" s="62"/>
-      <c r="R75" s="63"/>
+      <c r="P75" s="67"/>
+      <c r="Q75" s="68"/>
+      <c r="R75" s="69"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J76" s="9" t="s">
@@ -4493,11 +4517,11 @@
       <c r="O147" s="11">
         <v>-1</v>
       </c>
-      <c r="P147" s="58" t="s">
+      <c r="P147" s="61" t="s">
         <v>283</v>
       </c>
-      <c r="Q147" s="59"/>
-      <c r="R147" s="60"/>
+      <c r="Q147" s="62"/>
+      <c r="R147" s="63"/>
     </row>
     <row r="148" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
@@ -4509,9 +4533,9 @@
       <c r="M148" s="12"/>
       <c r="N148" s="15"/>
       <c r="O148" s="13"/>
-      <c r="P148" s="61"/>
-      <c r="Q148" s="62"/>
-      <c r="R148" s="63"/>
+      <c r="P148" s="67"/>
+      <c r="Q148" s="68"/>
+      <c r="R148" s="69"/>
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C149" s="2" t="s">
@@ -5439,11 +5463,11 @@
       <c r="O213" s="11">
         <v>-1</v>
       </c>
-      <c r="P213" s="58" t="s">
+      <c r="P213" s="61" t="s">
         <v>322</v>
       </c>
-      <c r="Q213" s="59"/>
-      <c r="R213" s="60"/>
+      <c r="Q213" s="62"/>
+      <c r="R213" s="63"/>
     </row>
     <row r="214" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
@@ -5455,9 +5479,9 @@
       <c r="L214" s="9"/>
       <c r="M214" s="16"/>
       <c r="O214" s="25"/>
-      <c r="P214" s="61"/>
-      <c r="Q214" s="62"/>
-      <c r="R214" s="63"/>
+      <c r="P214" s="67"/>
+      <c r="Q214" s="68"/>
+      <c r="R214" s="69"/>
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="16" t="s">
@@ -5558,11 +5582,11 @@
         <v>2853</v>
       </c>
       <c r="O221" s="11"/>
-      <c r="P221" s="58" t="s">
+      <c r="P221" s="61" t="s">
         <v>319</v>
       </c>
-      <c r="Q221" s="59"/>
-      <c r="R221" s="60"/>
+      <c r="Q221" s="62"/>
+      <c r="R221" s="63"/>
     </row>
     <row r="222" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="12" t="s">
@@ -5574,9 +5598,9 @@
       <c r="M222" s="12"/>
       <c r="N222" s="15"/>
       <c r="O222" s="13"/>
-      <c r="P222" s="61"/>
-      <c r="Q222" s="62"/>
-      <c r="R222" s="63"/>
+      <c r="P222" s="67"/>
+      <c r="Q222" s="68"/>
+      <c r="R222" s="69"/>
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
@@ -6470,11 +6494,11 @@
         <v>3984</v>
       </c>
       <c r="O284" s="11"/>
-      <c r="P284" s="58" t="s">
+      <c r="P284" s="61" t="s">
         <v>342</v>
       </c>
-      <c r="Q284" s="59"/>
-      <c r="R284" s="60"/>
+      <c r="Q284" s="62"/>
+      <c r="R284" s="63"/>
     </row>
     <row r="285" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="12" t="s">
@@ -6486,9 +6510,9 @@
       <c r="M285" s="12"/>
       <c r="N285" s="15"/>
       <c r="O285" s="13"/>
-      <c r="P285" s="61"/>
-      <c r="Q285" s="62"/>
-      <c r="R285" s="63"/>
+      <c r="P285" s="67"/>
+      <c r="Q285" s="68"/>
+      <c r="R285" s="69"/>
     </row>
     <row r="286" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
@@ -7185,11 +7209,11 @@
         <v>3584</v>
       </c>
       <c r="O334" s="11"/>
-      <c r="P334" s="58" t="s">
+      <c r="P334" s="61" t="s">
         <v>355</v>
       </c>
-      <c r="Q334" s="59"/>
-      <c r="R334" s="60"/>
+      <c r="Q334" s="62"/>
+      <c r="R334" s="63"/>
     </row>
     <row r="335" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A335" s="12" t="s">
@@ -7201,9 +7225,9 @@
       <c r="M335" s="12"/>
       <c r="N335" s="15"/>
       <c r="O335" s="13"/>
-      <c r="P335" s="61"/>
-      <c r="Q335" s="62"/>
-      <c r="R335" s="63"/>
+      <c r="P335" s="67"/>
+      <c r="Q335" s="68"/>
+      <c r="R335" s="69"/>
     </row>
     <row r="336" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F336" s="1" t="s">
@@ -8722,7 +8746,7 @@
       <c r="N445" s="1">
         <v>1744</v>
       </c>
-      <c r="O445" s="80"/>
+      <c r="O445" s="1"/>
       <c r="P445" s="52" t="s">
         <v>388</v>
       </c>
@@ -8954,7 +8978,6 @@
       </c>
       <c r="L462" s="9"/>
       <c r="M462" s="16"/>
-      <c r="N462" s="80"/>
       <c r="O462" s="25"/>
     </row>
     <row r="463" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9107,7 +9130,6 @@
         <v>98</v>
       </c>
       <c r="M473" s="16"/>
-      <c r="N473" s="80"/>
       <c r="O473" s="25"/>
     </row>
     <row r="474" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9269,7 +9291,7 @@
       <c r="E487" s="2">
         <v>1</v>
       </c>
-      <c r="K487" s="80"/>
+      <c r="K487" s="1"/>
       <c r="L487" s="40">
         <v>4</v>
       </c>
@@ -9422,7 +9444,7 @@
         <v>-3330</v>
       </c>
     </row>
-    <row r="497" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M497" s="1">
         <v>1372</v>
       </c>
@@ -9430,7 +9452,7 @@
         <v>-3744</v>
       </c>
     </row>
-    <row r="498" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A498" s="1" t="s">
         <v>328</v>
       </c>
@@ -9441,7 +9463,7 @@
         <v>-3593</v>
       </c>
     </row>
-    <row r="499" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D499" s="1" t="s">
         <v>416</v>
       </c>
@@ -9452,7 +9474,7 @@
         <v>4125</v>
       </c>
     </row>
-    <row r="500" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F500" s="1" t="s">
         <v>65</v>
       </c>
@@ -9466,19 +9488,321 @@
         <v>4194</v>
       </c>
     </row>
+    <row r="501" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A501" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B501" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M501" s="1">
+        <v>-4419</v>
+      </c>
+      <c r="N501" s="1">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="502" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C502" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="M502" s="1">
+        <v>-4192</v>
+      </c>
+      <c r="N502" s="1">
+        <v>894</v>
+      </c>
+      <c r="O502" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="503" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J503" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K503" s="2">
+        <v>3</v>
+      </c>
+      <c r="M503" s="1">
+        <v>-4164</v>
+      </c>
+      <c r="N503" s="1">
+        <v>864</v>
+      </c>
+      <c r="O503" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="504" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A504" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="M504" s="1">
+        <v>-4168</v>
+      </c>
+      <c r="N504" s="1">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="505" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D505" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="M505" s="1">
+        <v>-4040</v>
+      </c>
+      <c r="N505" s="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="506" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A506" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M506" s="1">
+        <v>-4016</v>
+      </c>
+      <c r="N506" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="507" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A507" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="M507" s="1">
+        <v>-1320</v>
+      </c>
+      <c r="N507" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="508" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D508" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="M508" s="1">
+        <v>-1487</v>
+      </c>
+      <c r="N508" s="1">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="509" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A509" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="M509" s="1">
+        <v>1995</v>
+      </c>
+      <c r="N509" s="1">
+        <v>-1198</v>
+      </c>
+    </row>
+    <row r="510" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A510" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="M510" s="1">
+        <v>2039</v>
+      </c>
+      <c r="N510" s="1">
+        <v>-1216</v>
+      </c>
+    </row>
+    <row r="511" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A511" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B511" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M511" s="1">
+        <v>2071</v>
+      </c>
+      <c r="N511" s="1">
+        <v>-322</v>
+      </c>
+      <c r="O511" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="512" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A512" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B512" s="2">
+        <v>1</v>
+      </c>
+      <c r="M512" s="1">
+        <v>2476</v>
+      </c>
+      <c r="N512" s="1">
+        <v>-719</v>
+      </c>
+    </row>
+    <row r="513" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A513" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B513" s="2">
+        <v>2</v>
+      </c>
+      <c r="M513" s="1">
+        <v>2476</v>
+      </c>
+      <c r="N513" s="1">
+        <v>-697</v>
+      </c>
+    </row>
+    <row r="514" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A514" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B514" s="2">
+        <v>3</v>
+      </c>
+      <c r="M514" s="1">
+        <v>2505</v>
+      </c>
+      <c r="N514" s="1">
+        <v>-651</v>
+      </c>
+    </row>
+    <row r="515" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F515" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G515" s="2">
+        <v>2</v>
+      </c>
+      <c r="M515" s="1">
+        <v>2495</v>
+      </c>
+      <c r="N515" s="1">
+        <v>-672</v>
+      </c>
+    </row>
+    <row r="516" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F516" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G516" s="2">
+        <v>1</v>
+      </c>
+      <c r="J516" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M516" s="1">
+        <v>2502</v>
+      </c>
+      <c r="N516" s="1">
+        <v>-656</v>
+      </c>
+    </row>
+    <row r="517" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F517" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G517" s="2">
+        <v>2</v>
+      </c>
+      <c r="M517" s="1">
+        <v>2463</v>
+      </c>
+      <c r="N517" s="1">
+        <v>-697</v>
+      </c>
+    </row>
+    <row r="518" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F518" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G518" s="2">
+        <v>1</v>
+      </c>
+      <c r="J518" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M518" s="1">
+        <v>2607</v>
+      </c>
+      <c r="N518" s="1">
+        <v>-591</v>
+      </c>
+    </row>
+    <row r="519" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A519" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B519" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M519" s="1">
+        <v>2429</v>
+      </c>
+      <c r="N519" s="1">
+        <v>-1473</v>
+      </c>
+    </row>
+    <row r="520" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J520" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M520" s="1">
+        <v>2432</v>
+      </c>
+      <c r="N520" s="1">
+        <v>-1462</v>
+      </c>
+    </row>
+    <row r="521" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D521" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="J521" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M521" s="1">
+        <v>2452</v>
+      </c>
+      <c r="N521" s="1">
+        <v>-1500</v>
+      </c>
+    </row>
+    <row r="522" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F522" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G522" s="2">
+        <v>2</v>
+      </c>
+      <c r="J522" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M522" s="1">
+        <v>2447</v>
+      </c>
+      <c r="N522" s="1">
+        <v>-1500</v>
+      </c>
+    </row>
+    <row r="523" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C523" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="M523" s="1">
+        <v>2916</v>
+      </c>
+      <c r="N523" s="1">
+        <v>-1495</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="P17:R22"/>
-    <mergeCell ref="P3:R15"/>
-    <mergeCell ref="P24:R25"/>
-    <mergeCell ref="P41:R42"/>
     <mergeCell ref="P284:R285"/>
     <mergeCell ref="P334:R335"/>
     <mergeCell ref="P147:R148"/>
@@ -9486,6 +9810,17 @@
     <mergeCell ref="P57:R58"/>
     <mergeCell ref="P74:R75"/>
     <mergeCell ref="P213:R214"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="P17:R22"/>
+    <mergeCell ref="P3:R15"/>
+    <mergeCell ref="P24:R25"/>
+    <mergeCell ref="P41:R42"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9496,9 +9831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
   <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Catch up on recycling
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5571F4A-40BA-4762-B360-E935D1FA57B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D241E1-0872-4E45-A125-0787F108E8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="450">
   <si>
     <t>Weapon</t>
   </si>
@@ -1350,6 +1350,45 @@
   </si>
   <si>
     <t>.50 BMG FMJ Ammo</t>
+  </si>
+  <si>
+    <t>Hermelinen Bunker - Warboard</t>
+  </si>
+  <si>
+    <t>Loud and Clear</t>
+  </si>
+  <si>
+    <t>Science of Deduction</t>
+  </si>
+  <si>
+    <t>Adhesive 2 | Rubber 5 | Aluminium 1</t>
+  </si>
+  <si>
+    <t>.50 BMG AP Ammo</t>
+  </si>
+  <si>
+    <t>Assault_Rifle_Barrel_Extenstion</t>
+  </si>
+  <si>
+    <t>Adhesive 2 | Plastic 5 | Titanium 1</t>
+  </si>
+  <si>
+    <t>Assault_Rifle_Silencer</t>
+  </si>
+  <si>
+    <t>Advesive 3 | Rubber 6 | Aluminium 1 | Tungsten 1</t>
+  </si>
+  <si>
+    <t>Submachine_Gun_Barrel_Extenstion</t>
+  </si>
+  <si>
+    <t>8_16x_Rifle_Scope</t>
+  </si>
+  <si>
+    <t>Adhesive 2 | Steel 5 | Titanium 1</t>
+  </si>
+  <si>
+    <t>Advesive 3 | Steel 6 | Titanium 1 | Tungsten 1</t>
   </si>
 </sst>
 </file>
@@ -1754,7 +1793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1957,6 +1996,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2274,11 +2316,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:T548"/>
+  <dimension ref="A1:T556"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K548" sqref="K548"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B557" sqref="B557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2289,7 +2331,7 @@
     <col min="4" max="4" width="3.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="28.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -10118,7 +10160,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="545" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B545" s="10">
         <v>586</v>
       </c>
@@ -10130,7 +10172,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="546" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B546" s="12"/>
       <c r="C546" s="15"/>
       <c r="D546" s="13"/>
@@ -10138,7 +10180,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="547" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B547" s="1">
         <v>585</v>
       </c>
@@ -10149,7 +10191,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="548" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B548" s="1">
         <v>597</v>
       </c>
@@ -10158,6 +10200,118 @@
       </c>
       <c r="J548" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="549" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B549" s="1">
+        <v>615</v>
+      </c>
+      <c r="C549" s="1">
+        <v>-3682</v>
+      </c>
+      <c r="H549" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="550" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B550" s="1">
+        <v>275</v>
+      </c>
+      <c r="C550" s="1">
+        <v>-3482</v>
+      </c>
+      <c r="J550" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="551" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B551" s="1">
+        <v>150</v>
+      </c>
+      <c r="C551" s="1">
+        <v>-3435</v>
+      </c>
+      <c r="J551" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="K551" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="552" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B552" s="1">
+        <v>173</v>
+      </c>
+      <c r="C552" s="1">
+        <v>-3458</v>
+      </c>
+      <c r="D552" s="2">
+        <v>-1</v>
+      </c>
+      <c r="J552" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="K552" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="553" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A553" s="9"/>
+      <c r="B553" s="10">
+        <v>130</v>
+      </c>
+      <c r="C553" s="14">
+        <v>-3351</v>
+      </c>
+      <c r="D553" s="11">
+        <v>-1</v>
+      </c>
+      <c r="I553" s="80"/>
+      <c r="J553" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="K553" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="554" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A554" s="9"/>
+      <c r="B554" s="16"/>
+      <c r="C554" s="80"/>
+      <c r="D554" s="25"/>
+      <c r="I554" s="80"/>
+      <c r="J554" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="K554" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="555" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A555" s="9"/>
+      <c r="B555" s="12"/>
+      <c r="C555" s="15"/>
+      <c r="D555" s="13"/>
+      <c r="I555" s="80"/>
+      <c r="J555" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="K555" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="556" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B556" s="1">
+        <v>218</v>
+      </c>
+      <c r="C556" s="1">
+        <v>-3378</v>
+      </c>
+      <c r="D556" s="2">
+        <v>-2</v>
+      </c>
+      <c r="M556" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -10189,11 +10343,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P129"/>
+  <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D123" sqref="D123"/>
+      <selection pane="topRight" activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10202,7 +10356,7 @@
     <col min="2" max="2" width="55.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
@@ -11599,97 +11753,103 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>247</v>
+        <v>252</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>245</v>
+        <v>304</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>246</v>
+        <v>272</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>249</v>
+        <v>355</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>270</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>255</v>
+        <v>447</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>315</v>
+        <v>243</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>315</v>
+        <v>244</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>262</v>
+        <v>249</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>270</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>247</v>
@@ -11697,144 +11857,153 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>263</v>
+        <v>253</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>247</v>
       </c>
+      <c r="E110" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>243</v>
+        <v>262</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>257</v>
+        <v>314</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>290</v>
+        <v>186</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>378</v>
+        <v>315</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>264</v>
+        <v>316</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>243</v>
+        <v>186</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>256</v>
+        <v>315</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>269</v>
+        <v>399</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>243</v>
+        <v>401</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>243</v>
+        <v>254</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>305</v>
+        <v>242</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>269</v>
+        <v>243</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>314</v>
+        <v>251</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>315</v>
+        <v>243</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>316</v>
+        <v>264</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>186</v>
+        <v>243</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>400</v>
+        <v>270</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>243</v>
@@ -11842,32 +12011,29 @@
       <c r="C123" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D123" s="1" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>270</v>
+        <v>444</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>364</v>
+        <v>290</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>290</v>
@@ -11878,26 +12044,73 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>379</v>
+        <v>257</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>290</v>
       </c>
+      <c r="C127" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>399</v>
+        <v>442</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>401</v>
+        <v>446</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>315</v>
+        <v>258</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weapon Schematic Loot Complete
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFE3440-6651-40BB-9F67-E8B5AD09147D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A213214B-7A6C-493E-A399-D6E031665E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="467">
   <si>
     <t>Weapon</t>
   </si>
@@ -1425,6 +1425,21 @@
   </si>
   <si>
     <t>Adhesive 6 | Plastic 11 |Aluminium 3 | Tungsten 1</t>
+  </si>
+  <si>
+    <t>Jultomten</t>
+  </si>
+  <si>
+    <t>Camouflage Shoes</t>
+  </si>
+  <si>
+    <t>Electrolyte</t>
+  </si>
+  <si>
+    <t>Electromagnetic Pulse Round</t>
+  </si>
+  <si>
+    <t>2_4x_Handgun_Scope</t>
   </si>
 </sst>
 </file>
@@ -2352,11 +2367,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:T583"/>
+  <dimension ref="A1:T595"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A566" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B584" sqref="B584"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A569" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B596" sqref="B596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2366,18 +2381,18 @@
     <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="28.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="37" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" style="2" customWidth="1"/>
     <col min="15" max="15" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="2"/>
+    <col min="16" max="16" width="3.7109375" style="2" customWidth="1"/>
     <col min="17" max="17" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="2"/>
+    <col min="18" max="18" width="3.7109375" style="2" customWidth="1"/>
     <col min="19" max="19" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
+    <col min="20" max="20" width="3.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -7364,7 +7379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B337" s="1">
         <v>-1342</v>
       </c>
@@ -7378,7 +7393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B338" s="1">
         <v>-1575</v>
       </c>
@@ -7392,7 +7407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B339" s="1">
         <v>-1559</v>
       </c>
@@ -7403,7 +7418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B340" s="1">
         <v>-1550</v>
       </c>
@@ -7413,20 +7428,20 @@
       <c r="D340" s="2">
         <v>2</v>
       </c>
-      <c r="H340" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="I340" s="2">
-        <v>2</v>
-      </c>
       <c r="O340" s="1" t="s">
         <v>61</v>
       </c>
       <c r="P340" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q340" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="R340" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B341" s="1">
         <v>-1603</v>
       </c>
@@ -7440,7 +7455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B342" s="1">
         <v>-1651</v>
       </c>
@@ -7454,7 +7469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B343" s="1">
         <v>-1726</v>
       </c>
@@ -7468,7 +7483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B344" s="1">
         <v>-1713</v>
       </c>
@@ -7482,7 +7497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B345" s="1">
         <v>-1730</v>
       </c>
@@ -7496,7 +7511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B346" s="1">
         <v>-1807</v>
       </c>
@@ -7519,7 +7534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B347" s="1">
         <v>-1978</v>
       </c>
@@ -7533,7 +7548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B348" s="1">
         <v>-2000</v>
       </c>
@@ -7547,7 +7562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B349" s="1">
         <v>-1771</v>
       </c>
@@ -7561,7 +7576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B350" s="1">
         <v>-1732</v>
       </c>
@@ -7575,7 +7590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A351" s="9"/>
       <c r="B351" s="9">
         <v>-1718</v>
@@ -7590,7 +7605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="352" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A352" s="9"/>
       <c r="B352" s="9">
         <v>-1705</v>
@@ -8389,16 +8404,16 @@
       <c r="D411" s="2">
         <v>2</v>
       </c>
-      <c r="H411" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="I411" s="2">
-        <v>1</v>
-      </c>
       <c r="O411" s="1" t="s">
         <v>61</v>
       </c>
       <c r="P411" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q411" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="R411" s="2">
         <v>1</v>
       </c>
     </row>
@@ -10709,6 +10724,188 @@
       <c r="D583" s="13"/>
       <c r="H583" s="9" t="s">
         <v>298</v>
+      </c>
+    </row>
+    <row r="584" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B584" s="1">
+        <v>-2383</v>
+      </c>
+      <c r="C584" s="1">
+        <v>-3433</v>
+      </c>
+      <c r="O584" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P584" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q584" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="R584" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="585" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A585" s="9"/>
+      <c r="B585" s="10">
+        <v>-2392</v>
+      </c>
+      <c r="C585" s="14">
+        <v>-3434</v>
+      </c>
+      <c r="D585" s="11"/>
+      <c r="H585" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="I585" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="586" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A586" s="9"/>
+      <c r="B586" s="16"/>
+      <c r="C586" s="80"/>
+      <c r="D586" s="25"/>
+      <c r="H586" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I586" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="587" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A587" s="9"/>
+      <c r="B587" s="12"/>
+      <c r="C587" s="15"/>
+      <c r="D587" s="13"/>
+      <c r="H587" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I587" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="588" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B588" s="1">
+        <v>-2910</v>
+      </c>
+      <c r="C588" s="1">
+        <v>-3710</v>
+      </c>
+      <c r="D588" s="2">
+        <v>3</v>
+      </c>
+      <c r="L588" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="M588" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="N588" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="589" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B589" s="1">
+        <v>-2175</v>
+      </c>
+      <c r="C589" s="1">
+        <v>-4410</v>
+      </c>
+      <c r="O589" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P589" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="590" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B590" s="1">
+        <v>-2178</v>
+      </c>
+      <c r="C590" s="1">
+        <v>-4405</v>
+      </c>
+      <c r="O590" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P590" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="591" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B591" s="1">
+        <v>-2157</v>
+      </c>
+      <c r="C591" s="1">
+        <v>-4442</v>
+      </c>
+      <c r="O591" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P591" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="592" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B592" s="1">
+        <v>-2136</v>
+      </c>
+      <c r="C592" s="1">
+        <v>-4424</v>
+      </c>
+      <c r="O592" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P592" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q592" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="R592" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="593" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B593" s="1">
+        <v>-2149</v>
+      </c>
+      <c r="C593" s="1">
+        <v>-4432</v>
+      </c>
+      <c r="O593" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P593" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="594" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B594" s="10">
+        <v>-2158</v>
+      </c>
+      <c r="C594" s="14">
+        <v>-4423</v>
+      </c>
+      <c r="D594" s="11"/>
+      <c r="H594" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M594" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="S594" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="595" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B595" s="12"/>
+      <c r="C595" s="15"/>
+      <c r="D595" s="13"/>
+      <c r="S595" s="1" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -10740,11 +10937,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P133"/>
+  <dimension ref="A1:P134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12176,29 +12373,26 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>440</v>
+        <v>466</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>272</v>
+        <v>304</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>270</v>
+      <c r="E102" s="1" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>355</v>
+        <v>272</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>243</v>
@@ -12206,90 +12400,84 @@
       <c r="C103" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>447</v>
+        <v>355</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>270</v>
       </c>
+      <c r="D104" s="1" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>255</v>
+        <v>447</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>448</v>
+        <v>247</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>186</v>
+        <v>249</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>449</v>
-      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>315</v>
@@ -12297,10 +12485,19 @@
       <c r="D111" s="1" t="s">
         <v>247</v>
       </c>
+      <c r="E111" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>247</v>
@@ -12308,7 +12505,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>247</v>
@@ -12316,18 +12513,15 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>315</v>
+        <v>263</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>186</v>
@@ -12335,54 +12529,48 @@
       <c r="C115" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>400</v>
-      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>247</v>
+        <v>316</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>315</v>
+        <v>399</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>245</v>
+        <v>401</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>440</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>270</v>
@@ -12390,32 +12578,35 @@
       <c r="D120" s="1" t="s">
         <v>256</v>
       </c>
+      <c r="E120" s="1" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>243</v>
       </c>
+      <c r="C121" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>358</v>
+        <v>264</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>243</v>
@@ -12423,32 +12614,35 @@
       <c r="C123" s="1" t="s">
         <v>270</v>
       </c>
+      <c r="D123" s="1" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>444</v>
+        <v>358</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F124" s="1" t="s">
-        <v>445</v>
+      <c r="C124" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>377</v>
+        <v>444</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>378</v>
+        <v>243</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>290</v>
@@ -12459,24 +12653,21 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>257</v>
+        <v>379</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="D127" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>443</v>
-      </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>442</v>
+        <v>257</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>258</v>
@@ -12484,10 +12675,13 @@
       <c r="D128" s="1" t="s">
         <v>378</v>
       </c>
+      <c r="E128" s="1" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>258</v>
@@ -12498,15 +12692,18 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>269</v>
+        <v>446</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>269</v>
@@ -12514,7 +12711,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>269</v>
@@ -12522,9 +12719,17 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B134" s="1" t="s">
         <v>364</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clothing location hunt started
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A213214B-7A6C-493E-A399-D6E031665E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F049F62-33D7-458E-871D-3304990000E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="482">
   <si>
     <t>Weapon</t>
   </si>
@@ -1440,6 +1440,51 @@
   </si>
   <si>
     <t>2_4x_Handgun_Scope</t>
+  </si>
+  <si>
+    <t>Dear Survivor and Fellow Friend</t>
+  </si>
+  <si>
+    <t>Camouflage Jacket</t>
+  </si>
+  <si>
+    <t>At Death's Door</t>
+  </si>
+  <si>
+    <t>Bullet-Resistant Shoes</t>
+  </si>
+  <si>
+    <t>Till Lillbrallan</t>
+  </si>
+  <si>
+    <t>Fireproofed Jacket</t>
+  </si>
+  <si>
+    <t>Adhesive</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Emblem Dala Horse</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>Wolf (Scout)</t>
+  </si>
+  <si>
+    <t>Emergency Supplies</t>
+  </si>
+  <si>
+    <t>Dual_Mode_IR_OPV_Module</t>
+  </si>
+  <si>
+    <t>Silver Gnome</t>
   </si>
 </sst>
 </file>
@@ -1986,10 +2031,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2001,6 +2046,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2008,15 +2062,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2049,7 +2094,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2367,11 +2412,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:T595"/>
+  <dimension ref="A1:T616"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A569" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B596" sqref="B596"/>
+      <pane ySplit="1" topLeftCell="A608" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B617" sqref="B617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2402,40 +2447,40 @@
       <c r="B1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="60"/>
       <c r="E1" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="60"/>
       <c r="H1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="59"/>
-      <c r="J1" s="60" t="s">
+      <c r="I1" s="60"/>
+      <c r="J1" s="59" t="s">
         <v>433</v>
       </c>
-      <c r="K1" s="59"/>
+      <c r="K1" s="60"/>
       <c r="L1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="M1" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="59"/>
+      <c r="N1" s="60"/>
       <c r="O1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="59"/>
+      <c r="P1" s="60"/>
       <c r="Q1" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="59"/>
+      <c r="R1" s="60"/>
       <c r="S1" s="58" t="s">
         <v>425</v>
       </c>
-      <c r="T1" s="59"/>
+      <c r="T1" s="60"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
@@ -2735,9 +2780,9 @@
       <c r="D18" s="14">
         <v>2</v>
       </c>
-      <c r="E18" s="64"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="66"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="69"/>
       <c r="H18" s="9" t="s">
         <v>13</v>
       </c>
@@ -2749,9 +2794,9 @@
       <c r="A19" s="9"/>
       <c r="B19" s="16"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="66"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="69"/>
       <c r="H19" s="29" t="s">
         <v>24</v>
       </c>
@@ -2760,17 +2805,17 @@
       <c r="A20" s="9"/>
       <c r="B20" s="16"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="69"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="16"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="66"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="69"/>
       <c r="O21" s="1" t="s">
         <v>21</v>
       </c>
@@ -2783,9 +2828,9 @@
       <c r="B22" s="12"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="69"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="66"/>
       <c r="Q22" s="1" t="s">
         <v>23</v>
       </c>
@@ -3358,9 +3403,9 @@
       <c r="B58" s="12"/>
       <c r="C58" s="15"/>
       <c r="D58" s="13"/>
-      <c r="E58" s="67"/>
-      <c r="F58" s="68"/>
-      <c r="G58" s="69"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="65"/>
+      <c r="G58" s="66"/>
       <c r="J58" s="12" t="s">
         <v>111</v>
       </c>
@@ -3618,9 +3663,9 @@
       <c r="B75" s="12"/>
       <c r="C75" s="15"/>
       <c r="D75" s="13"/>
-      <c r="E75" s="67"/>
-      <c r="F75" s="68"/>
-      <c r="G75" s="69"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="65"/>
+      <c r="G75" s="66"/>
       <c r="J75" s="12" t="s">
         <v>117</v>
       </c>
@@ -4663,9 +4708,9 @@
       <c r="B148" s="12"/>
       <c r="C148" s="15"/>
       <c r="D148" s="13"/>
-      <c r="E148" s="67"/>
-      <c r="F148" s="68"/>
-      <c r="G148" s="69"/>
+      <c r="E148" s="64"/>
+      <c r="F148" s="65"/>
+      <c r="G148" s="66"/>
       <c r="J148" s="12" t="s">
         <v>281</v>
       </c>
@@ -5609,9 +5654,9 @@
       <c r="A214" s="9"/>
       <c r="B214" s="16"/>
       <c r="D214" s="25"/>
-      <c r="E214" s="67"/>
-      <c r="F214" s="68"/>
-      <c r="G214" s="69"/>
+      <c r="E214" s="64"/>
+      <c r="F214" s="65"/>
+      <c r="G214" s="66"/>
       <c r="J214" s="1" t="s">
         <v>310</v>
       </c>
@@ -5728,9 +5773,9 @@
       <c r="B222" s="12"/>
       <c r="C222" s="15"/>
       <c r="D222" s="13"/>
-      <c r="E222" s="67"/>
-      <c r="F222" s="68"/>
-      <c r="G222" s="69"/>
+      <c r="E222" s="64"/>
+      <c r="F222" s="65"/>
+      <c r="G222" s="66"/>
       <c r="J222" s="12" t="s">
         <v>317</v>
       </c>
@@ -6640,9 +6685,9 @@
       <c r="B285" s="12"/>
       <c r="C285" s="15"/>
       <c r="D285" s="13"/>
-      <c r="E285" s="67"/>
-      <c r="F285" s="68"/>
-      <c r="G285" s="69"/>
+      <c r="E285" s="64"/>
+      <c r="F285" s="65"/>
+      <c r="G285" s="66"/>
       <c r="J285" s="12" t="s">
         <v>340</v>
       </c>
@@ -7355,9 +7400,9 @@
       <c r="B335" s="12"/>
       <c r="C335" s="15"/>
       <c r="D335" s="13"/>
-      <c r="E335" s="67"/>
-      <c r="F335" s="68"/>
-      <c r="G335" s="69"/>
+      <c r="E335" s="64"/>
+      <c r="F335" s="65"/>
+      <c r="G335" s="66"/>
       <c r="J335" s="12" t="s">
         <v>353</v>
       </c>
@@ -10318,7 +10363,7 @@
       <c r="D553" s="11">
         <v>-1</v>
       </c>
-      <c r="I553" s="80"/>
+      <c r="I553" s="1"/>
       <c r="J553" s="10" t="s">
         <v>437</v>
       </c>
@@ -10329,9 +10374,8 @@
     <row r="554" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A554" s="9"/>
       <c r="B554" s="16"/>
-      <c r="C554" s="80"/>
       <c r="D554" s="25"/>
-      <c r="I554" s="80"/>
+      <c r="I554" s="1"/>
       <c r="J554" s="16" t="s">
         <v>438</v>
       </c>
@@ -10344,7 +10388,7 @@
       <c r="B555" s="12"/>
       <c r="C555" s="15"/>
       <c r="D555" s="13"/>
-      <c r="I555" s="80"/>
+      <c r="I555" s="1"/>
       <c r="J555" s="12" t="s">
         <v>439</v>
       </c>
@@ -10705,8 +10749,6 @@
       <c r="A582" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="B582" s="80"/>
-      <c r="C582" s="80"/>
       <c r="D582" s="25"/>
       <c r="H582" s="9" t="s">
         <v>322</v>
@@ -10765,7 +10807,6 @@
     <row r="586" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A586" s="9"/>
       <c r="B586" s="16"/>
-      <c r="C586" s="80"/>
       <c r="D586" s="25"/>
       <c r="H586" s="9" t="s">
         <v>88</v>
@@ -10868,7 +10909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="593" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B593" s="1">
         <v>-2149</v>
       </c>
@@ -10882,7 +10923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="594" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B594" s="10">
         <v>-2158</v>
       </c>
@@ -10900,7 +10941,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="595" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B595" s="12"/>
       <c r="C595" s="15"/>
       <c r="D595" s="13"/>
@@ -10908,9 +10949,281 @@
         <v>426</v>
       </c>
     </row>
+    <row r="596" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B596" s="1">
+        <v>-4874</v>
+      </c>
+      <c r="C596" s="1">
+        <v>4796</v>
+      </c>
+      <c r="L596" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="597" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B597" s="1">
+        <v>-5082</v>
+      </c>
+      <c r="C597" s="1">
+        <v>4566</v>
+      </c>
+      <c r="M597" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="N597" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="598" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B598" s="10">
+        <v>-5664</v>
+      </c>
+      <c r="C598" s="14">
+        <v>4541</v>
+      </c>
+      <c r="D598" s="11">
+        <v>3</v>
+      </c>
+      <c r="H598" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J598" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="K598" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="599" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B599" s="12"/>
+      <c r="C599" s="15"/>
+      <c r="D599" s="13"/>
+      <c r="H599" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="600" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B600" s="1">
+        <v>-4736</v>
+      </c>
+      <c r="C600" s="1">
+        <v>336</v>
+      </c>
+      <c r="M600" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="N600" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="601" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B601" s="1">
+        <v>-5330</v>
+      </c>
+      <c r="C601" s="1">
+        <v>664</v>
+      </c>
+      <c r="L601" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="602" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B602" s="1">
+        <v>-5338</v>
+      </c>
+      <c r="C602" s="1">
+        <v>719</v>
+      </c>
+      <c r="M602" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="N602" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="603" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B603" s="1">
+        <v>-1759</v>
+      </c>
+      <c r="C603" s="1">
+        <v>-4128</v>
+      </c>
+      <c r="H603" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="604" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B604" s="1">
+        <v>-1861</v>
+      </c>
+      <c r="C604" s="1">
+        <v>-4290</v>
+      </c>
+      <c r="O604" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P604" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="605" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B605" s="1">
+        <v>-1808</v>
+      </c>
+      <c r="C605" s="1">
+        <v>-4323</v>
+      </c>
+      <c r="H605" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="S605" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="606" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A606" s="9"/>
+      <c r="B606" s="10">
+        <v>-1808</v>
+      </c>
+      <c r="C606" s="14">
+        <v>-4320</v>
+      </c>
+      <c r="D606" s="11"/>
+      <c r="H606" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S606" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="607" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A607" s="9"/>
+      <c r="B607" s="12"/>
+      <c r="C607" s="15"/>
+      <c r="D607" s="13"/>
+      <c r="S607" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="608" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B608" s="1">
+        <v>-1896</v>
+      </c>
+      <c r="C608" s="1">
+        <v>-4322</v>
+      </c>
+      <c r="H608" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="I608" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="609" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B609" s="1">
+        <v>-1862</v>
+      </c>
+      <c r="C609" s="1">
+        <v>-4321</v>
+      </c>
+      <c r="S609" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="610" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B610" s="1">
+        <v>-1856</v>
+      </c>
+      <c r="C610" s="1">
+        <v>-4332</v>
+      </c>
+      <c r="M610" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="611" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B611" s="1">
+        <v>-1862</v>
+      </c>
+      <c r="C611" s="1">
+        <v>-4288</v>
+      </c>
+      <c r="S611" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="612" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B612" s="1">
+        <v>-1859</v>
+      </c>
+      <c r="C612" s="1">
+        <v>-4289</v>
+      </c>
+      <c r="S612" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="613" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B613" s="1">
+        <v>-1564</v>
+      </c>
+      <c r="C613" s="1">
+        <v>-4146</v>
+      </c>
+      <c r="L613" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="614" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B614" s="1">
+        <v>-1205</v>
+      </c>
+      <c r="C614" s="1">
+        <v>-4168</v>
+      </c>
+      <c r="O614" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P614" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="615" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B615" s="1">
+        <v>-982</v>
+      </c>
+      <c r="C615" s="1">
+        <v>-4362</v>
+      </c>
+      <c r="J615" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="K615" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="616" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B616" s="1">
+        <v>-1017</v>
+      </c>
+      <c r="C616" s="1">
+        <v>-4344</v>
+      </c>
+      <c r="D616" s="2">
+        <v>3</v>
+      </c>
+      <c r="L616" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="E17:G22"/>
+    <mergeCell ref="E3:G15"/>
+    <mergeCell ref="E24:G25"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="E284:G285"/>
     <mergeCell ref="E334:G335"/>
     <mergeCell ref="E147:G148"/>
@@ -10918,17 +11231,12 @@
     <mergeCell ref="E57:G58"/>
     <mergeCell ref="E74:G75"/>
     <mergeCell ref="E213:G214"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E17:G22"/>
-    <mergeCell ref="E3:G15"/>
-    <mergeCell ref="E24:G25"/>
-    <mergeCell ref="E41:G42"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10937,11 +11245,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P134"/>
+  <dimension ref="A1:P135"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A101" sqref="A101"/>
+      <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11286,6 +11594,9 @@
       <c r="B13" s="1" t="s">
         <v>384</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>147</v>
       </c>
@@ -11713,6 +12024,9 @@
       </c>
       <c r="C48" s="1">
         <v>0.05</v>
+      </c>
+      <c r="D48" s="80" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -12603,6 +12917,12 @@
       <c r="B122" s="1" t="s">
         <v>243</v>
       </c>
+      <c r="C122" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
@@ -12730,6 +13050,14 @@
         <v>363</v>
       </c>
       <c r="B134" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>364</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fourth Char for 3c and up Weapons
</commit_message>
<xml_diff>
--- a/Map_Locations.xlsx
+++ b/Map_Locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tue-Ma Tocky\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC22FA6-B943-4179-B0BA-1C0E997F4FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C17EBAB-91B4-464F-B7C9-00E60C006015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{267F2BFC-1F61-4F4A-977C-12229A9E0BDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Names" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="509">
   <si>
     <t>Weapon</t>
   </si>
@@ -1540,6 +1539,33 @@
   </si>
   <si>
     <t>Adhesive 3 | Plastic 6 |Aluminium 2</t>
+  </si>
+  <si>
+    <t>Blast-Resistant Shirt</t>
+  </si>
+  <si>
+    <t>Of Machines and Men</t>
+  </si>
+  <si>
+    <t>Emergency Flare (Sticky)</t>
+  </si>
+  <si>
+    <t>Camouflage Shirt</t>
+  </si>
+  <si>
+    <t>Fireproofed Shirt</t>
+  </si>
+  <si>
+    <t>Adhesive 6 | Plastic 12 | Titanium 3</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>On the Road</t>
+  </si>
+  <si>
+    <t>Play me</t>
   </si>
 </sst>
 </file>
@@ -2172,72 +2198,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2268,14 +2228,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2592,11 +2618,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0CCAEA-98BE-4BB3-A3B1-6D45E2A7FDAA}">
-  <dimension ref="A1:T644"/>
+  <dimension ref="A1:T660"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A618" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B645" sqref="B645"/>
+      <pane ySplit="1" topLeftCell="A650" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B661" sqref="B661"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,43 +2650,43 @@
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="74" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="76"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="74" t="s">
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="75"/>
-      <c r="J1" s="76" t="s">
+      <c r="I1" s="70"/>
+      <c r="J1" s="69" t="s">
         <v>432</v>
       </c>
-      <c r="K1" s="75"/>
+      <c r="K1" s="70"/>
       <c r="L1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="M1" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="75"/>
-      <c r="O1" s="74" t="s">
+      <c r="N1" s="70"/>
+      <c r="O1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="74" t="s">
+      <c r="P1" s="70"/>
+      <c r="Q1" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="75"/>
-      <c r="S1" s="74" t="s">
+      <c r="R1" s="70"/>
+      <c r="S1" s="68" t="s">
         <v>424</v>
       </c>
-      <c r="T1" s="75"/>
+      <c r="T1" s="70"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
@@ -2722,11 +2748,11 @@
         <v>2197</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="67"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="82"/>
       <c r="J3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2742,9 +2768,9 @@
         <v>2199</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="70"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
       <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2758,9 +2784,9 @@
         <v>2209</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="70"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="85"/>
       <c r="O5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2773,9 +2799,9 @@
       <c r="B6" s="12"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
       <c r="H6" s="9" t="s">
         <v>10</v>
       </c>
@@ -2789,9 +2815,9 @@
         <v>2207</v>
       </c>
       <c r="D7" s="14"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
       <c r="H7" s="9" t="s">
         <v>37</v>
       </c>
@@ -2800,9 +2826,9 @@
       <c r="A8" s="9"/>
       <c r="B8" s="16"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="70"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="85"/>
       <c r="H8" s="9" t="s">
         <v>11</v>
       </c>
@@ -2811,9 +2837,9 @@
       <c r="A9" s="9"/>
       <c r="B9" s="16"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="85"/>
       <c r="H9" s="9" t="s">
         <v>13</v>
       </c>
@@ -2823,9 +2849,9 @@
       <c r="B10" s="12"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="70"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="85"/>
       <c r="O10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2843,9 +2869,9 @@
       <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="68"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="70"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85"/>
       <c r="H11" s="9" t="s">
         <v>13</v>
       </c>
@@ -2861,9 +2887,9 @@
       <c r="D12" s="14">
         <v>2</v>
       </c>
-      <c r="E12" s="68"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="70"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
       <c r="J12" s="1" t="s">
         <v>4</v>
       </c>
@@ -2876,9 +2902,9 @@
       <c r="B13" s="12"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="70"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
       <c r="H13" s="9" t="s">
         <v>16</v>
       </c>
@@ -2893,9 +2919,9 @@
       <c r="D14" s="1">
         <v>2</v>
       </c>
-      <c r="E14" s="68"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="70"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="85"/>
       <c r="H14" s="9" t="s">
         <v>11</v>
       </c>
@@ -2908,9 +2934,9 @@
         <v>2210</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="73"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="88"/>
       <c r="L15" s="2" t="s">
         <v>18</v>
       </c>
@@ -2937,11 +2963,11 @@
         <v>2243</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="73"/>
       <c r="H17" s="29" t="s">
         <v>10</v>
       </c>
@@ -2960,9 +2986,9 @@
       <c r="D18" s="14">
         <v>2</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="61"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
       <c r="H18" s="9" t="s">
         <v>13</v>
       </c>
@@ -2974,9 +3000,9 @@
       <c r="A19" s="9"/>
       <c r="B19" s="16"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="61"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
       <c r="H19" s="29" t="s">
         <v>24</v>
       </c>
@@ -2985,17 +3011,17 @@
       <c r="A20" s="9"/>
       <c r="B20" s="16"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="79"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="16"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="79"/>
       <c r="O21" s="1" t="s">
         <v>21</v>
       </c>
@@ -3008,9 +3034,9 @@
       <c r="B22" s="12"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="64"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="76"/>
       <c r="Q22" s="1" t="s">
         <v>23</v>
       </c>
@@ -3041,11 +3067,11 @@
         <v>2228</v>
       </c>
       <c r="D24" s="11"/>
-      <c r="E24" s="65" t="s">
+      <c r="E24" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="66"/>
-      <c r="G24" s="67"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="82"/>
       <c r="J24" s="10" t="s">
         <v>4</v>
       </c>
@@ -3058,9 +3084,9 @@
       <c r="B25" s="12"/>
       <c r="C25" s="15"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="73"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="88"/>
       <c r="J25" s="12" t="s">
         <v>28</v>
       </c>
@@ -3295,11 +3321,11 @@
       <c r="D41" s="11">
         <v>2</v>
       </c>
-      <c r="E41" s="65" t="s">
+      <c r="E41" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="66"/>
-      <c r="G41" s="67"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="82"/>
       <c r="J41" s="10" t="s">
         <v>28</v>
       </c>
@@ -3312,9 +3338,9 @@
       <c r="B42" s="12"/>
       <c r="C42" s="15"/>
       <c r="D42" s="13"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="72"/>
-      <c r="G42" s="73"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="88"/>
       <c r="J42" s="12" t="s">
         <v>41</v>
       </c>
@@ -3566,11 +3592,11 @@
       <c r="D57" s="11">
         <v>2</v>
       </c>
-      <c r="E57" s="56" t="s">
+      <c r="E57" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="F57" s="57"/>
-      <c r="G57" s="58"/>
+      <c r="F57" s="72"/>
+      <c r="G57" s="73"/>
       <c r="J57" s="10" t="s">
         <v>41</v>
       </c>
@@ -3583,9 +3609,9 @@
       <c r="B58" s="12"/>
       <c r="C58" s="15"/>
       <c r="D58" s="13"/>
-      <c r="E58" s="62"/>
-      <c r="F58" s="63"/>
-      <c r="G58" s="64"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="75"/>
+      <c r="G58" s="76"/>
       <c r="J58" s="12" t="s">
         <v>111</v>
       </c>
@@ -3827,11 +3853,11 @@
       <c r="D74" s="11">
         <v>-1</v>
       </c>
-      <c r="E74" s="56" t="s">
+      <c r="E74" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="F74" s="57"/>
-      <c r="G74" s="58"/>
+      <c r="F74" s="72"/>
+      <c r="G74" s="73"/>
       <c r="J74" s="10" t="s">
         <v>111</v>
       </c>
@@ -3843,9 +3869,9 @@
       <c r="B75" s="12"/>
       <c r="C75" s="15"/>
       <c r="D75" s="13"/>
-      <c r="E75" s="62"/>
-      <c r="F75" s="63"/>
-      <c r="G75" s="64"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="75"/>
+      <c r="G75" s="76"/>
       <c r="J75" s="12" t="s">
         <v>117</v>
       </c>
@@ -4074,16 +4100,16 @@
       </c>
     </row>
     <row r="91" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="78">
+      <c r="A91" s="56">
         <v>5</v>
       </c>
-      <c r="B91" s="79">
+      <c r="B91" s="57">
         <v>4223</v>
       </c>
-      <c r="C91" s="79">
+      <c r="C91" s="57">
         <v>1554</v>
       </c>
-      <c r="D91" s="80"/>
+      <c r="D91" s="58"/>
       <c r="I91" s="1"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
@@ -4286,28 +4312,28 @@
       </c>
     </row>
     <row r="107" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="81">
-        <v>2</v>
-      </c>
-      <c r="B107" s="82">
+      <c r="A107" s="59">
+        <v>2</v>
+      </c>
+      <c r="B107" s="60">
         <v>1937</v>
       </c>
-      <c r="C107" s="82">
+      <c r="C107" s="60">
         <v>3083</v>
       </c>
-      <c r="D107" s="83"/>
+      <c r="D107" s="61"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A108" s="81">
+      <c r="A108" s="59">
         <v>3</v>
       </c>
-      <c r="B108" s="82">
+      <c r="B108" s="60">
         <v>1946</v>
       </c>
-      <c r="C108" s="82">
+      <c r="C108" s="60">
         <v>3078</v>
       </c>
-      <c r="D108" s="83">
+      <c r="D108" s="61">
         <v>2</v>
       </c>
       <c r="E108" s="41" t="s">
@@ -4318,16 +4344,16 @@
       <c r="I108" s="1"/>
     </row>
     <row r="109" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="84" t="s">
+      <c r="A109" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="85">
+      <c r="B109" s="63">
         <v>1953</v>
       </c>
-      <c r="C109" s="85">
+      <c r="C109" s="63">
         <v>3081</v>
       </c>
-      <c r="D109" s="86">
+      <c r="D109" s="64">
         <v>2</v>
       </c>
       <c r="E109" s="44" t="s">
@@ -4543,16 +4569,16 @@
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A125" s="81">
+      <c r="A125" s="59">
         <v>5</v>
       </c>
-      <c r="B125" s="82">
+      <c r="B125" s="60">
         <v>1823</v>
       </c>
-      <c r="C125" s="82">
+      <c r="C125" s="60">
         <v>3088</v>
       </c>
-      <c r="D125" s="83"/>
+      <c r="D125" s="61"/>
       <c r="E125" s="40" t="s">
         <v>276</v>
       </c>
@@ -4560,16 +4586,16 @@
       <c r="G125" s="42"/>
     </row>
     <row r="126" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="84" t="s">
+      <c r="A126" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B126" s="85">
+      <c r="B126" s="63">
         <v>1817</v>
       </c>
-      <c r="C126" s="85">
+      <c r="C126" s="63">
         <v>3085</v>
       </c>
-      <c r="D126" s="86"/>
+      <c r="D126" s="64"/>
       <c r="E126" s="43"/>
       <c r="F126" s="44"/>
       <c r="G126" s="45"/>
@@ -4872,11 +4898,11 @@
       <c r="D147" s="11">
         <v>-1</v>
       </c>
-      <c r="E147" s="56" t="s">
+      <c r="E147" s="71" t="s">
         <v>281</v>
       </c>
-      <c r="F147" s="57"/>
-      <c r="G147" s="58"/>
+      <c r="F147" s="72"/>
+      <c r="G147" s="73"/>
       <c r="J147" s="10" t="s">
         <v>117</v>
       </c>
@@ -4888,9 +4914,9 @@
       <c r="B148" s="12"/>
       <c r="C148" s="15"/>
       <c r="D148" s="13"/>
-      <c r="E148" s="62"/>
-      <c r="F148" s="63"/>
-      <c r="G148" s="64"/>
+      <c r="E148" s="74"/>
+      <c r="F148" s="75"/>
+      <c r="G148" s="76"/>
       <c r="J148" s="12" t="s">
         <v>280</v>
       </c>
@@ -5460,16 +5486,16 @@
       </c>
     </row>
     <row r="189" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="78">
+      <c r="A189" s="56">
         <v>6</v>
       </c>
-      <c r="B189" s="79">
+      <c r="B189" s="57">
         <v>1537</v>
       </c>
-      <c r="C189" s="79">
+      <c r="C189" s="57">
         <v>3836</v>
       </c>
-      <c r="D189" s="80"/>
+      <c r="D189" s="58"/>
       <c r="I189" s="1"/>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
@@ -5512,16 +5538,16 @@
       </c>
     </row>
     <row r="193" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="78">
+      <c r="A193" s="56">
         <v>6</v>
       </c>
-      <c r="B193" s="79">
+      <c r="B193" s="57">
         <v>1382</v>
       </c>
-      <c r="C193" s="79">
+      <c r="C193" s="57">
         <v>3898</v>
       </c>
-      <c r="D193" s="80"/>
+      <c r="D193" s="58"/>
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
@@ -5626,16 +5652,16 @@
       </c>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A202" s="81" t="s">
+      <c r="A202" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="B202" s="82">
+      <c r="B202" s="60">
         <v>1564</v>
       </c>
-      <c r="C202" s="82">
+      <c r="C202" s="60">
         <v>4115</v>
       </c>
-      <c r="D202" s="83"/>
+      <c r="D202" s="61"/>
       <c r="H202" s="53" t="s">
         <v>297</v>
       </c>
@@ -5650,12 +5676,12 @@
       </c>
     </row>
     <row r="203" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="84" t="s">
+      <c r="A203" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B203" s="85"/>
-      <c r="C203" s="85"/>
-      <c r="D203" s="86"/>
+      <c r="B203" s="63"/>
+      <c r="C203" s="63"/>
+      <c r="D203" s="64"/>
       <c r="H203" s="9" t="s">
         <v>296</v>
       </c>
@@ -5666,7 +5692,7 @@
       <c r="B204" s="9">
         <v>1584</v>
       </c>
-      <c r="C204" s="88">
+      <c r="C204" s="1">
         <v>4274</v>
       </c>
       <c r="I204" s="1"/>
@@ -5819,11 +5845,11 @@
       <c r="D213" s="11">
         <v>-1</v>
       </c>
-      <c r="E213" s="56" t="s">
+      <c r="E213" s="71" t="s">
         <v>320</v>
       </c>
-      <c r="F213" s="57"/>
-      <c r="G213" s="58"/>
+      <c r="F213" s="72"/>
+      <c r="G213" s="73"/>
       <c r="J213" s="10" t="s">
         <v>280</v>
       </c>
@@ -5835,9 +5861,9 @@
       <c r="A214" s="9"/>
       <c r="B214" s="16"/>
       <c r="D214" s="25"/>
-      <c r="E214" s="62"/>
-      <c r="F214" s="63"/>
-      <c r="G214" s="64"/>
+      <c r="E214" s="74"/>
+      <c r="F214" s="75"/>
+      <c r="G214" s="76"/>
       <c r="J214" s="1" t="s">
         <v>309</v>
       </c>
@@ -5938,11 +5964,11 @@
         <v>2853</v>
       </c>
       <c r="D221" s="11"/>
-      <c r="E221" s="56" t="s">
+      <c r="E221" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="F221" s="57"/>
-      <c r="G221" s="58"/>
+      <c r="F221" s="72"/>
+      <c r="G221" s="73"/>
       <c r="J221" s="10" t="s">
         <v>310</v>
       </c>
@@ -5954,9 +5980,9 @@
       <c r="B222" s="12"/>
       <c r="C222" s="15"/>
       <c r="D222" s="13"/>
-      <c r="E222" s="62"/>
-      <c r="F222" s="63"/>
-      <c r="G222" s="64"/>
+      <c r="E222" s="74"/>
+      <c r="F222" s="75"/>
+      <c r="G222" s="76"/>
       <c r="J222" s="12" t="s">
         <v>316</v>
       </c>
@@ -6317,16 +6343,16 @@
       </c>
     </row>
     <row r="248" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="78" t="s">
+      <c r="A248" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B248" s="79">
+      <c r="B248" s="57">
         <v>1722</v>
       </c>
-      <c r="C248" s="79">
+      <c r="C248" s="57">
         <v>4532</v>
       </c>
-      <c r="D248" s="80">
+      <c r="D248" s="58">
         <v>0.5</v>
       </c>
       <c r="H248" s="9" t="s">
@@ -6337,16 +6363,16 @@
       </c>
     </row>
     <row r="249" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="78" t="s">
+      <c r="A249" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B249" s="79">
+      <c r="B249" s="57">
         <v>1721</v>
       </c>
-      <c r="C249" s="79">
+      <c r="C249" s="57">
         <v>4532</v>
       </c>
-      <c r="D249" s="80">
+      <c r="D249" s="58">
         <v>0.5</v>
       </c>
       <c r="I249" s="1"/>
@@ -6364,16 +6390,16 @@
       </c>
     </row>
     <row r="250" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250" s="78" t="s">
+      <c r="A250" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B250" s="79">
+      <c r="B250" s="57">
         <v>1721</v>
       </c>
-      <c r="C250" s="79">
+      <c r="C250" s="57">
         <v>4530</v>
       </c>
-      <c r="D250" s="80">
+      <c r="D250" s="58">
         <v>0.5</v>
       </c>
       <c r="H250" s="9" t="s">
@@ -6382,16 +6408,16 @@
       <c r="I250" s="1"/>
     </row>
     <row r="251" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A251" s="78" t="s">
+      <c r="A251" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B251" s="79">
+      <c r="B251" s="57">
         <v>1722</v>
       </c>
-      <c r="C251" s="79">
+      <c r="C251" s="57">
         <v>4542</v>
       </c>
-      <c r="D251" s="80">
+      <c r="D251" s="58">
         <v>0.5</v>
       </c>
       <c r="I251" s="1"/>
@@ -6403,16 +6429,16 @@
       </c>
     </row>
     <row r="252" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A252" s="81">
+      <c r="A252" s="59">
         <v>4</v>
       </c>
-      <c r="B252" s="82">
+      <c r="B252" s="60">
         <v>1823</v>
       </c>
-      <c r="C252" s="82">
+      <c r="C252" s="60">
         <v>4637</v>
       </c>
-      <c r="D252" s="83">
+      <c r="D252" s="61">
         <v>2</v>
       </c>
       <c r="H252" s="9" t="s">
@@ -6427,12 +6453,10 @@
       </c>
     </row>
     <row r="253" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A253" s="87" t="s">
+      <c r="A253" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="B253" s="88"/>
-      <c r="C253" s="88"/>
-      <c r="D253" s="89"/>
+      <c r="D253" s="66"/>
       <c r="H253" s="9" t="s">
         <v>275</v>
       </c>
@@ -6441,12 +6465,12 @@
       </c>
     </row>
     <row r="254" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A254" s="84" t="s">
+      <c r="A254" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B254" s="85"/>
-      <c r="C254" s="85"/>
-      <c r="D254" s="86"/>
+      <c r="B254" s="63"/>
+      <c r="C254" s="63"/>
+      <c r="D254" s="64"/>
       <c r="H254" s="9" t="s">
         <v>330</v>
       </c>
@@ -6654,29 +6678,29 @@
       </c>
     </row>
     <row r="270" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A270" s="81">
+      <c r="A270" s="59">
         <v>8</v>
       </c>
-      <c r="B270" s="82">
+      <c r="B270" s="60">
         <v>1180</v>
       </c>
-      <c r="C270" s="82">
+      <c r="C270" s="60">
         <v>3936</v>
       </c>
-      <c r="D270" s="83"/>
+      <c r="D270" s="61"/>
       <c r="I270" s="1"/>
     </row>
     <row r="271" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A271" s="81" t="s">
+      <c r="A271" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="B271" s="82">
+      <c r="B271" s="60">
         <v>1174</v>
       </c>
-      <c r="C271" s="82">
+      <c r="C271" s="60">
         <v>3936</v>
       </c>
-      <c r="D271" s="83"/>
+      <c r="D271" s="61"/>
       <c r="H271" s="9" t="s">
         <v>272</v>
       </c>
@@ -6689,24 +6713,20 @@
       </c>
     </row>
     <row r="272" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A272" s="87" t="s">
+      <c r="A272" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="B272" s="88"/>
-      <c r="C272" s="88"/>
-      <c r="D272" s="89"/>
+      <c r="D272" s="66"/>
       <c r="H272" s="9" t="s">
         <v>296</v>
       </c>
       <c r="I272" s="1"/>
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A273" s="87" t="s">
+      <c r="A273" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="B273" s="88"/>
-      <c r="C273" s="88"/>
-      <c r="D273" s="89"/>
+      <c r="D273" s="66"/>
       <c r="H273" s="9" t="s">
         <v>335</v>
       </c>
@@ -6715,12 +6735,12 @@
       </c>
     </row>
     <row r="274" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A274" s="84" t="s">
+      <c r="A274" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B274" s="85"/>
-      <c r="C274" s="85"/>
-      <c r="D274" s="86"/>
+      <c r="B274" s="63"/>
+      <c r="C274" s="63"/>
+      <c r="D274" s="64"/>
       <c r="H274" s="9" t="s">
         <v>336</v>
       </c>
@@ -6729,10 +6749,10 @@
       </c>
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B275" s="88">
+      <c r="B275" s="1">
         <v>887</v>
       </c>
-      <c r="C275" s="88">
+      <c r="C275" s="1">
         <v>3820</v>
       </c>
       <c r="I275" s="1"/>
@@ -6854,11 +6874,11 @@
         <v>3984</v>
       </c>
       <c r="D284" s="11"/>
-      <c r="E284" s="56" t="s">
+      <c r="E284" s="71" t="s">
         <v>340</v>
       </c>
-      <c r="F284" s="57"/>
-      <c r="G284" s="58"/>
+      <c r="F284" s="72"/>
+      <c r="G284" s="73"/>
       <c r="J284" s="10" t="s">
         <v>309</v>
       </c>
@@ -6870,9 +6890,9 @@
       <c r="B285" s="12"/>
       <c r="C285" s="15"/>
       <c r="D285" s="13"/>
-      <c r="E285" s="62"/>
-      <c r="F285" s="63"/>
-      <c r="G285" s="64"/>
+      <c r="E285" s="74"/>
+      <c r="F285" s="75"/>
+      <c r="G285" s="76"/>
       <c r="J285" s="12" t="s">
         <v>339</v>
       </c>
@@ -7569,11 +7589,11 @@
         <v>3584</v>
       </c>
       <c r="D334" s="11"/>
-      <c r="E334" s="56" t="s">
+      <c r="E334" s="71" t="s">
         <v>353</v>
       </c>
-      <c r="F334" s="57"/>
-      <c r="G334" s="58"/>
+      <c r="F334" s="72"/>
+      <c r="G334" s="73"/>
       <c r="J334" s="10" t="s">
         <v>350</v>
       </c>
@@ -7585,9 +7605,9 @@
       <c r="B335" s="12"/>
       <c r="C335" s="15"/>
       <c r="D335" s="13"/>
-      <c r="E335" s="62"/>
-      <c r="F335" s="63"/>
-      <c r="G335" s="64"/>
+      <c r="E335" s="74"/>
+      <c r="F335" s="75"/>
+      <c r="G335" s="76"/>
       <c r="J335" s="12" t="s">
         <v>352</v>
       </c>
@@ -8091,16 +8111,16 @@
       </c>
     </row>
     <row r="371" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A371" s="78">
+      <c r="A371" s="56">
         <v>4</v>
       </c>
-      <c r="B371" s="79">
+      <c r="B371" s="57">
         <v>-834</v>
       </c>
-      <c r="C371" s="79">
+      <c r="C371" s="57">
         <v>3295</v>
       </c>
-      <c r="D371" s="80"/>
+      <c r="D371" s="58"/>
       <c r="I371" s="1"/>
     </row>
     <row r="372" spans="1:18" x14ac:dyDescent="0.25">
@@ -8129,16 +8149,16 @@
       </c>
     </row>
     <row r="374" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A374" s="81">
+      <c r="A374" s="59">
         <v>6</v>
       </c>
-      <c r="B374" s="82">
+      <c r="B374" s="60">
         <v>-432</v>
       </c>
-      <c r="C374" s="82">
+      <c r="C374" s="60">
         <v>3124</v>
       </c>
-      <c r="D374" s="83"/>
+      <c r="D374" s="61"/>
       <c r="H374" s="9" t="s">
         <v>297</v>
       </c>
@@ -8151,10 +8171,8 @@
       </c>
     </row>
     <row r="375" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A375" s="87"/>
-      <c r="B375" s="88"/>
-      <c r="C375" s="88"/>
-      <c r="D375" s="89"/>
+      <c r="A375" s="65"/>
+      <c r="D375" s="66"/>
       <c r="H375" s="9" t="s">
         <v>360</v>
       </c>
@@ -8163,10 +8181,10 @@
       </c>
     </row>
     <row r="376" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A376" s="84"/>
-      <c r="B376" s="85"/>
-      <c r="C376" s="85"/>
-      <c r="D376" s="86"/>
+      <c r="A376" s="62"/>
+      <c r="B376" s="63"/>
+      <c r="C376" s="63"/>
+      <c r="D376" s="64"/>
       <c r="H376" s="9" t="s">
         <v>335</v>
       </c>
@@ -8490,28 +8508,28 @@
       </c>
     </row>
     <row r="401" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A401" s="81" t="s">
+      <c r="A401" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="B401" s="82">
+      <c r="B401" s="60">
         <v>525</v>
       </c>
-      <c r="C401" s="82">
+      <c r="C401" s="60">
         <v>2552</v>
       </c>
-      <c r="D401" s="83"/>
+      <c r="D401" s="61"/>
       <c r="H401" s="9" t="s">
         <v>360</v>
       </c>
       <c r="I401" s="1"/>
     </row>
     <row r="402" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A402" s="84" t="s">
+      <c r="A402" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B402" s="85"/>
-      <c r="C402" s="85"/>
-      <c r="D402" s="86"/>
+      <c r="B402" s="63"/>
+      <c r="C402" s="63"/>
+      <c r="D402" s="64"/>
       <c r="H402" s="9" t="s">
         <v>380</v>
       </c>
@@ -9653,16 +9671,16 @@
       </c>
     </row>
     <row r="487" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A487" s="78">
-        <v>4</v>
-      </c>
-      <c r="B487" s="79">
+      <c r="A487" s="56">
+        <v>5</v>
+      </c>
+      <c r="B487" s="57">
         <v>-365</v>
       </c>
-      <c r="C487" s="79">
+      <c r="C487" s="57">
         <v>924</v>
       </c>
-      <c r="D487" s="80"/>
+      <c r="D487" s="58"/>
       <c r="M487" s="1" t="s">
         <v>406</v>
       </c>
@@ -10397,7 +10415,7 @@
         <v>2</v>
       </c>
       <c r="H540" s="9" t="s">
-        <v>84</v>
+        <v>502</v>
       </c>
     </row>
     <row r="541" spans="1:14" x14ac:dyDescent="0.25">
@@ -10912,16 +10930,16 @@
       </c>
     </row>
     <row r="581" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A581" s="81">
+      <c r="A581" s="59">
         <v>7</v>
       </c>
-      <c r="B581" s="82">
+      <c r="B581" s="60">
         <v>2207</v>
       </c>
-      <c r="C581" s="82">
+      <c r="C581" s="60">
         <v>-3611</v>
       </c>
-      <c r="D581" s="83"/>
+      <c r="D581" s="61"/>
       <c r="H581" s="9" t="s">
         <v>335</v>
       </c>
@@ -10933,12 +10951,10 @@
       </c>
     </row>
     <row r="582" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A582" s="87" t="s">
+      <c r="A582" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="B582" s="88"/>
-      <c r="C582" s="88"/>
-      <c r="D582" s="89"/>
+      <c r="D582" s="66"/>
       <c r="H582" s="9" t="s">
         <v>321</v>
       </c>
@@ -10947,12 +10963,12 @@
       </c>
     </row>
     <row r="583" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A583" s="84" t="s">
+      <c r="A583" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="B583" s="85"/>
-      <c r="C583" s="85"/>
-      <c r="D583" s="86"/>
+      <c r="B583" s="63"/>
+      <c r="C583" s="63"/>
+      <c r="D583" s="64"/>
       <c r="H583" s="9" t="s">
         <v>297</v>
       </c>
@@ -11453,7 +11469,7 @@
       </c>
       <c r="D620" s="11"/>
       <c r="H620" s="9" t="s">
-        <v>84</v>
+        <v>502</v>
       </c>
       <c r="I620" s="2">
         <v>2</v>
@@ -11605,16 +11621,16 @@
       </c>
     </row>
     <row r="632" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A632" s="78">
+      <c r="A632" s="56">
         <v>6</v>
       </c>
-      <c r="B632" s="79">
+      <c r="B632" s="57">
         <v>-1520</v>
       </c>
-      <c r="C632" s="79">
+      <c r="C632" s="57">
         <v>-3388</v>
       </c>
-      <c r="D632" s="80"/>
+      <c r="D632" s="58"/>
     </row>
     <row r="633" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B633" s="1">
@@ -11661,7 +11677,7 @@
       <c r="D635" s="11">
         <v>-1</v>
       </c>
-      <c r="I635" s="88"/>
+      <c r="I635" s="1"/>
       <c r="J635" s="10" t="s">
         <v>489</v>
       </c>
@@ -11672,9 +11688,8 @@
     <row r="636" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A636" s="9"/>
       <c r="B636" s="16"/>
-      <c r="C636" s="88"/>
       <c r="D636" s="25"/>
-      <c r="I636" s="88"/>
+      <c r="I636" s="1"/>
       <c r="J636" s="16" t="s">
         <v>490</v>
       </c>
@@ -11685,9 +11700,8 @@
     <row r="637" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A637" s="9"/>
       <c r="B637" s="16"/>
-      <c r="C637" s="88"/>
       <c r="D637" s="25"/>
-      <c r="I637" s="88"/>
+      <c r="I637" s="1"/>
       <c r="J637" s="16" t="s">
         <v>491</v>
       </c>
@@ -11700,7 +11714,7 @@
       <c r="B638" s="12"/>
       <c r="C638" s="15"/>
       <c r="D638" s="13"/>
-      <c r="I638" s="88"/>
+      <c r="I638" s="1"/>
       <c r="J638" s="12" t="s">
         <v>492</v>
       </c>
@@ -11733,7 +11747,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="641" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B641" s="1">
         <v>-1376</v>
       </c>
@@ -11747,14 +11761,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="642" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B642" s="1">
         <v>-1363</v>
       </c>
       <c r="C642" s="1">
         <v>-4834</v>
       </c>
-      <c r="E642" s="90" t="s">
+      <c r="E642" s="67" t="s">
         <v>497</v>
       </c>
       <c r="J642" s="1" t="s">
@@ -11770,7 +11784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="643" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B643" s="1">
         <v>-1523</v>
       </c>
@@ -11784,7 +11798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="644" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B644" s="1">
         <v>-1559</v>
       </c>
@@ -11798,14 +11812,226 @@
         <v>3</v>
       </c>
     </row>
+    <row r="645" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B645" s="1">
+        <v>2671</v>
+      </c>
+      <c r="C645" s="1">
+        <v>-1260</v>
+      </c>
+      <c r="M645" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="N645" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="646" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B646" s="1">
+        <v>-872</v>
+      </c>
+      <c r="C646" s="1">
+        <v>647</v>
+      </c>
+      <c r="J646" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="647" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A647" s="9"/>
+      <c r="B647" s="10">
+        <v>-2957</v>
+      </c>
+      <c r="C647" s="14">
+        <v>1267</v>
+      </c>
+      <c r="D647" s="11"/>
+      <c r="H647" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="I647" s="2">
+        <v>2</v>
+      </c>
+      <c r="J647" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="K647" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M647" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="N647" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="648" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A648" s="9"/>
+      <c r="B648" s="16"/>
+      <c r="C648" s="90"/>
+      <c r="D648" s="25"/>
+      <c r="H648" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I648" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="649" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A649" s="9"/>
+      <c r="B649" s="16"/>
+      <c r="C649" s="90"/>
+      <c r="D649" s="25"/>
+      <c r="H649" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="650" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A650" s="9"/>
+      <c r="B650" s="16"/>
+      <c r="C650" s="90"/>
+      <c r="D650" s="25"/>
+      <c r="H650" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="651" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A651" s="9"/>
+      <c r="B651" s="12"/>
+      <c r="C651" s="15"/>
+      <c r="D651" s="13"/>
+      <c r="H651" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="652" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B652" s="1">
+        <v>-1540</v>
+      </c>
+      <c r="C652" s="1">
+        <v>-3165</v>
+      </c>
+      <c r="D652" s="2">
+        <v>-2</v>
+      </c>
+      <c r="M652" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="N652" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="653" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B653" s="1">
+        <v>-901</v>
+      </c>
+      <c r="C653" s="1">
+        <v>-1757</v>
+      </c>
+      <c r="O653" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P653" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="654" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B654" s="1">
+        <v>-1060</v>
+      </c>
+      <c r="C654" s="1">
+        <v>-1572</v>
+      </c>
+      <c r="J654" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="655" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B655" s="1">
+        <v>-1315</v>
+      </c>
+      <c r="C655" s="1">
+        <v>-1628</v>
+      </c>
+      <c r="M655" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="N655" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="656" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B656" s="1">
+        <v>-1295</v>
+      </c>
+      <c r="C656" s="1">
+        <v>-2231</v>
+      </c>
+      <c r="J656" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="657" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B657" s="1">
+        <v>-21</v>
+      </c>
+      <c r="C657" s="1">
+        <v>-777</v>
+      </c>
+      <c r="D657" s="2">
+        <v>2</v>
+      </c>
+      <c r="J657" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="K657" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="658" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B658" s="1">
+        <v>-41</v>
+      </c>
+      <c r="C658" s="1">
+        <v>-808</v>
+      </c>
+      <c r="L658" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="659" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B659" s="1">
+        <v>223</v>
+      </c>
+      <c r="C659" s="1">
+        <v>-532</v>
+      </c>
+      <c r="J659" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="660" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B660" s="1">
+        <v>-1131</v>
+      </c>
+      <c r="C660" s="1">
+        <v>-2423</v>
+      </c>
+      <c r="J660" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="K660" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E17:G22"/>
+    <mergeCell ref="E3:G15"/>
+    <mergeCell ref="E24:G25"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="E284:G285"/>
     <mergeCell ref="E334:G335"/>
     <mergeCell ref="E147:G148"/>
@@ -11813,12 +12039,12 @@
     <mergeCell ref="E57:G58"/>
     <mergeCell ref="E74:G75"/>
     <mergeCell ref="E213:G214"/>
-    <mergeCell ref="E17:G22"/>
-    <mergeCell ref="E3:G15"/>
-    <mergeCell ref="E24:G25"/>
-    <mergeCell ref="E41:G42"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11827,1863 +12053,2259 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1BA83C-AF5D-4BBC-8BCB-3BFD997FEBD8}">
-  <dimension ref="A1:P135"/>
+  <dimension ref="A1:AE135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H6" sqref="H6"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="52.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.7109375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.7109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="46" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="2.7109375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="E2" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="G2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="I2" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="K2" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="M2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="O2" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="Q2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="S2" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="U2" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="W2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="Y2" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="AA2" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="AC2" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="AE2" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="P3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="T3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="V3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="X3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="L4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="N4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="P4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="T4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="V4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="X4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AA4" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="R5" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="T5" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="X5" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AA5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="P6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="R6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AA6" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+    <row r="10" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="E10" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="G10" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="I10" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="K10" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="M10" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="O10" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="Q10" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="S10" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="K10" s="35" t="s">
+      <c r="U10" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="W10" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="Y10" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="N10" s="35" t="s">
+      <c r="AA10" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="O10" s="35" t="s">
+      <c r="AC10" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="P10" s="35" t="s">
+      <c r="AE10" s="35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>144</v>
+        <v>506</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>144</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="L11" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="N11" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="P11" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="T11" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="U11" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>142</v>
+        <v>506</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>142</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="L12" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="N12" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="P12" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="T12" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="U12" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="AB12" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="L13" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="U13" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="AA13" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="AC13" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="AD13" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AE13" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O14" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="AC15" s="1" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>109</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="W16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="36"/>
+      <c r="C21" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="D21" s="36"/>
+      <c r="E21" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="F21" s="36"/>
+      <c r="G21" s="36" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H21" s="36"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>10</v>
       </c>
-      <c r="C22" s="1">
+      <c r="E22" s="1">
         <v>0.05</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="1">
         <v>10</v>
       </c>
-      <c r="C23" s="1">
+      <c r="E23" s="1">
         <v>0.1</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C24" s="1">
         <v>10</v>
       </c>
-      <c r="C24" s="1">
+      <c r="E24" s="1">
         <v>0.2</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25" s="1">
         <v>20</v>
       </c>
-      <c r="C25" s="1">
+      <c r="E25" s="1">
         <v>0.2</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26" s="1">
         <v>10</v>
       </c>
-      <c r="C26" s="1">
+      <c r="E26" s="1">
         <v>0.05</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27" s="1">
         <v>5</v>
       </c>
-      <c r="C27" s="1">
+      <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C28" s="1">
         <v>5</v>
       </c>
-      <c r="C28" s="1">
+      <c r="E28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="1">
+      <c r="C29" s="1">
         <v>10</v>
       </c>
-      <c r="C29" s="1">
+      <c r="E29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="1">
+      <c r="C30" s="1">
         <v>5</v>
       </c>
-      <c r="C30" s="1">
+      <c r="E30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="1">
+      <c r="C31" s="1">
         <v>10</v>
       </c>
-      <c r="C31" s="1">
+      <c r="E31" s="1">
         <v>0.2</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="1">
+      <c r="C32" s="1">
         <v>5</v>
       </c>
-      <c r="C32" s="1">
+      <c r="E32" s="1">
         <v>1</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="1">
+      <c r="C33" s="1">
         <v>5</v>
       </c>
-      <c r="C33" s="1">
+      <c r="E33" s="1">
         <v>0.2</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="1">
+      <c r="C34" s="1">
         <v>5</v>
       </c>
-      <c r="C34" s="1">
+      <c r="E34" s="1">
         <v>1</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="1">
+      <c r="C36" s="1">
         <v>5</v>
       </c>
-      <c r="C36" s="1">
+      <c r="E36" s="1">
         <v>0.2</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="1">
+      <c r="C37" s="1">
         <v>10</v>
       </c>
-      <c r="C37" s="1">
+      <c r="E37" s="1">
         <v>1</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="1">
+      <c r="C38" s="1">
         <v>10</v>
       </c>
-      <c r="C38" s="1">
+      <c r="E38" s="1">
         <v>1</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B39" s="1">
+      <c r="C39" s="1">
         <v>10</v>
       </c>
-      <c r="C39" s="1">
+      <c r="E39" s="1">
         <v>1</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B40" s="1">
+      <c r="C40" s="1">
         <v>5</v>
       </c>
-      <c r="C40" s="1">
+      <c r="E40" s="1">
         <v>0.5</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="1">
+      <c r="C41" s="1">
         <v>10</v>
       </c>
-      <c r="C41" s="1">
+      <c r="E41" s="1">
         <v>1</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="1">
+      <c r="C43" s="1">
         <v>10</v>
       </c>
-      <c r="C43" s="1">
+      <c r="E43" s="1">
         <v>0.5</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="1">
+      <c r="C44" s="1">
         <v>10</v>
       </c>
-      <c r="C44" s="1">
+      <c r="E44" s="1">
         <v>1</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="1">
+      <c r="C45" s="1">
         <v>5</v>
       </c>
-      <c r="C45" s="1">
+      <c r="E45" s="1">
         <v>0.2</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="1">
+      <c r="C46" s="1">
         <v>5</v>
       </c>
-      <c r="C46" s="1">
+      <c r="E46" s="1">
         <v>1</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="1">
+      <c r="C47" s="1">
         <v>5</v>
       </c>
-      <c r="C47" s="1">
+      <c r="E47" s="1">
         <v>1</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="1">
+      <c r="C48" s="1">
         <v>0</v>
       </c>
-      <c r="C48" s="1">
+      <c r="E48" s="1">
         <v>0.05</v>
       </c>
-      <c r="D48" s="54" t="s">
+      <c r="G48" s="54" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H48" s="54"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="1">
+      <c r="C49" s="1">
         <v>10</v>
       </c>
-      <c r="C49" s="1">
+      <c r="E49" s="1">
         <v>0.2</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="1">
+      <c r="C50" s="1">
         <v>10</v>
       </c>
-      <c r="C50" s="1">
+      <c r="E50" s="1">
         <v>1</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="1">
+      <c r="C51" s="1">
         <v>5</v>
       </c>
-      <c r="C51" s="1">
+      <c r="E51" s="1">
         <v>0.2</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="1">
+      <c r="C53" s="1">
         <v>5</v>
       </c>
-      <c r="C53" s="1">
+      <c r="E53" s="1">
         <v>0.2</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="1">
+      <c r="C54" s="1">
         <v>5</v>
       </c>
-      <c r="C54" s="1">
+      <c r="E54" s="1">
         <v>0.2</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="1">
+      <c r="C55" s="1">
         <v>5</v>
       </c>
-      <c r="C55" s="1">
+      <c r="E55" s="1">
         <v>1</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="1">
+      <c r="C56" s="1">
         <v>5</v>
       </c>
-      <c r="C56" s="1">
+      <c r="E56" s="1">
         <v>1</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="1">
+      <c r="C58" s="1">
         <v>5</v>
       </c>
-      <c r="C58" s="1">
+      <c r="E58" s="1">
         <v>1</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B59" s="1">
+      <c r="C59" s="1">
         <v>5</v>
       </c>
-      <c r="C59" s="1">
+      <c r="E59" s="1">
         <v>0.05</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="B62" s="36" t="s">
+      <c r="B62" s="36"/>
+      <c r="C62" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="C62" s="36" t="s">
+      <c r="D62" s="36"/>
+      <c r="E62" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="D62" s="36" t="s">
+      <c r="F62" s="36"/>
+      <c r="G62" s="36" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H62" s="36"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="1">
+      <c r="C63" s="1">
         <v>100</v>
       </c>
-      <c r="C63" s="1">
+      <c r="E63" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="G63" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B64" s="1">
+      <c r="C64" s="1">
         <v>100</v>
       </c>
-      <c r="C64" s="1">
+      <c r="E64" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="G64" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B65" s="1">
+      <c r="C65" s="1">
         <v>100</v>
       </c>
-      <c r="C65" s="1">
+      <c r="E65" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="G65" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B66" s="1">
+      <c r="C66" s="1">
         <v>100</v>
       </c>
-      <c r="C66" s="1">
+      <c r="E66" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="G66" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B67" s="1">
+      <c r="C67" s="1">
         <v>100</v>
       </c>
-      <c r="C67" s="1">
+      <c r="E67" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="G67" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B68" s="1">
+      <c r="C68" s="1">
         <v>100</v>
       </c>
-      <c r="C68" s="1">
+      <c r="E68" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B69" s="1">
+      <c r="C69" s="1">
         <v>25</v>
       </c>
-      <c r="C69" s="1">
+      <c r="E69" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B70" s="1">
+      <c r="C70" s="1">
         <v>25</v>
       </c>
-      <c r="C70" s="1">
+      <c r="E70" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B71" s="1">
+      <c r="C71" s="1">
         <v>25</v>
       </c>
-      <c r="C71" s="1">
+      <c r="E71" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B72" s="1">
+      <c r="C72" s="1">
         <v>25</v>
       </c>
-      <c r="C72" s="1">
+      <c r="E72" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="G72" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B73" s="1">
+      <c r="C73" s="1">
         <v>25</v>
       </c>
-      <c r="C73" s="1">
+      <c r="E73" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="G73" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B74" s="1">
+      <c r="C74" s="1">
         <v>25</v>
       </c>
-      <c r="C74" s="1">
+      <c r="E74" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="G74" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B75" s="1">
+      <c r="C75" s="1">
         <v>25</v>
       </c>
-      <c r="C75" s="1">
+      <c r="E75" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="G75" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B76" s="1">
+      <c r="C76" s="1">
         <v>75</v>
       </c>
-      <c r="C76" s="1">
+      <c r="E76" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B77" s="1">
+      <c r="C77" s="1">
         <v>75</v>
       </c>
-      <c r="C77" s="1">
+      <c r="E77" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="G77" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B78" s="1">
+      <c r="C78" s="1">
         <v>125</v>
       </c>
-      <c r="C78" s="1">
+      <c r="E78" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="G78" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B79" s="1">
+      <c r="C79" s="1">
         <v>125</v>
       </c>
-      <c r="C79" s="1">
+      <c r="E79" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="G79" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B80" s="1">
+      <c r="C80" s="1">
         <v>75</v>
       </c>
-      <c r="C80" s="1">
+      <c r="E80" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="G80" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B81" s="1">
+      <c r="C81" s="1">
         <v>75</v>
       </c>
-      <c r="C81" s="1">
+      <c r="E81" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="G81" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B82" s="1">
+      <c r="C82" s="1">
         <v>20</v>
       </c>
-      <c r="C82" s="1">
+      <c r="E82" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="G82" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B83" s="1">
+      <c r="C83" s="1">
         <v>10</v>
       </c>
-      <c r="C83" s="1">
+      <c r="E83" s="1">
         <v>0.1</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="G83" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B84" s="1">
+      <c r="C84" s="1">
         <v>4</v>
       </c>
-      <c r="C84" s="1">
+      <c r="E84" s="1">
         <v>0.22</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="G84" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="1">
+      <c r="C85" s="1">
         <v>500</v>
       </c>
-      <c r="C85" s="1">
+      <c r="E85" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="G85" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B86" s="1">
+      <c r="C86" s="1">
         <v>4</v>
       </c>
-      <c r="C86" s="1">
+      <c r="E86" s="1">
         <v>0.25</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="G86" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B87" s="1">
+      <c r="C87" s="1">
         <v>50</v>
       </c>
-      <c r="C87" s="1">
+      <c r="E87" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="G87" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B88" s="1">
+      <c r="C88" s="1">
         <v>50</v>
       </c>
-      <c r="C88" s="1">
+      <c r="E88" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="G88" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B89" s="1">
+      <c r="C89" s="1">
         <v>4</v>
       </c>
-      <c r="C89" s="1">
+      <c r="E89" s="1">
         <v>0.25</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="G89" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B90" s="1">
+      <c r="C90" s="1">
         <v>4</v>
       </c>
-      <c r="C90" s="1">
+      <c r="E90" s="1">
         <v>0.25</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="G90" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B91" s="1">
+      <c r="C91" s="1">
         <v>4</v>
       </c>
-      <c r="C91" s="1">
+      <c r="E91" s="1">
         <v>0.25</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="G91" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B92" s="1">
+      <c r="C92" s="1">
         <v>4</v>
       </c>
-      <c r="C92" s="1">
+      <c r="E92" s="1">
         <v>0.25</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="G92" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B93" s="1">
+      <c r="C93" s="1">
         <v>4</v>
       </c>
-      <c r="C93" s="1">
+      <c r="E93" s="1">
         <v>0.25</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="G93" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B94" s="1">
+      <c r="C94" s="1">
         <v>4</v>
       </c>
-      <c r="C94" s="1">
+      <c r="E94" s="1">
         <v>0.25</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="G94" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="77" t="s">
+    <row r="97" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="89" t="s">
         <v>236</v>
       </c>
-      <c r="B97" s="77" t="s">
+      <c r="B97" s="36"/>
+      <c r="C97" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="C97" s="77"/>
-      <c r="D97" s="77"/>
-      <c r="E97" s="77"/>
-      <c r="F97" s="77"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="77"/>
-      <c r="B98" s="77"/>
-      <c r="C98" s="77"/>
-      <c r="D98" s="77"/>
-      <c r="E98" s="77"/>
-      <c r="F98" s="77"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="77"/>
-      <c r="B99" s="1" t="s">
+      <c r="D97" s="89"/>
+      <c r="E97" s="89"/>
+      <c r="F97" s="89"/>
+      <c r="G97" s="89"/>
+      <c r="H97" s="89"/>
+      <c r="I97" s="89"/>
+      <c r="J97" s="89"/>
+      <c r="K97" s="89"/>
+      <c r="L97" s="36"/>
+    </row>
+    <row r="98" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="89"/>
+      <c r="B98" s="36"/>
+      <c r="C98" s="89"/>
+      <c r="D98" s="89"/>
+      <c r="E98" s="89"/>
+      <c r="F98" s="89"/>
+      <c r="G98" s="89"/>
+      <c r="H98" s="89"/>
+      <c r="I98" s="89"/>
+      <c r="J98" s="89"/>
+      <c r="K98" s="89"/>
+      <c r="L98" s="36"/>
+    </row>
+    <row r="99" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="89"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="E99" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="G99" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="I99" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F99" s="1" t="s">
+      <c r="K99" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="90" t="s">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="67" t="s">
         <v>251</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="D100" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E100" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="G100" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="90" t="s">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="67" t="s">
         <v>465</v>
       </c>
-      <c r="F101" s="1" t="s">
+      <c r="B101" s="67"/>
+      <c r="K101" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="90" t="s">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="67" t="s">
         <v>303</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="I102" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="90" t="s">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="67" t="s">
         <v>271</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E103" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="90" t="s">
+      <c r="F103" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="67" t="s">
         <v>354</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="G104" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="90" t="s">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="67" t="s">
         <v>446</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="B105" s="67"/>
+      <c r="D105" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E105" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="G105" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="90" t="s">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="67" t="s">
         <v>249</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="G106" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="90" t="s">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="67" t="s">
         <v>247</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="B107" s="67"/>
+      <c r="F107" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G107" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="90" t="s">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A108" s="67" t="s">
         <v>258</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="B108" s="67"/>
+      <c r="G108" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="90" t="s">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A109" s="67" t="s">
         <v>494</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="B109" s="67"/>
+      <c r="F109" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G109" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="I109" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="90" t="s">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A110" s="67" t="s">
         <v>248</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="B110" s="67"/>
+      <c r="D110" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="G110" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="90" t="s">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" s="67" t="s">
         <v>252</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E111" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="F111" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="H111" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I111" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="F111" s="1" t="s">
+      <c r="K111" s="1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="90" t="s">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A112" s="67" t="s">
         <v>260</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="B112" s="67"/>
+      <c r="D112" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E112" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="G112" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="90" t="s">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" s="67" t="s">
         <v>261</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="B113" s="67"/>
+      <c r="F113" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="90" t="s">
+      <c r="I113" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" s="67" t="s">
         <v>262</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="B114" s="67"/>
+      <c r="G114" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="90" t="s">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="67" t="s">
         <v>313</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="E115" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="90" t="s">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" s="67" t="s">
         <v>315</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="F116" s="1" t="s">
+      <c r="K116" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="90" t="s">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="67" t="s">
         <v>398</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="B117" s="67"/>
+      <c r="G117" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="90" t="s">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="67" t="s">
         <v>400</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="B118" s="67"/>
+      <c r="E118" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="90" t="s">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="67" t="s">
         <v>259</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="B119" s="67"/>
+      <c r="G119" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="90" t="s">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="B120" s="67"/>
+      <c r="D120" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="F120" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G120" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E120" s="1" t="s">
+      <c r="I120" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="90" t="s">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="67" t="s">
         <v>242</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="F121" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G121" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="90" t="s">
+      <c r="I121" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="67" t="s">
         <v>250</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="E122" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="I122" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="90" t="s">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="67" t="s">
         <v>263</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="D123" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E123" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="F123" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G123" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="H123" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I123" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="90" t="s">
+      <c r="K123" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" s="67" t="s">
         <v>357</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="E124" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="90" t="s">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="67" t="s">
         <v>443</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F125" s="1" t="s">
+      <c r="D125" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K125" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="90" t="s">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="67" t="s">
         <v>376</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="F126" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G126" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="E126" s="1" t="s">
+      <c r="I126" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="90" t="s">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="D127" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D127" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="90" t="s">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" s="67" t="s">
         <v>256</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="F128" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G128" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="E128" s="1" t="s">
+      <c r="H128" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I128" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="K128" s="1" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="90" t="s">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="67" t="s">
         <v>441</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="B129" s="67"/>
+      <c r="D129" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E129" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="F129" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G129" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="E129" s="1" t="s">
+      <c r="H129" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="I129" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="90" t="s">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="67" t="s">
         <v>445</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="B130" s="67"/>
+      <c r="D130" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E130" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="F130" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G130" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="90" t="s">
+      <c r="I130" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="67" t="s">
         <v>267</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="90" t="s">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="67" t="s">
         <v>290</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="90" t="s">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="67" t="s">
         <v>304</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="90" t="s">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="67" t="s">
         <v>362</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="90" t="s">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="67" t="s">
         <v>479</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="67" t="s">
+        <v>506</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>363</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B97:F98"/>
+    <mergeCell ref="C97:K98"/>
     <mergeCell ref="A97:A99"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -15049,8 +15671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49260601-DFFC-49C5-BC21-5E0477EEDF42}">
   <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15270,7 +15892,7 @@
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>502</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>